<commit_message>
galacticPubs::publish() [2022-04-01 12:03:32]  fixed feedback and background sections
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -369,7 +369,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="112">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -1020,7 +1020,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="166">
+  <cellXfs count="331">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1285,6 +1285,501 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="1"/>
@@ -6170,62 +6665,62 @@
       <c r="Z2" s="4"/>
     </row>
     <row r="3" spans="1:26" ht="56" x14ac:dyDescent="0.15">
-      <c r="A3" s="111" t="s">
+      <c r="A3" s="276" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="114" t="s">
+      <c r="B3" s="279" t="s">
         <v>79</v>
       </c>
-      <c r="C3" s="117" t="s">
+      <c r="C3" s="282" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="120" t="s">
+      <c r="D3" s="285" t="s">
         <v>82</v>
       </c>
-      <c r="E3" s="123" t="s">
+      <c r="E3" s="288" t="s">
         <v>85</v>
       </c>
-      <c r="F3" s="126" t="s">
+      <c r="F3" s="291" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="56" x14ac:dyDescent="0.15">
-      <c r="A4" s="112" t="s">
+      <c r="A4" s="277" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="115" t="s">
+      <c r="B4" s="280" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="118" t="s">
+      <c r="C4" s="283" t="s">
         <v>81</v>
       </c>
-      <c r="D4" s="121" t="s">
+      <c r="D4" s="286" t="s">
         <v>83</v>
       </c>
-      <c r="E4" s="124" t="s">
+      <c r="E4" s="289" t="s">
         <v>86</v>
       </c>
-      <c r="F4" s="127" t="s">
+      <c r="F4" s="292" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="56" x14ac:dyDescent="0.15">
-      <c r="A5" s="113" t="s">
+      <c r="A5" s="278" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="116" t="s">
+      <c r="B5" s="281" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="119" t="s">
+      <c r="C5" s="284" t="s">
         <v>81</v>
       </c>
-      <c r="D5" s="122" t="s">
+      <c r="D5" s="287" t="s">
         <v>84</v>
       </c>
-      <c r="E5" s="125" t="s">
+      <c r="E5" s="290" t="s">
         <v>87</v>
       </c>
-      <c r="F5" s="128" t="s">
+      <c r="F5" s="293" t="s">
         <v>88</v>
       </c>
     </row>
@@ -7368,25 +7863,25 @@
     <row r="3" spans="1:30" ht="140" x14ac:dyDescent="0.15">
       <c r="A3" s="12"/>
       <c r="B3"/>
-      <c r="C3" s="129" t="s">
+      <c r="C3" s="294" t="s">
         <v>79</v>
       </c>
-      <c r="D3" s="130" t="s">
+      <c r="D3" s="295" t="s">
         <v>89</v>
       </c>
-      <c r="E3" s="131" t="s">
+      <c r="E3" s="296" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="132" t="s">
+      <c r="F3" s="297" t="s">
         <v>91</v>
       </c>
-      <c r="G3" s="133" t="s">
+      <c r="G3" s="298" t="s">
         <v>88</v>
       </c>
-      <c r="H3" s="134" t="s">
+      <c r="H3" s="299" t="s">
         <v>92</v>
       </c>
-      <c r="I3" s="135" t="s">
+      <c r="I3" s="300" t="s">
         <v>93</v>
       </c>
       <c r="J3"/>
@@ -8957,29 +9452,29 @@
     <row r="3" spans="1:31" ht="114" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
       <c r="B3"/>
-      <c r="C3" s="136" t="s">
+      <c r="C3" s="301" t="s">
         <v>79</v>
       </c>
-      <c r="D3" s="140" t="s">
+      <c r="D3" s="305" t="s">
         <v>89</v>
       </c>
-      <c r="E3" s="144" t="s">
+      <c r="E3" s="309" t="s">
         <v>100</v>
       </c>
       <c r="F3" s="13"/>
-      <c r="G3" s="146" t="s">
+      <c r="G3" s="311" t="s">
         <v>102</v>
       </c>
-      <c r="H3" s="150" t="s">
+      <c r="H3" s="315" t="s">
         <v>104</v>
       </c>
-      <c r="I3" s="154" t="s">
+      <c r="I3" s="319" t="s">
         <v>106</v>
       </c>
-      <c r="J3" s="158" t="s">
+      <c r="J3" s="323" t="s">
         <v>107</v>
       </c>
-      <c r="K3" s="162" t="s">
+      <c r="K3" s="327" t="s">
         <v>109</v>
       </c>
       <c r="U3" s="6"/>
@@ -8993,29 +9488,29 @@
     <row r="4" spans="1:31" ht="114" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
       <c r="B4"/>
-      <c r="C4" s="137" t="s">
+      <c r="C4" s="302" t="s">
         <v>79</v>
       </c>
-      <c r="D4" s="141" t="s">
+      <c r="D4" s="306" t="s">
         <v>89</v>
       </c>
-      <c r="E4" s="145" t="s">
+      <c r="E4" s="310" t="s">
         <v>101</v>
       </c>
       <c r="F4" s="13"/>
-      <c r="G4" s="147" t="s">
+      <c r="G4" s="312" t="s">
         <v>103</v>
       </c>
-      <c r="H4" s="151" t="s">
+      <c r="H4" s="316" t="s">
         <v>105</v>
       </c>
-      <c r="I4" s="155" t="s">
+      <c r="I4" s="320" t="s">
         <v>106</v>
       </c>
-      <c r="J4" s="159" t="s">
+      <c r="J4" s="324" t="s">
         <v>108</v>
       </c>
-      <c r="K4" s="163" t="s">
+      <c r="K4" s="328" t="s">
         <v>110</v>
       </c>
       <c r="U4" s="6"/>
@@ -9029,27 +9524,27 @@
     <row r="5" spans="1:31" ht="86" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5"/>
-      <c r="C5" s="138" t="s">
+      <c r="C5" s="303" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="142" t="s">
+      <c r="D5" s="307" t="s">
         <v>89</v>
       </c>
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
-      <c r="G5" s="148" t="s">
+      <c r="G5" s="313" t="s">
         <v>70</v>
       </c>
-      <c r="H5" s="152" t="s">
+      <c r="H5" s="317" t="s">
         <v>94</v>
       </c>
-      <c r="I5" s="156" t="s">
+      <c r="I5" s="321" t="s">
         <v>88</v>
       </c>
-      <c r="J5" s="160" t="s">
+      <c r="J5" s="325" t="s">
         <v>96</v>
       </c>
-      <c r="K5" s="164" t="s">
+      <c r="K5" s="329" t="s">
         <v>98</v>
       </c>
       <c r="U5" s="6"/>
@@ -9063,27 +9558,27 @@
     <row r="6" spans="1:31" ht="86" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6"/>
-      <c r="C6" s="139" t="s">
+      <c r="C6" s="304" t="s">
         <v>80</v>
       </c>
-      <c r="D6" s="143" t="s">
+      <c r="D6" s="308" t="s">
         <v>89</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
-      <c r="G6" s="149" t="s">
+      <c r="G6" s="314" t="s">
         <v>70</v>
       </c>
-      <c r="H6" s="153" t="s">
+      <c r="H6" s="318" t="s">
         <v>95</v>
       </c>
-      <c r="I6" s="157" t="s">
+      <c r="I6" s="322" t="s">
         <v>88</v>
       </c>
-      <c r="J6" s="161" t="s">
+      <c r="J6" s="326" t="s">
         <v>97</v>
       </c>
-      <c r="K6" s="165" t="s">
+      <c r="K6" s="330" t="s">
         <v>99</v>
       </c>
       <c r="U6" s="6"/>

</xml_diff>

<commit_message>
galacticPubs::publish() [2022-04-01 13:59:52]  added goyespaper.png to bundle
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -369,7 +369,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="112">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -1020,7 +1020,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="331">
+  <cellXfs count="386">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1285,6 +1285,171 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="1"/>
@@ -6665,62 +6830,62 @@
       <c r="Z2" s="4"/>
     </row>
     <row r="3" spans="1:26" ht="56" x14ac:dyDescent="0.15">
-      <c r="A3" s="276" t="s">
+      <c r="A3" s="331" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="279" t="s">
+      <c r="B3" s="334" t="s">
         <v>79</v>
       </c>
-      <c r="C3" s="282" t="s">
+      <c r="C3" s="337" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="285" t="s">
+      <c r="D3" s="340" t="s">
         <v>82</v>
       </c>
-      <c r="E3" s="288" t="s">
+      <c r="E3" s="343" t="s">
         <v>85</v>
       </c>
-      <c r="F3" s="291" t="s">
+      <c r="F3" s="346" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="56" x14ac:dyDescent="0.15">
-      <c r="A4" s="277" t="s">
+      <c r="A4" s="332" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="280" t="s">
+      <c r="B4" s="335" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="283" t="s">
+      <c r="C4" s="338" t="s">
         <v>81</v>
       </c>
-      <c r="D4" s="286" t="s">
+      <c r="D4" s="341" t="s">
         <v>83</v>
       </c>
-      <c r="E4" s="289" t="s">
+      <c r="E4" s="344" t="s">
         <v>86</v>
       </c>
-      <c r="F4" s="292" t="s">
+      <c r="F4" s="347" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="56" x14ac:dyDescent="0.15">
-      <c r="A5" s="278" t="s">
+      <c r="A5" s="333" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="281" t="s">
+      <c r="B5" s="336" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="284" t="s">
+      <c r="C5" s="339" t="s">
         <v>81</v>
       </c>
-      <c r="D5" s="287" t="s">
+      <c r="D5" s="342" t="s">
         <v>84</v>
       </c>
-      <c r="E5" s="290" t="s">
+      <c r="E5" s="345" t="s">
         <v>87</v>
       </c>
-      <c r="F5" s="293" t="s">
+      <c r="F5" s="348" t="s">
         <v>88</v>
       </c>
     </row>
@@ -7863,25 +8028,25 @@
     <row r="3" spans="1:30" ht="140" x14ac:dyDescent="0.15">
       <c r="A3" s="12"/>
       <c r="B3"/>
-      <c r="C3" s="294" t="s">
+      <c r="C3" s="349" t="s">
         <v>79</v>
       </c>
-      <c r="D3" s="295" t="s">
+      <c r="D3" s="350" t="s">
         <v>89</v>
       </c>
-      <c r="E3" s="296" t="s">
+      <c r="E3" s="351" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="297" t="s">
+      <c r="F3" s="352" t="s">
         <v>91</v>
       </c>
-      <c r="G3" s="298" t="s">
+      <c r="G3" s="353" t="s">
         <v>88</v>
       </c>
-      <c r="H3" s="299" t="s">
+      <c r="H3" s="354" t="s">
         <v>92</v>
       </c>
-      <c r="I3" s="300" t="s">
+      <c r="I3" s="355" t="s">
         <v>93</v>
       </c>
       <c r="J3"/>
@@ -9452,29 +9617,29 @@
     <row r="3" spans="1:31" ht="114" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
       <c r="B3"/>
-      <c r="C3" s="301" t="s">
+      <c r="C3" s="356" t="s">
         <v>79</v>
       </c>
-      <c r="D3" s="305" t="s">
+      <c r="D3" s="360" t="s">
         <v>89</v>
       </c>
-      <c r="E3" s="309" t="s">
+      <c r="E3" s="364" t="s">
         <v>100</v>
       </c>
       <c r="F3" s="13"/>
-      <c r="G3" s="311" t="s">
+      <c r="G3" s="366" t="s">
         <v>102</v>
       </c>
-      <c r="H3" s="315" t="s">
+      <c r="H3" s="370" t="s">
         <v>104</v>
       </c>
-      <c r="I3" s="319" t="s">
+      <c r="I3" s="374" t="s">
         <v>106</v>
       </c>
-      <c r="J3" s="323" t="s">
+      <c r="J3" s="378" t="s">
         <v>107</v>
       </c>
-      <c r="K3" s="327" t="s">
+      <c r="K3" s="382" t="s">
         <v>109</v>
       </c>
       <c r="U3" s="6"/>
@@ -9488,29 +9653,29 @@
     <row r="4" spans="1:31" ht="114" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
       <c r="B4"/>
-      <c r="C4" s="302" t="s">
+      <c r="C4" s="357" t="s">
         <v>79</v>
       </c>
-      <c r="D4" s="306" t="s">
+      <c r="D4" s="361" t="s">
         <v>89</v>
       </c>
-      <c r="E4" s="310" t="s">
+      <c r="E4" s="365" t="s">
         <v>101</v>
       </c>
       <c r="F4" s="13"/>
-      <c r="G4" s="312" t="s">
+      <c r="G4" s="367" t="s">
         <v>103</v>
       </c>
-      <c r="H4" s="316" t="s">
+      <c r="H4" s="371" t="s">
         <v>105</v>
       </c>
-      <c r="I4" s="320" t="s">
+      <c r="I4" s="375" t="s">
         <v>106</v>
       </c>
-      <c r="J4" s="324" t="s">
+      <c r="J4" s="379" t="s">
         <v>108</v>
       </c>
-      <c r="K4" s="328" t="s">
+      <c r="K4" s="383" t="s">
         <v>110</v>
       </c>
       <c r="U4" s="6"/>
@@ -9524,27 +9689,27 @@
     <row r="5" spans="1:31" ht="86" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5"/>
-      <c r="C5" s="303" t="s">
+      <c r="C5" s="358" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="307" t="s">
+      <c r="D5" s="362" t="s">
         <v>89</v>
       </c>
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
-      <c r="G5" s="313" t="s">
+      <c r="G5" s="368" t="s">
         <v>70</v>
       </c>
-      <c r="H5" s="317" t="s">
+      <c r="H5" s="372" t="s">
         <v>94</v>
       </c>
-      <c r="I5" s="321" t="s">
+      <c r="I5" s="376" t="s">
         <v>88</v>
       </c>
-      <c r="J5" s="325" t="s">
+      <c r="J5" s="380" t="s">
         <v>96</v>
       </c>
-      <c r="K5" s="329" t="s">
+      <c r="K5" s="384" t="s">
         <v>98</v>
       </c>
       <c r="U5" s="6"/>
@@ -9558,27 +9723,27 @@
     <row r="6" spans="1:31" ht="86" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6"/>
-      <c r="C6" s="304" t="s">
+      <c r="C6" s="359" t="s">
         <v>80</v>
       </c>
-      <c r="D6" s="308" t="s">
+      <c r="D6" s="363" t="s">
         <v>89</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
-      <c r="G6" s="314" t="s">
+      <c r="G6" s="369" t="s">
         <v>70</v>
       </c>
-      <c r="H6" s="318" t="s">
+      <c r="H6" s="373" t="s">
         <v>95</v>
       </c>
-      <c r="I6" s="322" t="s">
+      <c r="I6" s="377" t="s">
         <v>88</v>
       </c>
-      <c r="J6" s="326" t="s">
+      <c r="J6" s="381" t="s">
         <v>97</v>
       </c>
-      <c r="K6" s="330" t="s">
+      <c r="K6" s="385" t="s">
         <v>99</v>
       </c>
       <c r="U6" s="6"/>

</xml_diff>

<commit_message>
galacticPubs::publish() [2022-04-01 15:10:37]  minor stuff
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -369,7 +369,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="112">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -1020,7 +1020,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="386">
+  <cellXfs count="441">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1285,6 +1285,171 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="1"/>
@@ -6830,62 +6995,62 @@
       <c r="Z2" s="4"/>
     </row>
     <row r="3" spans="1:26" ht="56" x14ac:dyDescent="0.15">
-      <c r="A3" s="331" t="s">
+      <c r="A3" s="386" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="334" t="s">
+      <c r="B3" s="389" t="s">
         <v>79</v>
       </c>
-      <c r="C3" s="337" t="s">
+      <c r="C3" s="392" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="340" t="s">
+      <c r="D3" s="395" t="s">
         <v>82</v>
       </c>
-      <c r="E3" s="343" t="s">
+      <c r="E3" s="398" t="s">
         <v>85</v>
       </c>
-      <c r="F3" s="346" t="s">
+      <c r="F3" s="401" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="56" x14ac:dyDescent="0.15">
-      <c r="A4" s="332" t="s">
+      <c r="A4" s="387" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="335" t="s">
+      <c r="B4" s="390" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="338" t="s">
+      <c r="C4" s="393" t="s">
         <v>81</v>
       </c>
-      <c r="D4" s="341" t="s">
+      <c r="D4" s="396" t="s">
         <v>83</v>
       </c>
-      <c r="E4" s="344" t="s">
+      <c r="E4" s="399" t="s">
         <v>86</v>
       </c>
-      <c r="F4" s="347" t="s">
+      <c r="F4" s="402" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="56" x14ac:dyDescent="0.15">
-      <c r="A5" s="333" t="s">
+      <c r="A5" s="388" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="336" t="s">
+      <c r="B5" s="391" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="339" t="s">
+      <c r="C5" s="394" t="s">
         <v>81</v>
       </c>
-      <c r="D5" s="342" t="s">
+      <c r="D5" s="397" t="s">
         <v>84</v>
       </c>
-      <c r="E5" s="345" t="s">
+      <c r="E5" s="400" t="s">
         <v>87</v>
       </c>
-      <c r="F5" s="348" t="s">
+      <c r="F5" s="403" t="s">
         <v>88</v>
       </c>
     </row>
@@ -8028,25 +8193,25 @@
     <row r="3" spans="1:30" ht="140" x14ac:dyDescent="0.15">
       <c r="A3" s="12"/>
       <c r="B3"/>
-      <c r="C3" s="349" t="s">
+      <c r="C3" s="404" t="s">
         <v>79</v>
       </c>
-      <c r="D3" s="350" t="s">
+      <c r="D3" s="405" t="s">
         <v>89</v>
       </c>
-      <c r="E3" s="351" t="s">
+      <c r="E3" s="406" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="352" t="s">
+      <c r="F3" s="407" t="s">
         <v>91</v>
       </c>
-      <c r="G3" s="353" t="s">
+      <c r="G3" s="408" t="s">
         <v>88</v>
       </c>
-      <c r="H3" s="354" t="s">
+      <c r="H3" s="409" t="s">
         <v>92</v>
       </c>
-      <c r="I3" s="355" t="s">
+      <c r="I3" s="410" t="s">
         <v>93</v>
       </c>
       <c r="J3"/>
@@ -9617,29 +9782,29 @@
     <row r="3" spans="1:31" ht="114" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
       <c r="B3"/>
-      <c r="C3" s="356" t="s">
+      <c r="C3" s="411" t="s">
         <v>79</v>
       </c>
-      <c r="D3" s="360" t="s">
+      <c r="D3" s="415" t="s">
         <v>89</v>
       </c>
-      <c r="E3" s="364" t="s">
+      <c r="E3" s="419" t="s">
         <v>100</v>
       </c>
       <c r="F3" s="13"/>
-      <c r="G3" s="366" t="s">
+      <c r="G3" s="421" t="s">
         <v>102</v>
       </c>
-      <c r="H3" s="370" t="s">
+      <c r="H3" s="425" t="s">
         <v>104</v>
       </c>
-      <c r="I3" s="374" t="s">
+      <c r="I3" s="429" t="s">
         <v>106</v>
       </c>
-      <c r="J3" s="378" t="s">
+      <c r="J3" s="433" t="s">
         <v>107</v>
       </c>
-      <c r="K3" s="382" t="s">
+      <c r="K3" s="437" t="s">
         <v>109</v>
       </c>
       <c r="U3" s="6"/>
@@ -9653,29 +9818,29 @@
     <row r="4" spans="1:31" ht="114" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
       <c r="B4"/>
-      <c r="C4" s="357" t="s">
+      <c r="C4" s="412" t="s">
         <v>79</v>
       </c>
-      <c r="D4" s="361" t="s">
+      <c r="D4" s="416" t="s">
         <v>89</v>
       </c>
-      <c r="E4" s="365" t="s">
+      <c r="E4" s="420" t="s">
         <v>101</v>
       </c>
       <c r="F4" s="13"/>
-      <c r="G4" s="367" t="s">
+      <c r="G4" s="422" t="s">
         <v>103</v>
       </c>
-      <c r="H4" s="371" t="s">
+      <c r="H4" s="426" t="s">
         <v>105</v>
       </c>
-      <c r="I4" s="375" t="s">
+      <c r="I4" s="430" t="s">
         <v>106</v>
       </c>
-      <c r="J4" s="379" t="s">
+      <c r="J4" s="434" t="s">
         <v>108</v>
       </c>
-      <c r="K4" s="383" t="s">
+      <c r="K4" s="438" t="s">
         <v>110</v>
       </c>
       <c r="U4" s="6"/>
@@ -9689,27 +9854,27 @@
     <row r="5" spans="1:31" ht="86" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5"/>
-      <c r="C5" s="358" t="s">
+      <c r="C5" s="413" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="362" t="s">
+      <c r="D5" s="417" t="s">
         <v>89</v>
       </c>
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
-      <c r="G5" s="368" t="s">
+      <c r="G5" s="423" t="s">
         <v>70</v>
       </c>
-      <c r="H5" s="372" t="s">
+      <c r="H5" s="427" t="s">
         <v>94</v>
       </c>
-      <c r="I5" s="376" t="s">
+      <c r="I5" s="431" t="s">
         <v>88</v>
       </c>
-      <c r="J5" s="380" t="s">
+      <c r="J5" s="435" t="s">
         <v>96</v>
       </c>
-      <c r="K5" s="384" t="s">
+      <c r="K5" s="439" t="s">
         <v>98</v>
       </c>
       <c r="U5" s="6"/>
@@ -9723,27 +9888,27 @@
     <row r="6" spans="1:31" ht="86" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6"/>
-      <c r="C6" s="359" t="s">
+      <c r="C6" s="414" t="s">
         <v>80</v>
       </c>
-      <c r="D6" s="363" t="s">
+      <c r="D6" s="418" t="s">
         <v>89</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
-      <c r="G6" s="369" t="s">
+      <c r="G6" s="424" t="s">
         <v>70</v>
       </c>
-      <c r="H6" s="373" t="s">
+      <c r="H6" s="428" t="s">
         <v>95</v>
       </c>
-      <c r="I6" s="377" t="s">
+      <c r="I6" s="432" t="s">
         <v>88</v>
       </c>
-      <c r="J6" s="381" t="s">
+      <c r="J6" s="436" t="s">
         <v>97</v>
       </c>
-      <c r="K6" s="385" t="s">
+      <c r="K6" s="440" t="s">
         <v>99</v>
       </c>
       <c r="U6" s="6"/>

</xml_diff>

<commit_message>
galacticPubs::publish() [2022-04-01 15:51:04]  fix Lesson.json??
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -369,7 +369,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="112">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -1020,7 +1020,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="441">
+  <cellXfs count="551">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1285,6 +1285,336 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="1"/>
@@ -6995,62 +7325,62 @@
       <c r="Z2" s="4"/>
     </row>
     <row r="3" spans="1:26" ht="56" x14ac:dyDescent="0.15">
-      <c r="A3" s="386" t="s">
+      <c r="A3" s="496" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="389" t="s">
+      <c r="B3" s="499" t="s">
         <v>79</v>
       </c>
-      <c r="C3" s="392" t="s">
+      <c r="C3" s="502" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="395" t="s">
+      <c r="D3" s="505" t="s">
         <v>82</v>
       </c>
-      <c r="E3" s="398" t="s">
+      <c r="E3" s="508" t="s">
         <v>85</v>
       </c>
-      <c r="F3" s="401" t="s">
+      <c r="F3" s="511" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="56" x14ac:dyDescent="0.15">
-      <c r="A4" s="387" t="s">
+      <c r="A4" s="497" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="390" t="s">
+      <c r="B4" s="500" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="393" t="s">
+      <c r="C4" s="503" t="s">
         <v>81</v>
       </c>
-      <c r="D4" s="396" t="s">
+      <c r="D4" s="506" t="s">
         <v>83</v>
       </c>
-      <c r="E4" s="399" t="s">
+      <c r="E4" s="509" t="s">
         <v>86</v>
       </c>
-      <c r="F4" s="402" t="s">
+      <c r="F4" s="512" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="56" x14ac:dyDescent="0.15">
-      <c r="A5" s="388" t="s">
+      <c r="A5" s="498" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="391" t="s">
+      <c r="B5" s="501" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="394" t="s">
+      <c r="C5" s="504" t="s">
         <v>81</v>
       </c>
-      <c r="D5" s="397" t="s">
+      <c r="D5" s="507" t="s">
         <v>84</v>
       </c>
-      <c r="E5" s="400" t="s">
+      <c r="E5" s="510" t="s">
         <v>87</v>
       </c>
-      <c r="F5" s="403" t="s">
+      <c r="F5" s="513" t="s">
         <v>88</v>
       </c>
     </row>
@@ -8193,25 +8523,25 @@
     <row r="3" spans="1:30" ht="140" x14ac:dyDescent="0.15">
       <c r="A3" s="12"/>
       <c r="B3"/>
-      <c r="C3" s="404" t="s">
+      <c r="C3" s="514" t="s">
         <v>79</v>
       </c>
-      <c r="D3" s="405" t="s">
+      <c r="D3" s="515" t="s">
         <v>89</v>
       </c>
-      <c r="E3" s="406" t="s">
+      <c r="E3" s="516" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="407" t="s">
+      <c r="F3" s="517" t="s">
         <v>91</v>
       </c>
-      <c r="G3" s="408" t="s">
+      <c r="G3" s="518" t="s">
         <v>88</v>
       </c>
-      <c r="H3" s="409" t="s">
+      <c r="H3" s="519" t="s">
         <v>92</v>
       </c>
-      <c r="I3" s="410" t="s">
+      <c r="I3" s="520" t="s">
         <v>93</v>
       </c>
       <c r="J3"/>
@@ -9782,29 +10112,29 @@
     <row r="3" spans="1:31" ht="114" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
       <c r="B3"/>
-      <c r="C3" s="411" t="s">
+      <c r="C3" s="521" t="s">
         <v>79</v>
       </c>
-      <c r="D3" s="415" t="s">
+      <c r="D3" s="525" t="s">
         <v>89</v>
       </c>
-      <c r="E3" s="419" t="s">
+      <c r="E3" s="529" t="s">
         <v>100</v>
       </c>
       <c r="F3" s="13"/>
-      <c r="G3" s="421" t="s">
+      <c r="G3" s="531" t="s">
         <v>102</v>
       </c>
-      <c r="H3" s="425" t="s">
+      <c r="H3" s="535" t="s">
         <v>104</v>
       </c>
-      <c r="I3" s="429" t="s">
+      <c r="I3" s="539" t="s">
         <v>106</v>
       </c>
-      <c r="J3" s="433" t="s">
+      <c r="J3" s="543" t="s">
         <v>107</v>
       </c>
-      <c r="K3" s="437" t="s">
+      <c r="K3" s="547" t="s">
         <v>109</v>
       </c>
       <c r="U3" s="6"/>
@@ -9818,29 +10148,29 @@
     <row r="4" spans="1:31" ht="114" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
       <c r="B4"/>
-      <c r="C4" s="412" t="s">
+      <c r="C4" s="522" t="s">
         <v>79</v>
       </c>
-      <c r="D4" s="416" t="s">
+      <c r="D4" s="526" t="s">
         <v>89</v>
       </c>
-      <c r="E4" s="420" t="s">
+      <c r="E4" s="530" t="s">
         <v>101</v>
       </c>
       <c r="F4" s="13"/>
-      <c r="G4" s="422" t="s">
+      <c r="G4" s="532" t="s">
         <v>103</v>
       </c>
-      <c r="H4" s="426" t="s">
+      <c r="H4" s="536" t="s">
         <v>105</v>
       </c>
-      <c r="I4" s="430" t="s">
+      <c r="I4" s="540" t="s">
         <v>106</v>
       </c>
-      <c r="J4" s="434" t="s">
+      <c r="J4" s="544" t="s">
         <v>108</v>
       </c>
-      <c r="K4" s="438" t="s">
+      <c r="K4" s="548" t="s">
         <v>110</v>
       </c>
       <c r="U4" s="6"/>
@@ -9854,27 +10184,27 @@
     <row r="5" spans="1:31" ht="86" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5"/>
-      <c r="C5" s="413" t="s">
+      <c r="C5" s="523" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="417" t="s">
+      <c r="D5" s="527" t="s">
         <v>89</v>
       </c>
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
-      <c r="G5" s="423" t="s">
+      <c r="G5" s="533" t="s">
         <v>70</v>
       </c>
-      <c r="H5" s="427" t="s">
+      <c r="H5" s="537" t="s">
         <v>94</v>
       </c>
-      <c r="I5" s="431" t="s">
+      <c r="I5" s="541" t="s">
         <v>88</v>
       </c>
-      <c r="J5" s="435" t="s">
+      <c r="J5" s="545" t="s">
         <v>96</v>
       </c>
-      <c r="K5" s="439" t="s">
+      <c r="K5" s="549" t="s">
         <v>98</v>
       </c>
       <c r="U5" s="6"/>
@@ -9888,27 +10218,27 @@
     <row r="6" spans="1:31" ht="86" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6"/>
-      <c r="C6" s="414" t="s">
+      <c r="C6" s="524" t="s">
         <v>80</v>
       </c>
-      <c r="D6" s="418" t="s">
+      <c r="D6" s="528" t="s">
         <v>89</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
-      <c r="G6" s="424" t="s">
+      <c r="G6" s="534" t="s">
         <v>70</v>
       </c>
-      <c r="H6" s="428" t="s">
+      <c r="H6" s="538" t="s">
         <v>95</v>
       </c>
-      <c r="I6" s="432" t="s">
+      <c r="I6" s="542" t="s">
         <v>88</v>
       </c>
-      <c r="J6" s="436" t="s">
+      <c r="J6" s="546" t="s">
         <v>97</v>
       </c>
-      <c r="K6" s="440" t="s">
+      <c r="K6" s="550" t="s">
         <v>99</v>
       </c>
       <c r="U6" s="6"/>

</xml_diff>

<commit_message>
galacticPubs::publish() [2022-04-07 16:22:14]  fix newline in matts credit
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -333,7 +333,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="110">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -971,7 +971,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="269">
+  <cellXfs count="328">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1230,6 +1230,183 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="1"/>
@@ -4821,42 +4998,42 @@
       <c r="Z2" s="4"/>
     </row>
     <row r="3" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A3" s="210" t="s">
+      <c r="A3" s="269" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="212" t="s">
+      <c r="B3" s="271" t="s">
         <v>88</v>
       </c>
-      <c r="C3" s="214" t="s">
+      <c r="C3" s="273" t="s">
         <v>89</v>
       </c>
-      <c r="D3" s="216" t="s">
+      <c r="D3" s="275" t="s">
         <v>90</v>
       </c>
-      <c r="E3" s="218" t="s">
+      <c r="E3" s="277" t="s">
         <v>92</v>
       </c>
-      <c r="F3" s="220" t="s">
+      <c r="F3" s="279" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A4" s="211" t="s">
+      <c r="A4" s="270" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="213" t="s">
+      <c r="B4" s="272" t="s">
         <v>89</v>
       </c>
-      <c r="C4" s="215" t="s">
+      <c r="C4" s="274" t="s">
         <v>89</v>
       </c>
-      <c r="D4" s="217" t="s">
+      <c r="D4" s="276" t="s">
         <v>91</v>
       </c>
-      <c r="E4" s="219" t="s">
+      <c r="E4" s="278" t="s">
         <v>93</v>
       </c>
-      <c r="F4" s="221" t="s">
+      <c r="F4" s="280" t="s">
         <v>94</v>
       </c>
     </row>
@@ -6007,25 +6184,25 @@
     <row r="3" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="18"/>
       <c r="B3"/>
-      <c r="C3" s="222" t="s">
+      <c r="C3" s="281" t="s">
         <v>88</v>
       </c>
-      <c r="D3" s="224" t="s">
+      <c r="D3" s="283" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="226" t="s">
+      <c r="E3" s="285" t="s">
         <v>95</v>
       </c>
-      <c r="F3" s="228" t="s">
+      <c r="F3" s="287" t="s">
         <v>96</v>
       </c>
-      <c r="G3" s="230" t="s">
+      <c r="G3" s="289" t="s">
         <v>97</v>
       </c>
-      <c r="H3" s="232" t="s">
+      <c r="H3" s="291" t="s">
         <v>98</v>
       </c>
-      <c r="I3" s="234" t="s">
+      <c r="I3" s="293" t="s">
         <v>99</v>
       </c>
       <c r="J3"/>
@@ -6033,25 +6210,25 @@
     <row r="4" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="18"/>
       <c r="B4"/>
-      <c r="C4" s="223" t="s">
+      <c r="C4" s="282" t="s">
         <v>88</v>
       </c>
-      <c r="D4" s="225" t="s">
+      <c r="D4" s="284" t="s">
         <v>100</v>
       </c>
-      <c r="E4" s="227" t="s">
+      <c r="E4" s="286" t="s">
         <v>101</v>
       </c>
-      <c r="F4" s="229" t="s">
+      <c r="F4" s="288" t="s">
         <v>102</v>
       </c>
-      <c r="G4" s="231" t="s">
+      <c r="G4" s="290" t="s">
         <v>103</v>
       </c>
-      <c r="H4" s="233" t="s">
+      <c r="H4" s="292" t="s">
         <v>104</v>
       </c>
-      <c r="I4" s="235" t="s">
+      <c r="I4" s="294" t="s">
         <v>105</v>
       </c>
       <c r="J4"/>
@@ -7612,31 +7789,31 @@
     <row r="3" spans="1:31" ht="114" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
       <c r="B3"/>
-      <c r="C3" s="236" t="s">
+      <c r="C3" s="295" t="s">
         <v>88</v>
       </c>
-      <c r="D3" s="240" t="s">
+      <c r="D3" s="299" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="244" t="s">
+      <c r="E3" s="303" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="247" t="s">
+      <c r="F3" s="306" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="250" t="s">
+      <c r="G3" s="309" t="s">
         <v>41</v>
       </c>
-      <c r="H3" s="254" t="s">
+      <c r="H3" s="313" t="s">
         <v>42</v>
       </c>
-      <c r="I3" s="258" t="s">
+      <c r="I3" s="317" t="s">
         <v>43</v>
       </c>
-      <c r="J3" s="262" t="s">
+      <c r="J3" s="321" t="s">
         <v>44</v>
       </c>
-      <c r="K3" s="265" t="s">
+      <c r="K3" s="324" t="s">
         <v>45</v>
       </c>
       <c r="U3" s="6"/>
@@ -7650,31 +7827,31 @@
     <row r="4" spans="1:31" ht="114" x14ac:dyDescent="0.25">
       <c r="A4" s="18"/>
       <c r="B4"/>
-      <c r="C4" s="237" t="s">
+      <c r="C4" s="296" t="s">
         <v>88</v>
       </c>
-      <c r="D4" s="241" t="s">
+      <c r="D4" s="300" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="245" t="s">
+      <c r="E4" s="304" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="248" t="s">
+      <c r="F4" s="307" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="251" t="s">
+      <c r="G4" s="310" t="s">
         <v>47</v>
       </c>
-      <c r="H4" s="255" t="s">
+      <c r="H4" s="314" t="s">
         <v>48</v>
       </c>
-      <c r="I4" s="259" t="s">
+      <c r="I4" s="318" t="s">
         <v>43</v>
       </c>
-      <c r="J4" s="263" t="s">
+      <c r="J4" s="322" t="s">
         <v>49</v>
       </c>
-      <c r="K4" s="266" t="s">
+      <c r="K4" s="325" t="s">
         <v>50</v>
       </c>
       <c r="U4" s="6"/>
@@ -7688,27 +7865,27 @@
     <row r="5" spans="1:31" ht="86" x14ac:dyDescent="0.25">
       <c r="A5" s="18"/>
       <c r="B5"/>
-      <c r="C5" s="238" t="s">
+      <c r="C5" s="297" t="s">
         <v>88</v>
       </c>
-      <c r="D5" s="242" t="s">
+      <c r="D5" s="301" t="s">
         <v>35</v>
       </c>
       <c r="E5" s="10"/>
-      <c r="F5" s="249" t="s">
+      <c r="F5" s="308" t="s">
         <v>51</v>
       </c>
-      <c r="G5" s="252" t="s">
+      <c r="G5" s="311" t="s">
         <v>52</v>
       </c>
-      <c r="H5" s="256" t="s">
+      <c r="H5" s="315" t="s">
         <v>53</v>
       </c>
-      <c r="I5" s="260" t="s">
+      <c r="I5" s="319" t="s">
         <v>43</v>
       </c>
       <c r="J5" s="10"/>
-      <c r="K5" s="267" t="s">
+      <c r="K5" s="326" t="s">
         <v>54</v>
       </c>
       <c r="U5" s="6"/>
@@ -7722,29 +7899,29 @@
     <row r="6" spans="1:31" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="18"/>
       <c r="B6"/>
-      <c r="C6" s="239" t="s">
+      <c r="C6" s="298" t="s">
         <v>88</v>
       </c>
-      <c r="D6" s="243" t="s">
+      <c r="D6" s="302" t="s">
         <v>100</v>
       </c>
-      <c r="E6" s="246" t="s">
+      <c r="E6" s="305" t="s">
         <v>46</v>
       </c>
       <c r="F6" s="45"/>
-      <c r="G6" s="253" t="s">
+      <c r="G6" s="312" t="s">
         <v>106</v>
       </c>
-      <c r="H6" s="257" t="s">
+      <c r="H6" s="316" t="s">
         <v>107</v>
       </c>
-      <c r="I6" s="261" t="s">
+      <c r="I6" s="320" t="s">
         <v>103</v>
       </c>
-      <c r="J6" s="264" t="s">
+      <c r="J6" s="323" t="s">
         <v>108</v>
       </c>
-      <c r="K6" s="268" t="s">
+      <c r="K6" s="327" t="s">
         <v>109</v>
       </c>
       <c r="U6" s="6"/>

</xml_diff>

<commit_message>
galacticPubs::publish() [2022-04-13 21:13:39]  update description
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -333,7 +333,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="120">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -664,6 +664,36 @@
   <si>
     <t>https://docs.google.com/document/d/1pUnNjrLkayEH_1K1iulty1cXUvgHyXWgZ-oofdWXgKA/export?format=pdf</t>
   </si>
+  <si>
+    <t>Guardian Frogs_P1_wksht (STUDENT)</t>
+  </si>
+  <si>
+    <t>GuardianFrogs_P2_G5-8_Worksheet (STUDENT)</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/19keieRWuq3pJS_zOyp9hTqrGTC7z-vJzge7FF3y-64o/edit?usp=drivesdk</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/1pFSciyHTTZclKGkx8qYPAvp8n_dXXR00I7IGLHCUOQI/edit?usp=drivesdk</t>
+  </si>
+  <si>
+    <t>trashed?</t>
+  </si>
+  <si>
+    <t>Wed Apr 13 21:13:23 2022</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/19keieRWuq3pJS_zOyp9hTqrGTC7z-vJzge7FF3y-64o/</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/1pFSciyHTTZclKGkx8qYPAvp8n_dXXR00I7IGLHCUOQI/</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/19keieRWuq3pJS_zOyp9hTqrGTC7z-vJzge7FF3y-64o/export?format=pdf</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/1pFSciyHTTZclKGkx8qYPAvp8n_dXXR00I7IGLHCUOQI/export?format=pdf</t>
+  </si>
 </sst>
 </file>
 
@@ -971,7 +1001,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="328">
+  <cellXfs count="403">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1230,6 +1260,231 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="1"/>
@@ -4998,42 +5253,42 @@
       <c r="Z2" s="4"/>
     </row>
     <row r="3" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A3" s="269" t="s">
+      <c r="A3" s="328" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="271" t="s">
+      <c r="B3" s="330" t="s">
         <v>88</v>
       </c>
-      <c r="C3" s="273" t="s">
+      <c r="C3" s="332" t="s">
         <v>89</v>
       </c>
-      <c r="D3" s="275" t="s">
+      <c r="D3" s="334" t="s">
         <v>90</v>
       </c>
-      <c r="E3" s="277" t="s">
+      <c r="E3" s="336" t="s">
         <v>92</v>
       </c>
-      <c r="F3" s="279" t="s">
+      <c r="F3" s="338" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A4" s="270" t="s">
+      <c r="A4" s="329" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="272" t="s">
+      <c r="B4" s="331" t="s">
         <v>89</v>
       </c>
-      <c r="C4" s="274" t="s">
+      <c r="C4" s="333" t="s">
         <v>89</v>
       </c>
-      <c r="D4" s="276" t="s">
+      <c r="D4" s="335" t="s">
         <v>91</v>
       </c>
-      <c r="E4" s="278" t="s">
+      <c r="E4" s="337" t="s">
         <v>93</v>
       </c>
-      <c r="F4" s="280" t="s">
+      <c r="F4" s="339" t="s">
         <v>94</v>
       </c>
     </row>
@@ -6184,25 +6439,25 @@
     <row r="3" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="18"/>
       <c r="B3"/>
-      <c r="C3" s="281" t="s">
+      <c r="C3" s="340" t="s">
         <v>88</v>
       </c>
-      <c r="D3" s="283" t="s">
+      <c r="D3" s="342" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="285" t="s">
+      <c r="E3" s="344" t="s">
         <v>95</v>
       </c>
-      <c r="F3" s="287" t="s">
+      <c r="F3" s="346" t="s">
         <v>96</v>
       </c>
-      <c r="G3" s="289" t="s">
+      <c r="G3" s="348" t="s">
         <v>97</v>
       </c>
-      <c r="H3" s="291" t="s">
+      <c r="H3" s="350" t="s">
         <v>98</v>
       </c>
-      <c r="I3" s="293" t="s">
+      <c r="I3" s="352" t="s">
         <v>99</v>
       </c>
       <c r="J3"/>
@@ -6210,25 +6465,25 @@
     <row r="4" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="18"/>
       <c r="B4"/>
-      <c r="C4" s="282" t="s">
+      <c r="C4" s="341" t="s">
         <v>88</v>
       </c>
-      <c r="D4" s="284" t="s">
+      <c r="D4" s="343" t="s">
         <v>100</v>
       </c>
-      <c r="E4" s="286" t="s">
+      <c r="E4" s="345" t="s">
         <v>101</v>
       </c>
-      <c r="F4" s="288" t="s">
+      <c r="F4" s="347" t="s">
         <v>102</v>
       </c>
-      <c r="G4" s="290" t="s">
+      <c r="G4" s="349" t="s">
         <v>103</v>
       </c>
-      <c r="H4" s="292" t="s">
+      <c r="H4" s="351" t="s">
         <v>104</v>
       </c>
-      <c r="I4" s="294" t="s">
+      <c r="I4" s="353" t="s">
         <v>105</v>
       </c>
       <c r="J4"/>
@@ -7789,31 +8044,31 @@
     <row r="3" spans="1:31" ht="114" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
       <c r="B3"/>
-      <c r="C3" s="295" t="s">
+      <c r="C3" s="354" t="s">
         <v>88</v>
       </c>
-      <c r="D3" s="299" t="s">
+      <c r="D3" s="360" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="303" t="s">
+      <c r="E3" s="366" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="306" t="s">
+      <c r="F3" s="371" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="309" t="s">
+      <c r="G3" s="374" t="s">
         <v>41</v>
       </c>
-      <c r="H3" s="313" t="s">
+      <c r="H3" s="380" t="s">
         <v>42</v>
       </c>
-      <c r="I3" s="317" t="s">
-        <v>43</v>
-      </c>
-      <c r="J3" s="321" t="s">
+      <c r="I3" s="386" t="s">
+        <v>114</v>
+      </c>
+      <c r="J3" s="392" t="s">
         <v>44</v>
       </c>
-      <c r="K3" s="324" t="s">
+      <c r="K3" s="397" t="s">
         <v>45</v>
       </c>
       <c r="U3" s="6"/>
@@ -7827,32 +8082,30 @@
     <row r="4" spans="1:31" ht="114" x14ac:dyDescent="0.25">
       <c r="A4" s="18"/>
       <c r="B4"/>
-      <c r="C4" s="296" t="s">
+      <c r="C4" s="355" t="s">
         <v>88</v>
       </c>
-      <c r="D4" s="300" t="s">
+      <c r="D4" s="361" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="304" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" s="307" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="310" t="s">
-        <v>47</v>
-      </c>
-      <c r="H4" s="314" t="s">
-        <v>48</v>
-      </c>
-      <c r="I4" s="318" t="s">
-        <v>43</v>
-      </c>
-      <c r="J4" s="322" t="s">
-        <v>49</v>
-      </c>
-      <c r="K4" s="325" t="s">
-        <v>50</v>
+      <c r="E4" s="367" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="307"/>
+      <c r="G4" s="375" t="s">
+        <v>110</v>
+      </c>
+      <c r="H4" s="381" t="s">
+        <v>112</v>
+      </c>
+      <c r="I4" s="387" t="s">
+        <v>115</v>
+      </c>
+      <c r="J4" s="393" t="s">
+        <v>116</v>
+      </c>
+      <c r="K4" s="398" t="s">
+        <v>118</v>
       </c>
       <c r="U4" s="6"/>
       <c r="V4" s="6"/>
@@ -7865,28 +8118,32 @@
     <row r="5" spans="1:31" ht="86" x14ac:dyDescent="0.25">
       <c r="A5" s="18"/>
       <c r="B5"/>
-      <c r="C5" s="297" t="s">
+      <c r="C5" s="356" t="s">
         <v>88</v>
       </c>
-      <c r="D5" s="301" t="s">
+      <c r="D5" s="362" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="308" t="s">
-        <v>51</v>
-      </c>
-      <c r="G5" s="311" t="s">
-        <v>52</v>
-      </c>
-      <c r="H5" s="315" t="s">
-        <v>53</v>
-      </c>
-      <c r="I5" s="319" t="s">
+      <c r="E5" s="368" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" s="372" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="376" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" s="382" t="s">
+        <v>48</v>
+      </c>
+      <c r="I5" s="388" t="s">
         <v>43</v>
       </c>
-      <c r="J5" s="10"/>
-      <c r="K5" s="326" t="s">
-        <v>54</v>
+      <c r="J5" s="394" t="s">
+        <v>49</v>
+      </c>
+      <c r="K5" s="399" t="s">
+        <v>50</v>
       </c>
       <c r="U5" s="6"/>
       <c r="V5" s="6"/>
@@ -7899,30 +8156,28 @@
     <row r="6" spans="1:31" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="18"/>
       <c r="B6"/>
-      <c r="C6" s="298" t="s">
+      <c r="C6" s="357" t="s">
         <v>88</v>
       </c>
-      <c r="D6" s="302" t="s">
-        <v>100</v>
-      </c>
-      <c r="E6" s="305" t="s">
-        <v>46</v>
-      </c>
-      <c r="F6" s="45"/>
-      <c r="G6" s="312" t="s">
-        <v>106</v>
-      </c>
-      <c r="H6" s="316" t="s">
-        <v>107</v>
-      </c>
-      <c r="I6" s="320" t="s">
-        <v>103</v>
-      </c>
-      <c r="J6" s="323" t="s">
-        <v>108</v>
-      </c>
-      <c r="K6" s="327" t="s">
-        <v>109</v>
+      <c r="D6" s="363" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="305"/>
+      <c r="F6" s="373" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" s="377" t="s">
+        <v>52</v>
+      </c>
+      <c r="H6" s="383" t="s">
+        <v>53</v>
+      </c>
+      <c r="I6" s="389" t="s">
+        <v>43</v>
+      </c>
+      <c r="J6" s="323"/>
+      <c r="K6" s="400" t="s">
+        <v>54</v>
       </c>
       <c r="U6" s="6"/>
       <c r="V6" s="6"/>
@@ -7934,15 +8189,32 @@
     </row>
     <row r="7" spans="1:31" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="18"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
+      <c r="B7"/>
+      <c r="C7" s="358" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" s="364" t="s">
+        <v>100</v>
+      </c>
+      <c r="E7" s="369" t="s">
+        <v>40</v>
+      </c>
       <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
+      <c r="G7" s="378" t="s">
+        <v>111</v>
+      </c>
+      <c r="H7" s="384" t="s">
+        <v>113</v>
+      </c>
+      <c r="I7" s="390" t="s">
+        <v>115</v>
+      </c>
+      <c r="J7" s="395" t="s">
+        <v>117</v>
+      </c>
+      <c r="K7" s="401" t="s">
+        <v>119</v>
+      </c>
       <c r="U7" s="6"/>
       <c r="V7" s="6"/>
       <c r="W7" s="6"/>
@@ -7953,15 +8225,32 @@
     </row>
     <row r="8" spans="1:31" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" s="18"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
+      <c r="B8"/>
+      <c r="C8" s="359" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" s="365" t="s">
+        <v>100</v>
+      </c>
+      <c r="E8" s="370" t="s">
+        <v>46</v>
+      </c>
       <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
+      <c r="G8" s="379" t="s">
+        <v>106</v>
+      </c>
+      <c r="H8" s="385" t="s">
+        <v>107</v>
+      </c>
+      <c r="I8" s="391" t="s">
+        <v>103</v>
+      </c>
+      <c r="J8" s="396" t="s">
+        <v>108</v>
+      </c>
+      <c r="K8" s="402" t="s">
+        <v>109</v>
+      </c>
       <c r="U8" s="6"/>
       <c r="V8" s="6"/>
       <c r="W8" s="6"/>

</xml_diff>

<commit_message>
galacticPubs::publish() [2022-04-13 22:36:32]  adding in preview item #3
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Edu/Lessons/guardianFrogs_sci/meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E942C2-126E-7949-8780-8085CE90AB6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B93560AA-BCD5-BC4B-845E-470402F40468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,8 +30,18 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">r_handouts!$B$2:$T$100</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">r_pres!$A$2:$L$20</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId12" roundtripDataSignature="AMtx7mi8jE6NK7+9sXLqlVt44Zdkb/euag=="/>
     </ext>
@@ -333,7 +343,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="121">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -680,9 +690,6 @@
     <t>https://docs.google.com/document/d/1pFSciyHTTZclKGkx8qYPAvp8n_dXXR00I7IGLHCUOQI/export?format=pdf</t>
   </si>
   <si>
-    <t>Background</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=eX5abcrmE7g&amp;t=170s</t>
   </si>
   <si>
@@ -690,6 +697,15 @@
   </si>
   <si>
     <t>For Part 2: We show parts of this video to introduce students to Dr. Goyes-Vallejos and her research. They will then analyze some of her data.</t>
+  </si>
+  <si>
+    <t>Do Female Frogs Call?</t>
+  </si>
+  <si>
+    <t>iBiology</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/channel/UCsvqEZBO-kNmwuDBbKbfL6A</t>
   </si>
 </sst>
 </file>
@@ -699,7 +715,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -866,6 +882,13 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -998,7 +1021,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="390">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1311,6 +1334,799 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1610,12 +2426,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.83203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.5" customWidth="1" collapsed="1"/>
-    <col min="6" max="25" width="9.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="18.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="26.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.83203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="7.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="6" max="25" customWidth="true" width="9.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.15">
@@ -4356,13 +5172,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.5" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="98.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="26" width="9.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="17.5" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="10.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="9.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="98.33203125" collapsed="true"/>
+    <col min="7" max="26" customWidth="true" width="9.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4416,42 +5232,42 @@
       <c r="Z2" s="4"/>
     </row>
     <row r="3" spans="1:26" ht="56" x14ac:dyDescent="0.15">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="321" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="323" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="325" t="s">
         <v>85</v>
       </c>
-      <c r="D3" s="57" t="s">
+      <c r="D3" s="327" t="s">
         <v>86</v>
       </c>
-      <c r="E3" s="59" t="s">
+      <c r="E3" s="329" t="s">
         <v>88</v>
       </c>
-      <c r="F3" s="61" t="s">
+      <c r="F3" s="331" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="56" x14ac:dyDescent="0.15">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="322" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="54" t="s">
+      <c r="B4" s="324" t="s">
         <v>85</v>
       </c>
-      <c r="C4" s="56" t="s">
+      <c r="C4" s="326" t="s">
         <v>85</v>
       </c>
-      <c r="D4" s="58" t="s">
+      <c r="D4" s="328" t="s">
         <v>87</v>
       </c>
-      <c r="E4" s="60" t="s">
+      <c r="E4" s="330" t="s">
         <v>89</v>
       </c>
-      <c r="F4" s="62" t="s">
+      <c r="F4" s="332" t="s">
         <v>90</v>
       </c>
     </row>
@@ -5518,17 +6334,17 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.5" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.83203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="24.83203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.6640625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.1640625" customWidth="1" collapsed="1"/>
-    <col min="8" max="9" width="18.6640625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="30.6640625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="14.6640625" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="19" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="8.5" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="10.83203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="7.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="24.83203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="13.1640625" collapsed="true"/>
+    <col min="8" max="9" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="30.6640625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="19.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -5601,51 +6417,55 @@
     </row>
     <row r="3" spans="1:30" ht="140" x14ac:dyDescent="0.15">
       <c r="A3" s="18"/>
-      <c r="C3" s="63" t="s">
+      <c r="B3"/>
+      <c r="C3" s="333" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="65" t="s">
+      <c r="D3" s="335" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="67" t="s">
+      <c r="E3" s="337" t="s">
         <v>91</v>
       </c>
-      <c r="F3" s="69" t="s">
+      <c r="F3" s="339" t="s">
         <v>92</v>
       </c>
-      <c r="G3" s="71" t="s">
+      <c r="G3" s="341" t="s">
         <v>93</v>
       </c>
-      <c r="H3" s="73" t="s">
+      <c r="H3" s="343" t="s">
         <v>94</v>
       </c>
-      <c r="I3" s="75" t="s">
+      <c r="I3" s="345" t="s">
         <v>95</v>
       </c>
+      <c r="J3"/>
     </row>
     <row r="4" spans="1:30" ht="126" x14ac:dyDescent="0.15">
       <c r="A4" s="18"/>
-      <c r="C4" s="64" t="s">
+      <c r="B4"/>
+      <c r="C4" s="334" t="s">
         <v>84</v>
       </c>
-      <c r="D4" s="66" t="s">
+      <c r="D4" s="336" t="s">
         <v>96</v>
       </c>
-      <c r="E4" s="68" t="s">
+      <c r="E4" s="338" t="s">
         <v>97</v>
       </c>
-      <c r="F4" s="70" t="s">
+      <c r="F4" s="340" t="s">
         <v>98</v>
       </c>
-      <c r="G4" s="72" t="s">
+      <c r="G4" s="342" t="s">
         <v>99</v>
       </c>
-      <c r="H4" s="74" t="s">
+      <c r="H4" s="344" t="s">
         <v>100</v>
       </c>
-      <c r="I4" s="76" t="s">
+      <c r="I4" s="346" t="s">
         <v>101</v>
       </c>
+      <c r="J4"/>
     </row>
     <row r="5" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A5" s="18"/>
@@ -7096,18 +7916,18 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="11.5" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.1640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.1640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.1640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.6640625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.6640625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="18.6640625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.6640625" customWidth="1" collapsed="1"/>
-    <col min="12" max="31" width="9.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="11.5" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="10.1640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="8.1640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.1640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.6640625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="14.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="16.6640625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="16.6640625" collapsed="true"/>
+    <col min="12" max="31" customWidth="true" width="9.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -7202,31 +8022,32 @@
     </row>
     <row r="3" spans="1:31" ht="114" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
-      <c r="C3" s="77" t="s">
+      <c r="B3"/>
+      <c r="C3" s="347" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="82" t="s">
+      <c r="D3" s="352" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="87" t="s">
+      <c r="E3" s="357" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="91" t="s">
+      <c r="F3" s="361" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="94" t="s">
+      <c r="G3" s="366" t="s">
         <v>106</v>
       </c>
-      <c r="H3" s="99" t="s">
+      <c r="H3" s="371" t="s">
         <v>108</v>
       </c>
-      <c r="I3" s="104" t="s">
+      <c r="I3" s="376" t="s">
         <v>110</v>
       </c>
-      <c r="J3" s="109" t="s">
+      <c r="J3" s="381" t="s">
         <v>111</v>
       </c>
-      <c r="K3" s="113" t="s">
+      <c r="K3" s="385" t="s">
         <v>113</v>
       </c>
       <c r="U3" s="6"/>
@@ -7239,31 +8060,32 @@
     </row>
     <row r="4" spans="1:31" ht="114" x14ac:dyDescent="0.25">
       <c r="A4" s="18"/>
-      <c r="C4" s="78" t="s">
+      <c r="B4"/>
+      <c r="C4" s="348" t="s">
         <v>84</v>
       </c>
-      <c r="D4" s="83" t="s">
+      <c r="D4" s="353" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="88" t="s">
+      <c r="E4" s="358" t="s">
         <v>42</v>
       </c>
-      <c r="F4" s="92" t="s">
+      <c r="F4" s="362" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="95" t="s">
+      <c r="G4" s="367" t="s">
         <v>43</v>
       </c>
-      <c r="H4" s="100" t="s">
+      <c r="H4" s="372" t="s">
         <v>44</v>
       </c>
-      <c r="I4" s="105" t="s">
+      <c r="I4" s="377" t="s">
         <v>41</v>
       </c>
-      <c r="J4" s="110" t="s">
+      <c r="J4" s="382" t="s">
         <v>45</v>
       </c>
-      <c r="K4" s="114" t="s">
+      <c r="K4" s="386" t="s">
         <v>46</v>
       </c>
       <c r="U4" s="6"/>
@@ -7276,27 +8098,28 @@
     </row>
     <row r="5" spans="1:31" ht="86" x14ac:dyDescent="0.25">
       <c r="A5" s="18"/>
-      <c r="C5" s="79" t="s">
+      <c r="B5"/>
+      <c r="C5" s="349" t="s">
         <v>84</v>
       </c>
-      <c r="D5" s="84" t="s">
+      <c r="D5" s="354" t="s">
         <v>35</v>
       </c>
       <c r="E5" s="49"/>
-      <c r="F5" s="93" t="s">
+      <c r="F5" s="363" t="s">
         <v>47</v>
       </c>
-      <c r="G5" s="96" t="s">
+      <c r="G5" s="368" t="s">
         <v>48</v>
       </c>
-      <c r="H5" s="101" t="s">
+      <c r="H5" s="373" t="s">
         <v>49</v>
       </c>
-      <c r="I5" s="106" t="s">
+      <c r="I5" s="378" t="s">
         <v>41</v>
       </c>
       <c r="J5" s="50"/>
-      <c r="K5" s="115" t="s">
+      <c r="K5" s="387" t="s">
         <v>50</v>
       </c>
       <c r="U5" s="6"/>
@@ -7309,31 +8132,32 @@
     </row>
     <row r="6" spans="1:31" ht="100" x14ac:dyDescent="0.25">
       <c r="A6" s="18"/>
-      <c r="C6" s="80" t="s">
+      <c r="B6"/>
+      <c r="C6" s="350" t="s">
         <v>84</v>
       </c>
-      <c r="D6" s="85" t="s">
+      <c r="D6" s="355" t="s">
         <v>96</v>
       </c>
-      <c r="E6" s="89" t="s">
+      <c r="E6" s="359" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="364" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="97" t="s">
+      <c r="G6" s="369" t="s">
         <v>107</v>
       </c>
-      <c r="H6" s="102" t="s">
+      <c r="H6" s="374" t="s">
         <v>109</v>
       </c>
-      <c r="I6" s="107" t="s">
+      <c r="I6" s="379" t="s">
         <v>110</v>
       </c>
-      <c r="J6" s="111" t="s">
+      <c r="J6" s="383" t="s">
         <v>112</v>
       </c>
-      <c r="K6" s="116" t="s">
+      <c r="K6" s="388" t="s">
         <v>114</v>
       </c>
       <c r="U6" s="6"/>
@@ -7346,31 +8170,32 @@
     </row>
     <row r="7" spans="1:31" ht="100" x14ac:dyDescent="0.25">
       <c r="A7" s="18"/>
-      <c r="C7" s="81" t="s">
+      <c r="B7"/>
+      <c r="C7" s="351" t="s">
         <v>84</v>
       </c>
-      <c r="D7" s="86" t="s">
+      <c r="D7" s="356" t="s">
         <v>96</v>
       </c>
-      <c r="E7" s="90" t="s">
+      <c r="E7" s="360" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="365" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="98" t="s">
+      <c r="G7" s="370" t="s">
         <v>102</v>
       </c>
-      <c r="H7" s="103" t="s">
+      <c r="H7" s="375" t="s">
         <v>103</v>
       </c>
-      <c r="I7" s="108" t="s">
+      <c r="I7" s="380" t="s">
         <v>99</v>
       </c>
-      <c r="J7" s="112" t="s">
+      <c r="J7" s="384" t="s">
         <v>104</v>
       </c>
-      <c r="K7" s="117" t="s">
+      <c r="K7" s="389" t="s">
         <v>105</v>
       </c>
       <c r="U7" s="6"/>
@@ -9369,19 +10194,19 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.1640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="6.1640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.5" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.5" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.83203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.1640625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="19.1640625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="24.6640625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14.6640625" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="19" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="11.1640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="6.1640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.5" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="13.5" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="16.83203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.1640625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="19.1640625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="24.6640625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="19.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -11003,19 +11828,19 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="6.1640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="7.1640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.1640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="34.1640625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="19.6640625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.1640625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.5" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.83203125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.33203125" customWidth="1" collapsed="1"/>
-    <col min="12" max="13" width="9.5" customWidth="1" collapsed="1"/>
-    <col min="14" max="31" width="9.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="6.1640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="7.1640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="8.1640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="34.1640625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="19.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="15.1640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.5" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="14.83203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="14.33203125" collapsed="true"/>
+    <col min="12" max="13" customWidth="true" width="9.5" collapsed="true"/>
+    <col min="14" max="31" customWidth="true" width="9.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -13335,22 +14160,22 @@
   </sheetPr>
   <dimension ref="A1:AI1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.1640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="7.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="13.5" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="30.1640625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="21.1640625" customWidth="1" collapsed="1"/>
-    <col min="8" max="9" width="12.5" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17.83203125" customWidth="1" collapsed="1"/>
-    <col min="11" max="13" width="10.6640625" customWidth="1" collapsed="1"/>
-    <col min="14" max="15" width="14.1640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="7.1640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="7.6640625" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" width="13.5" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="30.1640625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="21.1640625" collapsed="true"/>
+    <col min="8" max="9" customWidth="true" width="12.5" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="17.83203125" collapsed="true"/>
+    <col min="11" max="13" customWidth="true" width="10.6640625" collapsed="true"/>
+    <col min="14" max="15" customWidth="true" width="14.1640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="18" customHeight="1" x14ac:dyDescent="0.15">
@@ -13503,7 +14328,7 @@
       <c r="O4" s="34"/>
       <c r="P4" s="35"/>
     </row>
-    <row r="5" spans="1:35" ht="356" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:35" ht="203" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="28" t="s">
         <v>73</v>
       </c>
@@ -13515,20 +14340,24 @@
         <v>2</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="F5" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="G5" s="31" t="s">
         <v>117</v>
-      </c>
-      <c r="G5" s="31" t="s">
-        <v>118</v>
       </c>
       <c r="H5" s="31"/>
       <c r="J5" s="32"/>
-      <c r="K5" s="32"/>
-      <c r="L5" s="32"/>
+      <c r="K5" s="125" t="s">
+        <v>119</v>
+      </c>
+      <c r="L5" s="32" t="s">
+        <v>120</v>
+      </c>
       <c r="M5" s="32" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="N5" s="29"/>
       <c r="O5" s="34"/>
@@ -18200,14 +19029,14 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:F1000"/>
+  <dimension ref="A1:A1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="131.1640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="6" width="9.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="131.1640625" collapsed="true"/>
+    <col min="2" max="6" customWidth="true" width="9.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
galacticPubs::publish() [2022-04-21 16:22:53]  first part of procedure drafted
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -343,7 +343,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="127">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -1039,7 +1039,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="266">
+  <cellXfs count="335">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1359,6 +1359,213 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="1"/>
@@ -4878,42 +5085,42 @@
       <c r="Z2" s="4"/>
     </row>
     <row r="3" spans="1:26" ht="56">
-      <c r="A3" s="197" t="s">
+      <c r="A3" s="266" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="199" t="s">
+      <c r="B3" s="268" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="201" t="s">
+      <c r="C3" s="270" t="s">
         <v>85</v>
       </c>
-      <c r="D3" s="203" t="s">
+      <c r="D3" s="272" t="s">
         <v>86</v>
       </c>
-      <c r="E3" s="205" t="s">
+      <c r="E3" s="274" t="s">
         <v>88</v>
       </c>
-      <c r="F3" s="207" t="s">
+      <c r="F3" s="276" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="56">
-      <c r="A4" s="198" t="s">
+      <c r="A4" s="267" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="200" t="s">
+      <c r="B4" s="269" t="s">
         <v>85</v>
       </c>
-      <c r="C4" s="202" t="s">
+      <c r="C4" s="271" t="s">
         <v>85</v>
       </c>
-      <c r="D4" s="204" t="s">
+      <c r="D4" s="273" t="s">
         <v>87</v>
       </c>
-      <c r="E4" s="206" t="s">
+      <c r="E4" s="275" t="s">
         <v>89</v>
       </c>
-      <c r="F4" s="208" t="s">
+      <c r="F4" s="277" t="s">
         <v>90</v>
       </c>
     </row>
@@ -6064,25 +6271,25 @@
     <row r="3" spans="1:30" ht="140">
       <c r="A3" s="18"/>
       <c r="B3"/>
-      <c r="C3" s="209" t="s">
+      <c r="C3" s="278" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="211" t="s">
+      <c r="D3" s="280" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="213" t="s">
+      <c r="E3" s="282" t="s">
         <v>91</v>
       </c>
-      <c r="F3" s="215" t="s">
+      <c r="F3" s="284" t="s">
         <v>92</v>
       </c>
-      <c r="G3" s="217" t="s">
+      <c r="G3" s="286" t="s">
         <v>93</v>
       </c>
-      <c r="H3" s="219" t="s">
+      <c r="H3" s="288" t="s">
         <v>94</v>
       </c>
-      <c r="I3" s="221" t="s">
+      <c r="I3" s="290" t="s">
         <v>95</v>
       </c>
       <c r="J3"/>
@@ -6090,25 +6297,25 @@
     <row r="4" spans="1:30" ht="126">
       <c r="A4" s="18"/>
       <c r="B4"/>
-      <c r="C4" s="210" t="s">
+      <c r="C4" s="279" t="s">
         <v>84</v>
       </c>
-      <c r="D4" s="212" t="s">
+      <c r="D4" s="281" t="s">
         <v>96</v>
       </c>
-      <c r="E4" s="214" t="s">
+      <c r="E4" s="283" t="s">
         <v>97</v>
       </c>
-      <c r="F4" s="216" t="s">
+      <c r="F4" s="285" t="s">
         <v>98</v>
       </c>
-      <c r="G4" s="218" t="s">
+      <c r="G4" s="287" t="s">
         <v>99</v>
       </c>
-      <c r="H4" s="220" t="s">
+      <c r="H4" s="289" t="s">
         <v>100</v>
       </c>
-      <c r="I4" s="222" t="s">
+      <c r="I4" s="291" t="s">
         <v>101</v>
       </c>
       <c r="J4"/>
@@ -7669,31 +7876,31 @@
     <row r="3" spans="1:31" ht="113">
       <c r="A3" s="18"/>
       <c r="B3"/>
-      <c r="C3" s="223" t="s">
+      <c r="C3" s="292" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="228" t="s">
+      <c r="D3" s="297" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="233" t="s">
+      <c r="E3" s="302" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="237" t="s">
+      <c r="F3" s="306" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="242" t="s">
+      <c r="G3" s="311" t="s">
         <v>106</v>
       </c>
-      <c r="H3" s="247" t="s">
+      <c r="H3" s="316" t="s">
         <v>108</v>
       </c>
-      <c r="I3" s="252" t="s">
+      <c r="I3" s="321" t="s">
         <v>110</v>
       </c>
-      <c r="J3" s="257" t="s">
+      <c r="J3" s="326" t="s">
         <v>111</v>
       </c>
-      <c r="K3" s="261" t="s">
+      <c r="K3" s="330" t="s">
         <v>113</v>
       </c>
       <c r="U3" s="6"/>
@@ -7707,31 +7914,31 @@
     <row r="4" spans="1:31" ht="113">
       <c r="A4" s="18"/>
       <c r="B4"/>
-      <c r="C4" s="224" t="s">
+      <c r="C4" s="293" t="s">
         <v>84</v>
       </c>
-      <c r="D4" s="229" t="s">
+      <c r="D4" s="298" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="234" t="s">
+      <c r="E4" s="303" t="s">
         <v>42</v>
       </c>
-      <c r="F4" s="238" t="s">
+      <c r="F4" s="307" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="243" t="s">
+      <c r="G4" s="312" t="s">
         <v>43</v>
       </c>
-      <c r="H4" s="248" t="s">
+      <c r="H4" s="317" t="s">
         <v>44</v>
       </c>
-      <c r="I4" s="253" t="s">
+      <c r="I4" s="322" t="s">
         <v>41</v>
       </c>
-      <c r="J4" s="258" t="s">
+      <c r="J4" s="327" t="s">
         <v>45</v>
       </c>
-      <c r="K4" s="262" t="s">
+      <c r="K4" s="331" t="s">
         <v>46</v>
       </c>
       <c r="U4" s="6"/>
@@ -7745,27 +7952,27 @@
     <row r="5" spans="1:31" ht="85">
       <c r="A5" s="18"/>
       <c r="B5"/>
-      <c r="C5" s="225" t="s">
+      <c r="C5" s="294" t="s">
         <v>84</v>
       </c>
-      <c r="D5" s="230" t="s">
+      <c r="D5" s="299" t="s">
         <v>35</v>
       </c>
       <c r="E5" s="49"/>
-      <c r="F5" s="239" t="s">
+      <c r="F5" s="308" t="s">
         <v>47</v>
       </c>
-      <c r="G5" s="244" t="s">
+      <c r="G5" s="313" t="s">
         <v>48</v>
       </c>
-      <c r="H5" s="249" t="s">
+      <c r="H5" s="318" t="s">
         <v>49</v>
       </c>
-      <c r="I5" s="254" t="s">
+      <c r="I5" s="323" t="s">
         <v>41</v>
       </c>
       <c r="J5" s="50"/>
-      <c r="K5" s="263" t="s">
+      <c r="K5" s="332" t="s">
         <v>50</v>
       </c>
       <c r="U5" s="6"/>
@@ -7779,31 +7986,31 @@
     <row r="6" spans="1:31" ht="99">
       <c r="A6" s="18"/>
       <c r="B6"/>
-      <c r="C6" s="226" t="s">
+      <c r="C6" s="295" t="s">
         <v>84</v>
       </c>
-      <c r="D6" s="231" t="s">
+      <c r="D6" s="300" t="s">
         <v>96</v>
       </c>
-      <c r="E6" s="235" t="s">
+      <c r="E6" s="304" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="240" t="s">
+      <c r="F6" s="309" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="245" t="s">
+      <c r="G6" s="314" t="s">
         <v>107</v>
       </c>
-      <c r="H6" s="250" t="s">
+      <c r="H6" s="319" t="s">
         <v>109</v>
       </c>
-      <c r="I6" s="255" t="s">
+      <c r="I6" s="324" t="s">
         <v>110</v>
       </c>
-      <c r="J6" s="259" t="s">
+      <c r="J6" s="328" t="s">
         <v>112</v>
       </c>
-      <c r="K6" s="264" t="s">
+      <c r="K6" s="333" t="s">
         <v>114</v>
       </c>
       <c r="U6" s="6"/>
@@ -7817,31 +8024,31 @@
     <row r="7" spans="1:31" ht="99">
       <c r="A7" s="18"/>
       <c r="B7"/>
-      <c r="C7" s="227" t="s">
+      <c r="C7" s="296" t="s">
         <v>84</v>
       </c>
-      <c r="D7" s="232" t="s">
+      <c r="D7" s="301" t="s">
         <v>96</v>
       </c>
-      <c r="E7" s="236" t="s">
+      <c r="E7" s="305" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="241" t="s">
+      <c r="F7" s="310" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="246" t="s">
+      <c r="G7" s="315" t="s">
         <v>102</v>
       </c>
-      <c r="H7" s="251" t="s">
+      <c r="H7" s="320" t="s">
         <v>103</v>
       </c>
-      <c r="I7" s="256" t="s">
+      <c r="I7" s="325" t="s">
         <v>99</v>
       </c>
-      <c r="J7" s="260" t="s">
+      <c r="J7" s="329" t="s">
         <v>104</v>
       </c>
-      <c r="K7" s="265" t="s">
+      <c r="K7" s="334" t="s">
         <v>105</v>
       </c>
       <c r="U7" s="6"/>

</xml_diff>

<commit_message>
galacticPubs::publish() [2022-04-21 18:17:07]  broke up P1
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -343,7 +343,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="127">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -1039,7 +1039,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="335">
+  <cellXfs count="473">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1359,6 +1359,420 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="1"/>
@@ -5085,42 +5499,42 @@
       <c r="Z2" s="4"/>
     </row>
     <row r="3" spans="1:26" ht="56">
-      <c r="A3" s="266" t="s">
+      <c r="A3" s="404" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="268" t="s">
+      <c r="B3" s="406" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="270" t="s">
+      <c r="C3" s="408" t="s">
         <v>85</v>
       </c>
-      <c r="D3" s="272" t="s">
+      <c r="D3" s="410" t="s">
         <v>86</v>
       </c>
-      <c r="E3" s="274" t="s">
+      <c r="E3" s="412" t="s">
         <v>88</v>
       </c>
-      <c r="F3" s="276" t="s">
+      <c r="F3" s="414" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="56">
-      <c r="A4" s="267" t="s">
+      <c r="A4" s="405" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="269" t="s">
+      <c r="B4" s="407" t="s">
         <v>85</v>
       </c>
-      <c r="C4" s="271" t="s">
+      <c r="C4" s="409" t="s">
         <v>85</v>
       </c>
-      <c r="D4" s="273" t="s">
+      <c r="D4" s="411" t="s">
         <v>87</v>
       </c>
-      <c r="E4" s="275" t="s">
+      <c r="E4" s="413" t="s">
         <v>89</v>
       </c>
-      <c r="F4" s="277" t="s">
+      <c r="F4" s="415" t="s">
         <v>90</v>
       </c>
     </row>
@@ -6271,25 +6685,25 @@
     <row r="3" spans="1:30" ht="140">
       <c r="A3" s="18"/>
       <c r="B3"/>
-      <c r="C3" s="278" t="s">
+      <c r="C3" s="416" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="280" t="s">
+      <c r="D3" s="418" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="282" t="s">
+      <c r="E3" s="420" t="s">
         <v>91</v>
       </c>
-      <c r="F3" s="284" t="s">
+      <c r="F3" s="422" t="s">
         <v>92</v>
       </c>
-      <c r="G3" s="286" t="s">
+      <c r="G3" s="424" t="s">
         <v>93</v>
       </c>
-      <c r="H3" s="288" t="s">
+      <c r="H3" s="426" t="s">
         <v>94</v>
       </c>
-      <c r="I3" s="290" t="s">
+      <c r="I3" s="428" t="s">
         <v>95</v>
       </c>
       <c r="J3"/>
@@ -6297,25 +6711,25 @@
     <row r="4" spans="1:30" ht="126">
       <c r="A4" s="18"/>
       <c r="B4"/>
-      <c r="C4" s="279" t="s">
+      <c r="C4" s="417" t="s">
         <v>84</v>
       </c>
-      <c r="D4" s="281" t="s">
+      <c r="D4" s="419" t="s">
         <v>96</v>
       </c>
-      <c r="E4" s="283" t="s">
+      <c r="E4" s="421" t="s">
         <v>97</v>
       </c>
-      <c r="F4" s="285" t="s">
+      <c r="F4" s="423" t="s">
         <v>98</v>
       </c>
-      <c r="G4" s="287" t="s">
+      <c r="G4" s="425" t="s">
         <v>99</v>
       </c>
-      <c r="H4" s="289" t="s">
+      <c r="H4" s="427" t="s">
         <v>100</v>
       </c>
-      <c r="I4" s="291" t="s">
+      <c r="I4" s="429" t="s">
         <v>101</v>
       </c>
       <c r="J4"/>
@@ -7876,31 +8290,31 @@
     <row r="3" spans="1:31" ht="113">
       <c r="A3" s="18"/>
       <c r="B3"/>
-      <c r="C3" s="292" t="s">
+      <c r="C3" s="430" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="297" t="s">
+      <c r="D3" s="435" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="302" t="s">
+      <c r="E3" s="440" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="306" t="s">
+      <c r="F3" s="444" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="311" t="s">
+      <c r="G3" s="449" t="s">
         <v>106</v>
       </c>
-      <c r="H3" s="316" t="s">
+      <c r="H3" s="454" t="s">
         <v>108</v>
       </c>
-      <c r="I3" s="321" t="s">
+      <c r="I3" s="459" t="s">
         <v>110</v>
       </c>
-      <c r="J3" s="326" t="s">
+      <c r="J3" s="464" t="s">
         <v>111</v>
       </c>
-      <c r="K3" s="330" t="s">
+      <c r="K3" s="468" t="s">
         <v>113</v>
       </c>
       <c r="U3" s="6"/>
@@ -7914,31 +8328,31 @@
     <row r="4" spans="1:31" ht="113">
       <c r="A4" s="18"/>
       <c r="B4"/>
-      <c r="C4" s="293" t="s">
+      <c r="C4" s="431" t="s">
         <v>84</v>
       </c>
-      <c r="D4" s="298" t="s">
+      <c r="D4" s="436" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="303" t="s">
+      <c r="E4" s="441" t="s">
         <v>42</v>
       </c>
-      <c r="F4" s="307" t="s">
+      <c r="F4" s="445" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="312" t="s">
+      <c r="G4" s="450" t="s">
         <v>43</v>
       </c>
-      <c r="H4" s="317" t="s">
+      <c r="H4" s="455" t="s">
         <v>44</v>
       </c>
-      <c r="I4" s="322" t="s">
+      <c r="I4" s="460" t="s">
         <v>41</v>
       </c>
-      <c r="J4" s="327" t="s">
+      <c r="J4" s="465" t="s">
         <v>45</v>
       </c>
-      <c r="K4" s="331" t="s">
+      <c r="K4" s="469" t="s">
         <v>46</v>
       </c>
       <c r="U4" s="6"/>
@@ -7952,27 +8366,27 @@
     <row r="5" spans="1:31" ht="85">
       <c r="A5" s="18"/>
       <c r="B5"/>
-      <c r="C5" s="294" t="s">
+      <c r="C5" s="432" t="s">
         <v>84</v>
       </c>
-      <c r="D5" s="299" t="s">
+      <c r="D5" s="437" t="s">
         <v>35</v>
       </c>
       <c r="E5" s="49"/>
-      <c r="F5" s="308" t="s">
+      <c r="F5" s="446" t="s">
         <v>47</v>
       </c>
-      <c r="G5" s="313" t="s">
+      <c r="G5" s="451" t="s">
         <v>48</v>
       </c>
-      <c r="H5" s="318" t="s">
+      <c r="H5" s="456" t="s">
         <v>49</v>
       </c>
-      <c r="I5" s="323" t="s">
+      <c r="I5" s="461" t="s">
         <v>41</v>
       </c>
       <c r="J5" s="50"/>
-      <c r="K5" s="332" t="s">
+      <c r="K5" s="470" t="s">
         <v>50</v>
       </c>
       <c r="U5" s="6"/>
@@ -7986,31 +8400,31 @@
     <row r="6" spans="1:31" ht="99">
       <c r="A6" s="18"/>
       <c r="B6"/>
-      <c r="C6" s="295" t="s">
+      <c r="C6" s="433" t="s">
         <v>84</v>
       </c>
-      <c r="D6" s="300" t="s">
+      <c r="D6" s="438" t="s">
         <v>96</v>
       </c>
-      <c r="E6" s="304" t="s">
+      <c r="E6" s="442" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="309" t="s">
+      <c r="F6" s="447" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="314" t="s">
+      <c r="G6" s="452" t="s">
         <v>107</v>
       </c>
-      <c r="H6" s="319" t="s">
+      <c r="H6" s="457" t="s">
         <v>109</v>
       </c>
-      <c r="I6" s="324" t="s">
+      <c r="I6" s="462" t="s">
         <v>110</v>
       </c>
-      <c r="J6" s="328" t="s">
+      <c r="J6" s="466" t="s">
         <v>112</v>
       </c>
-      <c r="K6" s="333" t="s">
+      <c r="K6" s="471" t="s">
         <v>114</v>
       </c>
       <c r="U6" s="6"/>
@@ -8024,31 +8438,31 @@
     <row r="7" spans="1:31" ht="99">
       <c r="A7" s="18"/>
       <c r="B7"/>
-      <c r="C7" s="296" t="s">
+      <c r="C7" s="434" t="s">
         <v>84</v>
       </c>
-      <c r="D7" s="301" t="s">
+      <c r="D7" s="439" t="s">
         <v>96</v>
       </c>
-      <c r="E7" s="305" t="s">
+      <c r="E7" s="443" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="310" t="s">
+      <c r="F7" s="448" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="315" t="s">
+      <c r="G7" s="453" t="s">
         <v>102</v>
       </c>
-      <c r="H7" s="320" t="s">
+      <c r="H7" s="458" t="s">
         <v>103</v>
       </c>
-      <c r="I7" s="325" t="s">
+      <c r="I7" s="463" t="s">
         <v>99</v>
       </c>
-      <c r="J7" s="329" t="s">
+      <c r="J7" s="467" t="s">
         <v>104</v>
       </c>
-      <c r="K7" s="334" t="s">
+      <c r="K7" s="472" t="s">
         <v>105</v>
       </c>
       <c r="U7" s="6"/>

</xml_diff>

<commit_message>
galacticPubs::publish() [2022-04-21 19:15:54]  what happens if I make teaching materials be P1 &2?
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Edu/Lessons/guardianFrogs_sci/meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29FA4AF0-46AB-5B45-93D4-30CECEE0548C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5319E6D1-E3A8-F24D-9578-27717D6544CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -358,7 +358,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="129">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -463,9 +463,6 @@
   </si>
   <si>
     <t>namedPresentLink</t>
-  </si>
-  <si>
-    <t>1</t>
   </si>
   <si>
     <t>Classroom Handouts</t>
@@ -633,9 +630,6 @@
     <t>Thu Apr  7 09:58:25 2022</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>Thu Apr  7 16:14:56 2022</t>
   </si>
   <si>
@@ -743,6 +737,15 @@
   <si>
     <t>https://docs.google.com/presentation/d/1iH4-CCvup14kiu6juEt4w8FnQlgyTxHn3oimebkrtEc/present</t>
   </si>
+  <si>
+    <t>Student Worksheet for Parts 1 &amp; 2</t>
+  </si>
+  <si>
+    <t>Teacher Worksheet for Parts 1 &amp; 2</t>
+  </si>
+  <si>
+    <t>1 &amp; 2</t>
+  </si>
 </sst>
 </file>
 
@@ -751,7 +754,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="31">
+  <fonts count="32">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -939,6 +942,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -1071,7 +1080,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="197">
+  <cellXfs count="194">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1363,18 +1372,6 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1392,6 +1389,7 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="1"/>
     </xf>
@@ -1906,13 +1904,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="18" customHeight="1">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="117" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="122"/>
-      <c r="C1" s="122"/>
-      <c r="D1" s="122"/>
-      <c r="E1" s="123"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="119"/>
     </row>
     <row r="2" spans="1:25" ht="18" customHeight="1">
       <c r="A2" s="1" t="s">
@@ -4653,14 +4651,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A1" s="124" t="s">
+      <c r="A1" s="120" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="122"/>
-      <c r="C1" s="122"/>
-      <c r="D1" s="122"/>
-      <c r="E1" s="122"/>
-      <c r="F1" s="123"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="119"/>
     </row>
     <row r="2" spans="1:26" ht="18" customHeight="1">
       <c r="A2" s="5" t="s">
@@ -4703,43 +4701,43 @@
       <c r="Z2" s="4"/>
     </row>
     <row r="3" spans="1:26" ht="56">
-      <c r="A3" s="128" t="s">
+      <c r="A3" s="125" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="130" t="s">
+      <c r="B3" s="127" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="129" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="132" t="s">
+      <c r="D3" s="131" t="s">
         <v>85</v>
       </c>
-      <c r="D3" s="134" t="s">
+      <c r="E3" s="133" t="s">
+        <v>87</v>
+      </c>
+      <c r="F3" s="135" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="56">
+      <c r="A4" s="126" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="128" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="130" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" s="132" t="s">
         <v>86</v>
       </c>
-      <c r="E3" s="136" t="s">
+      <c r="E4" s="134" t="s">
         <v>88</v>
       </c>
-      <c r="F3" s="138" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="56">
-      <c r="A4" s="129" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="131" t="s">
-        <v>85</v>
-      </c>
-      <c r="C4" s="133" t="s">
-        <v>85</v>
-      </c>
-      <c r="D4" s="135" t="s">
-        <v>87</v>
-      </c>
-      <c r="E4" s="137" t="s">
+      <c r="F4" s="136" t="s">
         <v>89</v>
-      </c>
-      <c r="F4" s="139" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="13">
@@ -5800,7 +5798,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I21" sqref="I21"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -5819,19 +5817,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="19.5" customHeight="1">
-      <c r="A1" s="125" t="s">
+      <c r="A1" s="121" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="122"/>
-      <c r="C1" s="122"/>
-      <c r="D1" s="122"/>
-      <c r="E1" s="122"/>
-      <c r="F1" s="122"/>
-      <c r="G1" s="122"/>
-      <c r="H1" s="122"/>
-      <c r="I1" s="122"/>
-      <c r="J1" s="122"/>
-      <c r="K1" s="123"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
+      <c r="I1" s="118"/>
+      <c r="J1" s="118"/>
+      <c r="K1" s="119"/>
       <c r="L1" s="11"/>
       <c r="M1" s="12"/>
       <c r="N1" s="12"/>
@@ -5886,55 +5884,55 @@
       <c r="K2" s="16"/>
       <c r="L2" s="17"/>
     </row>
-    <row r="3" spans="1:30" ht="13">
+    <row r="3" spans="1:30" ht="140">
       <c r="A3" s="18"/>
       <c r="B3"/>
-      <c r="C3" s="140" t="s">
-        <v>84</v>
-      </c>
-      <c r="D3" s="142" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="144" t="s">
+      <c r="C3" s="137" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="139" t="s">
+        <v>128</v>
+      </c>
+      <c r="E3" s="141" t="s">
+        <v>117</v>
+      </c>
+      <c r="F3" s="143" t="s">
         <v>119</v>
       </c>
-      <c r="F3" s="146" t="s">
+      <c r="G3" s="145" t="s">
         <v>121</v>
       </c>
-      <c r="G3" s="148" t="s">
-        <v>123</v>
-      </c>
-      <c r="H3" s="150" t="s">
+      <c r="H3" s="147" t="s">
+        <v>122</v>
+      </c>
+      <c r="I3" s="149" t="s">
         <v>124</v>
       </c>
-      <c r="I3" s="152" t="s">
-        <v>126</v>
-      </c>
       <c r="J3"/>
     </row>
-    <row r="4" spans="1:30" ht="13">
+    <row r="4" spans="1:30" ht="126">
       <c r="A4" s="18"/>
       <c r="B4"/>
-      <c r="C4" s="141" t="s">
-        <v>84</v>
-      </c>
-      <c r="D4" s="143" t="s">
+      <c r="C4" s="138" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="140" t="s">
+        <v>116</v>
+      </c>
+      <c r="E4" s="142" t="s">
         <v>118</v>
       </c>
-      <c r="E4" s="145" t="s">
+      <c r="F4" s="144" t="s">
         <v>120</v>
       </c>
-      <c r="F4" s="147" t="s">
-        <v>122</v>
-      </c>
-      <c r="G4" s="149" t="s">
+      <c r="G4" s="146" t="s">
+        <v>121</v>
+      </c>
+      <c r="H4" s="148" t="s">
         <v>123</v>
       </c>
-      <c r="H4" s="151" t="s">
+      <c r="I4" s="150" t="s">
         <v>125</v>
-      </c>
-      <c r="I4" s="153" t="s">
-        <v>127</v>
       </c>
       <c r="J4"/>
     </row>
@@ -7382,7 +7380,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -7402,19 +7400,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="19.5" customHeight="1">
-      <c r="A1" s="125" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="122"/>
-      <c r="C1" s="122"/>
-      <c r="D1" s="122"/>
-      <c r="E1" s="122"/>
-      <c r="F1" s="122"/>
-      <c r="G1" s="122"/>
-      <c r="H1" s="122"/>
-      <c r="I1" s="122"/>
-      <c r="J1" s="122"/>
-      <c r="K1" s="123"/>
+      <c r="A1" s="121" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
+      <c r="I1" s="118"/>
+      <c r="J1" s="118"/>
+      <c r="K1" s="119"/>
       <c r="L1" s="19"/>
       <c r="M1" s="19"/>
       <c r="N1" s="19"/>
@@ -7450,10 +7448,10 @@
         <v>24</v>
       </c>
       <c r="E2" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="20" t="s">
         <v>37</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>38</v>
       </c>
       <c r="G2" s="13" t="s">
         <v>31</v>
@@ -7468,7 +7466,7 @@
         <v>32</v>
       </c>
       <c r="K2" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L2" s="8"/>
       <c r="M2" s="8"/>
@@ -7494,32 +7492,32 @@
     <row r="3" spans="1:31" ht="113">
       <c r="A3" s="18"/>
       <c r="B3"/>
-      <c r="C3" s="154" t="s">
-        <v>84</v>
-      </c>
-      <c r="D3" s="159" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="164" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" s="168" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="173" t="s">
+      <c r="C3" s="151" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="156" t="s">
+        <v>128</v>
+      </c>
+      <c r="E3" s="161" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="165" t="s">
+        <v>126</v>
+      </c>
+      <c r="G3" s="170" t="s">
+        <v>95</v>
+      </c>
+      <c r="H3" s="175" t="s">
         <v>97</v>
       </c>
-      <c r="H3" s="178" t="s">
+      <c r="I3" s="180" t="s">
         <v>99</v>
       </c>
-      <c r="I3" s="183" t="s">
-        <v>101</v>
-      </c>
-      <c r="J3" s="188" t="s">
+      <c r="J3" s="185" t="s">
+        <v>100</v>
+      </c>
+      <c r="K3" s="189" t="s">
         <v>102</v>
-      </c>
-      <c r="K3" s="192" t="s">
-        <v>104</v>
       </c>
       <c r="U3" s="6"/>
       <c r="V3" s="6"/>
@@ -7532,32 +7530,32 @@
     <row r="4" spans="1:31" ht="113">
       <c r="A4" s="18"/>
       <c r="B4"/>
-      <c r="C4" s="155" t="s">
-        <v>84</v>
-      </c>
-      <c r="D4" s="160" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="165" t="s">
+      <c r="C4" s="152" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="157" t="s">
+        <v>128</v>
+      </c>
+      <c r="E4" s="162" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="166" t="s">
+        <v>127</v>
+      </c>
+      <c r="G4" s="171" t="s">
         <v>42</v>
       </c>
-      <c r="F4" s="169" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="174" t="s">
+      <c r="H4" s="176" t="s">
         <v>43</v>
       </c>
-      <c r="H4" s="179" t="s">
+      <c r="I4" s="181" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" s="186" t="s">
         <v>44</v>
       </c>
-      <c r="I4" s="184" t="s">
-        <v>41</v>
-      </c>
-      <c r="J4" s="189" t="s">
+      <c r="K4" s="190" t="s">
         <v>45</v>
-      </c>
-      <c r="K4" s="193" t="s">
-        <v>46</v>
       </c>
       <c r="U4" s="6"/>
       <c r="V4" s="6"/>
@@ -7570,28 +7568,28 @@
     <row r="5" spans="1:31" ht="85">
       <c r="A5" s="18"/>
       <c r="B5"/>
-      <c r="C5" s="156" t="s">
-        <v>84</v>
-      </c>
-      <c r="D5" s="161" t="s">
-        <v>35</v>
+      <c r="C5" s="153" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" s="158" t="s">
+        <v>128</v>
       </c>
       <c r="E5" s="49"/>
-      <c r="F5" s="170" t="s">
+      <c r="F5" s="167" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="172" t="s">
         <v>47</v>
       </c>
-      <c r="G5" s="175" t="s">
+      <c r="H5" s="177" t="s">
         <v>48</v>
       </c>
-      <c r="H5" s="180" t="s">
+      <c r="I5" s="182" t="s">
+        <v>40</v>
+      </c>
+      <c r="J5" s="50"/>
+      <c r="K5" s="191" t="s">
         <v>49</v>
-      </c>
-      <c r="I5" s="185" t="s">
-        <v>41</v>
-      </c>
-      <c r="J5" s="50"/>
-      <c r="K5" s="194" t="s">
-        <v>50</v>
       </c>
       <c r="U5" s="6"/>
       <c r="V5" s="6"/>
@@ -7604,32 +7602,32 @@
     <row r="6" spans="1:31" ht="99">
       <c r="A6" s="18"/>
       <c r="B6"/>
-      <c r="C6" s="157" t="s">
-        <v>84</v>
-      </c>
-      <c r="D6" s="162" t="s">
-        <v>91</v>
-      </c>
-      <c r="E6" s="166" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" s="171" t="s">
+      <c r="C6" s="154" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" s="159" t="s">
+        <v>116</v>
+      </c>
+      <c r="E6" s="163" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="168" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="176" t="s">
+      <c r="G6" s="173" t="s">
+        <v>96</v>
+      </c>
+      <c r="H6" s="178" t="s">
         <v>98</v>
       </c>
-      <c r="H6" s="181" t="s">
-        <v>100</v>
-      </c>
-      <c r="I6" s="186" t="s">
+      <c r="I6" s="183" t="s">
+        <v>99</v>
+      </c>
+      <c r="J6" s="187" t="s">
         <v>101</v>
       </c>
-      <c r="J6" s="190" t="s">
+      <c r="K6" s="192" t="s">
         <v>103</v>
-      </c>
-      <c r="K6" s="195" t="s">
-        <v>105</v>
       </c>
       <c r="U6" s="6"/>
       <c r="V6" s="6"/>
@@ -7642,32 +7640,32 @@
     <row r="7" spans="1:31" ht="99">
       <c r="A7" s="18"/>
       <c r="B7"/>
-      <c r="C7" s="158" t="s">
-        <v>84</v>
-      </c>
-      <c r="D7" s="163" t="s">
+      <c r="C7" s="155" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="160" t="s">
+        <v>116</v>
+      </c>
+      <c r="E7" s="164" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="169" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="174" t="s">
         <v>91</v>
       </c>
-      <c r="E7" s="167" t="s">
-        <v>42</v>
-      </c>
-      <c r="F7" s="172" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="177" t="s">
+      <c r="H7" s="179" t="s">
+        <v>92</v>
+      </c>
+      <c r="I7" s="184" t="s">
+        <v>90</v>
+      </c>
+      <c r="J7" s="188" t="s">
         <v>93</v>
       </c>
-      <c r="H7" s="182" t="s">
+      <c r="K7" s="193" t="s">
         <v>94</v>
-      </c>
-      <c r="I7" s="187" t="s">
-        <v>92</v>
-      </c>
-      <c r="J7" s="191" t="s">
-        <v>95</v>
-      </c>
-      <c r="K7" s="196" t="s">
-        <v>96</v>
       </c>
       <c r="U7" s="6"/>
       <c r="V7" s="6"/>
@@ -9632,6 +9630,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:K1"/>
   </mergeCells>
+  <phoneticPr fontId="31" type="noConversion"/>
   <conditionalFormatting sqref="F19:F94">
     <cfRule type="expression" dxfId="1" priority="1">
       <formula>IF(AND($F19="",NOT($J19="")),1,0)</formula>
@@ -9681,19 +9680,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="21.75" customHeight="1">
-      <c r="A1" s="126" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" s="122"/>
-      <c r="C1" s="122"/>
-      <c r="D1" s="122"/>
-      <c r="E1" s="122"/>
-      <c r="F1" s="122"/>
-      <c r="G1" s="122"/>
-      <c r="H1" s="122"/>
-      <c r="I1" s="122"/>
-      <c r="J1" s="122"/>
-      <c r="K1" s="123"/>
+      <c r="A1" s="122" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
+      <c r="I1" s="118"/>
+      <c r="J1" s="118"/>
+      <c r="K1" s="119"/>
       <c r="L1" s="22"/>
       <c r="M1" s="22"/>
     </row>
@@ -9723,10 +9722,10 @@
         <v>32</v>
       </c>
       <c r="I2" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="J2" s="24" t="s">
         <v>52</v>
-      </c>
-      <c r="J2" s="24" t="s">
-        <v>53</v>
       </c>
       <c r="K2" s="25" t="s">
         <v>34</v>
@@ -11315,19 +11314,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="18.75" customHeight="1">
-      <c r="A1" s="126" t="s">
-        <v>54</v>
-      </c>
-      <c r="B1" s="122"/>
-      <c r="C1" s="122"/>
-      <c r="D1" s="122"/>
-      <c r="E1" s="122"/>
-      <c r="F1" s="122"/>
-      <c r="G1" s="122"/>
-      <c r="H1" s="122"/>
-      <c r="I1" s="122"/>
-      <c r="J1" s="122"/>
-      <c r="K1" s="123"/>
+      <c r="A1" s="122" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
+      <c r="I1" s="118"/>
+      <c r="J1" s="118"/>
+      <c r="K1" s="119"/>
     </row>
     <row r="2" spans="1:31" ht="18.75" customHeight="1">
       <c r="A2" s="9" t="s">
@@ -11343,10 +11342,10 @@
         <v>24</v>
       </c>
       <c r="E2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>37</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>38</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>31</v>
@@ -11361,7 +11360,7 @@
         <v>32</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L2" s="8"/>
       <c r="M2" s="8"/>
@@ -13651,23 +13650,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="18" customHeight="1">
-      <c r="A1" s="127" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="122"/>
-      <c r="C1" s="122"/>
-      <c r="D1" s="122"/>
-      <c r="E1" s="122"/>
-      <c r="F1" s="122"/>
-      <c r="G1" s="122"/>
-      <c r="H1" s="122"/>
-      <c r="I1" s="122"/>
-      <c r="J1" s="122"/>
-      <c r="K1" s="122"/>
-      <c r="L1" s="122"/>
-      <c r="M1" s="122"/>
-      <c r="N1" s="122"/>
-      <c r="O1" s="123"/>
+      <c r="A1" s="123" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
+      <c r="I1" s="118"/>
+      <c r="J1" s="118"/>
+      <c r="K1" s="118"/>
+      <c r="L1" s="118"/>
+      <c r="M1" s="118"/>
+      <c r="N1" s="118"/>
+      <c r="O1" s="119"/>
     </row>
     <row r="2" spans="1:35" ht="15" customHeight="1">
       <c r="A2" s="8" t="s">
@@ -13677,43 +13676,43 @@
         <v>23</v>
       </c>
       <c r="C2" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="E2" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="E2" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" s="27" t="s">
+      <c r="G2" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="H2" s="27" t="s">
         <v>60</v>
-      </c>
-      <c r="H2" s="27" t="s">
-        <v>61</v>
       </c>
       <c r="I2" s="8" t="s">
         <v>31</v>
       </c>
       <c r="J2" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="K2" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="K2" s="27" t="s">
+      <c r="L2" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="L2" s="27" t="s">
+      <c r="M2" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="M2" s="27" t="s">
+      <c r="N2" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="N2" s="27" t="s">
+      <c r="O2" s="27" t="s">
         <v>66</v>
-      </c>
-      <c r="O2" s="27" t="s">
-        <v>67</v>
       </c>
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
@@ -13738,7 +13737,7 @@
     </row>
     <row r="3" spans="1:35" ht="84">
       <c r="A3" s="28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" s="29"/>
       <c r="C3" s="28">
@@ -13748,22 +13747,22 @@
         <v>1</v>
       </c>
       <c r="E3" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="G3" s="31" t="s">
         <v>69</v>
-      </c>
-      <c r="G3" s="31" t="s">
-        <v>70</v>
       </c>
       <c r="H3" s="31"/>
       <c r="I3" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J3" s="32"/>
       <c r="K3" s="33" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L3" s="32"/>
       <c r="M3" s="32" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N3" s="29"/>
       <c r="O3" s="34"/>
@@ -13771,7 +13770,7 @@
     </row>
     <row r="4" spans="1:35" ht="98">
       <c r="A4" s="28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B4" s="29"/>
       <c r="C4" s="28">
@@ -13781,20 +13780,20 @@
         <v>2</v>
       </c>
       <c r="E4" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="F4" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="F4" s="31" t="s">
+      <c r="G4" s="31" t="s">
         <v>75</v>
-      </c>
-      <c r="G4" s="31" t="s">
-        <v>76</v>
       </c>
       <c r="H4" s="31"/>
       <c r="J4" s="32"/>
       <c r="K4" s="32"/>
       <c r="L4" s="32"/>
       <c r="M4" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N4" s="32"/>
       <c r="O4" s="34"/>
@@ -13802,7 +13801,7 @@
     </row>
     <row r="5" spans="1:35" ht="203" customHeight="1">
       <c r="A5" s="28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B5" s="29"/>
       <c r="C5" s="28">
@@ -13812,24 +13811,24 @@
         <v>2</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F5" s="31" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G5" s="31" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H5" s="31"/>
       <c r="J5" s="32"/>
       <c r="K5" s="51" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L5" s="32" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="M5" s="32" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="N5" s="29"/>
       <c r="O5" s="34"/>
@@ -13837,7 +13836,7 @@
     </row>
     <row r="6" spans="1:35" ht="84">
       <c r="A6" s="28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B6" s="29"/>
       <c r="C6" s="28">
@@ -13847,24 +13846,24 @@
         <v>2</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F6" s="31" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G6" s="31" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H6" s="31"/>
       <c r="J6" s="32"/>
       <c r="K6" s="51" t="s">
+        <v>112</v>
+      </c>
+      <c r="L6" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="M6" s="32" t="s">
         <v>114</v>
-      </c>
-      <c r="L6" s="32" t="s">
-        <v>115</v>
-      </c>
-      <c r="M6" s="32" t="s">
-        <v>116</v>
       </c>
       <c r="N6" s="29"/>
       <c r="O6" s="34"/>
@@ -18531,27 +18530,27 @@
   <sheetData>
     <row r="1" spans="1:1" ht="26.25" customHeight="1">
       <c r="A1" s="41" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="40.5" customHeight="1">
       <c r="A2" s="42" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="40.5" customHeight="1">
       <c r="A3" s="42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="40.5" customHeight="1">
       <c r="A4" s="42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="40.5" customHeight="1">
       <c r="A5" s="42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="22.5" customHeight="1">
@@ -18559,7 +18558,7 @@
     </row>
     <row r="7" spans="1:1" ht="22.5" customHeight="1">
       <c r="A7" s="42" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="22.5" customHeight="1">

</xml_diff>

<commit_message>
galacticPubs::publish() [2022-04-21 23:41:34]  procedure done
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Edu/Lessons/guardianFrogs_sci/meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5319E6D1-E3A8-F24D-9578-27717D6544CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C16C6A57-373C-2F46-A095-F8934998CA06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rsrcSumm" sheetId="1" r:id="rId1"/>
@@ -358,7 +358,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="130">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -385,9 +385,6 @@
   </si>
   <si>
     <t>Presentation</t>
-  </si>
-  <si>
-    <t>x 2 Parts</t>
   </si>
   <si>
     <t>Printed Items</t>
@@ -582,12 +579,6 @@
     <t>Borneo Atmospheric Video</t>
   </si>
   <si>
-    <t>This video sets the ambience for the beginning of Part 2 of our "Guardian Frogs" lesson. It situates students in the geographic location, sights, and sounds, and a sense of mystery regarding the island of Borneo.</t>
-  </si>
-  <si>
-    <t>For Part 2: An atmospheric video plays as students enter the classroom, immediately immersing them in the lesson's sights, sounds, geographic location, and sense of mystery.</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=G7xvfIhL6bU</t>
   </si>
   <si>
@@ -678,9 +669,6 @@
     <t xml:space="preserve">Dr. Johana Goyes-Vallejos discovers that in the smooth guardian frog of Borneo, female frogs call. In frog species, typically male frogs call, while females stay silent. Dr. Johana Goyes-Vallejos shows that in the smooth guardian frog of Borneo (Limnonectes palavanensis) this is not the case and that female frogs call, too, producing spontaneous vocalizations to attract males. Dr. Goyes-Vallejos’ discovery that female frogs call suggests that L. palavanensis exhibits a reversal in calling behavior and possibly a sex-role-reversed mating system, which would be the first ever observed in a frog species. </t>
   </si>
   <si>
-    <t>For Part 2: We show parts of this video to introduce students to Dr. Goyes-Vallejos and her research. They will then analyze some of her data.</t>
-  </si>
-  <si>
     <t>Do Female Frogs Call?</t>
   </si>
   <si>
@@ -691,9 +679,6 @@
   </si>
   <si>
     <t>Calling behavior of male and female Guardian Frogs</t>
-  </si>
-  <si>
-    <t>For Part 2: Background video showing that male and female Guardian Frogs look similar, but have a distinct call.</t>
   </si>
   <si>
     <t>Johana Goyes Vallejos</t>
@@ -745,6 +730,24 @@
   </si>
   <si>
     <t>1 &amp; 2</t>
+  </si>
+  <si>
+    <t>This video sets the ambience for the beginning of Part 3 of our "Guardian Frogs" lesson. It situates students in the geographic location, sights, and sounds, and a sense of mystery regarding the island of Borneo.</t>
+  </si>
+  <si>
+    <t>For Part 3: We show parts of this video to introduce students to Dr. Goyes-Vallejos and her research. They will then analyze some of her data.</t>
+  </si>
+  <si>
+    <t>For Part 3: Background video showing that male and female Guardian Frogs look similar, but have a distinct call.</t>
+  </si>
+  <si>
+    <t>For Part 3: An atmospheric video plays as students enter the classroom, immediately immersing them in the lesson's sights, sounds, geographic location, and sense of mystery.</t>
+  </si>
+  <si>
+    <t>x 2 (for Parts 1&amp;2 and Part 3)</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
@@ -1080,7 +1083,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="194">
+  <cellXfs count="197">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1372,6 +1375,18 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1389,7 +1404,6 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="1"/>
     </xf>
@@ -1890,7 +1904,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -1904,13 +1918,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="18" customHeight="1">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="121" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
-      <c r="E1" s="119"/>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="123"/>
     </row>
     <row r="2" spans="1:25" ht="18" customHeight="1">
       <c r="A2" s="1" t="s">
@@ -1963,7 +1977,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>9</v>
+        <v>128</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
@@ -1977,16 +1991,16 @@
         <v>6</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>10</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>11</v>
       </c>
       <c r="D4" s="5">
         <v>1</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>9</v>
+        <v>128</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -2000,16 +2014,16 @@
         <v>6</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="5">
         <v>1</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>9</v>
+        <v>128</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
@@ -2023,14 +2037,14 @@
         <v>6</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -2044,10 +2058,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>16</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="6"/>
@@ -2063,10 +2077,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="6"/>
@@ -2082,10 +2096,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="6"/>
@@ -2101,10 +2115,10 @@
         <v>6</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="6"/>
@@ -2120,16 +2134,16 @@
         <v>6</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D11" s="5">
         <v>1</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
@@ -4651,33 +4665,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A1" s="120" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
-      <c r="E1" s="118"/>
-      <c r="F1" s="119"/>
+      <c r="A1" s="124" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="123"/>
     </row>
     <row r="2" spans="1:26" ht="18" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="D2" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="E2" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="F2" s="9" t="s">
         <v>26</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>27</v>
       </c>
       <c r="G2" s="9"/>
       <c r="H2" s="9"/>
@@ -4701,43 +4715,43 @@
       <c r="Z2" s="4"/>
     </row>
     <row r="3" spans="1:26" ht="56">
-      <c r="A3" s="125" t="s">
+      <c r="A3" s="128" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="127" t="s">
+      <c r="B3" s="130" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="132" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="134" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" s="136" t="s">
+        <v>84</v>
+      </c>
+      <c r="F3" s="138" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="56">
+      <c r="A4" s="129" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="131" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="133" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="135" t="s">
         <v>83</v>
       </c>
-      <c r="C3" s="129" t="s">
-        <v>84</v>
-      </c>
-      <c r="D3" s="131" t="s">
+      <c r="E4" s="137" t="s">
         <v>85</v>
       </c>
-      <c r="E3" s="133" t="s">
-        <v>87</v>
-      </c>
-      <c r="F3" s="135" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="56">
-      <c r="A4" s="126" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="128" t="s">
-        <v>84</v>
-      </c>
-      <c r="C4" s="130" t="s">
-        <v>84</v>
-      </c>
-      <c r="D4" s="132" t="s">
+      <c r="F4" s="139" t="s">
         <v>86</v>
-      </c>
-      <c r="E4" s="134" t="s">
-        <v>88</v>
-      </c>
-      <c r="F4" s="136" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="13">
@@ -5796,7 +5810,7 @@
   </sheetPr>
   <dimension ref="A1:AD1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
@@ -5817,19 +5831,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="19.5" customHeight="1">
-      <c r="A1" s="121" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
-      <c r="E1" s="118"/>
-      <c r="F1" s="118"/>
-      <c r="G1" s="118"/>
-      <c r="H1" s="118"/>
-      <c r="I1" s="118"/>
-      <c r="J1" s="118"/>
-      <c r="K1" s="119"/>
+      <c r="A1" s="125" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="122"/>
+      <c r="G1" s="122"/>
+      <c r="H1" s="122"/>
+      <c r="I1" s="122"/>
+      <c r="J1" s="122"/>
+      <c r="K1" s="123"/>
       <c r="L1" s="11"/>
       <c r="M1" s="12"/>
       <c r="N1" s="12"/>
@@ -5852,34 +5866,34 @@
     </row>
     <row r="2" spans="1:30" ht="15.75" customHeight="1">
       <c r="A2" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="C2" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="15" t="s">
+      <c r="F2" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" s="13" t="s">
+      <c r="I2" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="J2" s="13" t="s">
         <v>33</v>
-      </c>
-      <c r="J2" s="13" t="s">
-        <v>34</v>
       </c>
       <c r="K2" s="16"/>
       <c r="L2" s="17"/>
@@ -5887,52 +5901,52 @@
     <row r="3" spans="1:30" ht="140">
       <c r="A3" s="18"/>
       <c r="B3"/>
-      <c r="C3" s="137" t="s">
-        <v>83</v>
-      </c>
-      <c r="D3" s="139" t="s">
-        <v>128</v>
-      </c>
-      <c r="E3" s="141" t="s">
+      <c r="C3" s="140" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="142" t="s">
+        <v>123</v>
+      </c>
+      <c r="E3" s="144" t="s">
+        <v>112</v>
+      </c>
+      <c r="F3" s="146" t="s">
+        <v>114</v>
+      </c>
+      <c r="G3" s="148" t="s">
+        <v>116</v>
+      </c>
+      <c r="H3" s="150" t="s">
         <v>117</v>
       </c>
-      <c r="F3" s="143" t="s">
+      <c r="I3" s="152" t="s">
         <v>119</v>
-      </c>
-      <c r="G3" s="145" t="s">
-        <v>121</v>
-      </c>
-      <c r="H3" s="147" t="s">
-        <v>122</v>
-      </c>
-      <c r="I3" s="149" t="s">
-        <v>124</v>
       </c>
       <c r="J3"/>
     </row>
     <row r="4" spans="1:30" ht="126">
       <c r="A4" s="18"/>
       <c r="B4"/>
-      <c r="C4" s="138" t="s">
-        <v>83</v>
-      </c>
-      <c r="D4" s="140" t="s">
+      <c r="C4" s="141" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="143" t="s">
+        <v>111</v>
+      </c>
+      <c r="E4" s="145" t="s">
+        <v>113</v>
+      </c>
+      <c r="F4" s="147" t="s">
+        <v>115</v>
+      </c>
+      <c r="G4" s="149" t="s">
         <v>116</v>
       </c>
-      <c r="E4" s="142" t="s">
+      <c r="H4" s="151" t="s">
         <v>118</v>
       </c>
-      <c r="F4" s="144" t="s">
+      <c r="I4" s="153" t="s">
         <v>120</v>
-      </c>
-      <c r="G4" s="146" t="s">
-        <v>121</v>
-      </c>
-      <c r="H4" s="148" t="s">
-        <v>123</v>
-      </c>
-      <c r="I4" s="150" t="s">
-        <v>125</v>
       </c>
       <c r="J4"/>
     </row>
@@ -7378,9 +7392,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AE995"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3:D5"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -7400,19 +7414,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="19.5" customHeight="1">
-      <c r="A1" s="121" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
-      <c r="E1" s="118"/>
-      <c r="F1" s="118"/>
-      <c r="G1" s="118"/>
-      <c r="H1" s="118"/>
-      <c r="I1" s="118"/>
-      <c r="J1" s="118"/>
-      <c r="K1" s="119"/>
+      <c r="A1" s="125" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="122"/>
+      <c r="G1" s="122"/>
+      <c r="H1" s="122"/>
+      <c r="I1" s="122"/>
+      <c r="J1" s="122"/>
+      <c r="K1" s="123"/>
       <c r="L1" s="19"/>
       <c r="M1" s="19"/>
       <c r="N1" s="19"/>
@@ -7436,37 +7450,37 @@
     </row>
     <row r="2" spans="1:31" ht="18.75" customHeight="1">
       <c r="A2" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="C2" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="20" t="s">
+      <c r="H2" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" s="13" t="s">
         <v>37</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="J2" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="K2" s="13" t="s">
-        <v>38</v>
       </c>
       <c r="L2" s="8"/>
       <c r="M2" s="8"/>
@@ -7492,32 +7506,32 @@
     <row r="3" spans="1:31" ht="113">
       <c r="A3" s="18"/>
       <c r="B3"/>
-      <c r="C3" s="151" t="s">
-        <v>83</v>
-      </c>
-      <c r="D3" s="156" t="s">
-        <v>128</v>
-      </c>
-      <c r="E3" s="161" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="165" t="s">
-        <v>126</v>
-      </c>
-      <c r="G3" s="170" t="s">
-        <v>95</v>
-      </c>
-      <c r="H3" s="175" t="s">
+      <c r="C3" s="154" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="159" t="s">
+        <v>129</v>
+      </c>
+      <c r="E3" s="164" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="168" t="s">
+        <v>121</v>
+      </c>
+      <c r="G3" s="173" t="s">
+        <v>92</v>
+      </c>
+      <c r="H3" s="178" t="s">
+        <v>94</v>
+      </c>
+      <c r="I3" s="183" t="s">
+        <v>96</v>
+      </c>
+      <c r="J3" s="188" t="s">
         <v>97</v>
       </c>
-      <c r="I3" s="180" t="s">
+      <c r="K3" s="192" t="s">
         <v>99</v>
-      </c>
-      <c r="J3" s="185" t="s">
-        <v>100</v>
-      </c>
-      <c r="K3" s="189" t="s">
-        <v>102</v>
       </c>
       <c r="U3" s="6"/>
       <c r="V3" s="6"/>
@@ -7530,32 +7544,32 @@
     <row r="4" spans="1:31" ht="113">
       <c r="A4" s="18"/>
       <c r="B4"/>
-      <c r="C4" s="152" t="s">
-        <v>83</v>
-      </c>
-      <c r="D4" s="157" t="s">
-        <v>128</v>
-      </c>
-      <c r="E4" s="162" t="s">
+      <c r="C4" s="155" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="160" t="s">
+        <v>129</v>
+      </c>
+      <c r="E4" s="165" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="169" t="s">
+        <v>122</v>
+      </c>
+      <c r="G4" s="174" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="166" t="s">
-        <v>127</v>
-      </c>
-      <c r="G4" s="171" t="s">
+      <c r="H4" s="179" t="s">
         <v>42</v>
       </c>
-      <c r="H4" s="176" t="s">
+      <c r="I4" s="184" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" s="189" t="s">
         <v>43</v>
       </c>
-      <c r="I4" s="181" t="s">
-        <v>40</v>
-      </c>
-      <c r="J4" s="186" t="s">
+      <c r="K4" s="193" t="s">
         <v>44</v>
-      </c>
-      <c r="K4" s="190" t="s">
-        <v>45</v>
       </c>
       <c r="U4" s="6"/>
       <c r="V4" s="6"/>
@@ -7568,28 +7582,28 @@
     <row r="5" spans="1:31" ht="85">
       <c r="A5" s="18"/>
       <c r="B5"/>
-      <c r="C5" s="153" t="s">
-        <v>83</v>
-      </c>
-      <c r="D5" s="158" t="s">
-        <v>128</v>
+      <c r="C5" s="156" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="161" t="s">
+        <v>129</v>
       </c>
       <c r="E5" s="49"/>
-      <c r="F5" s="167" t="s">
+      <c r="F5" s="170" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="175" t="s">
         <v>46</v>
       </c>
-      <c r="G5" s="172" t="s">
+      <c r="H5" s="180" t="s">
         <v>47</v>
       </c>
-      <c r="H5" s="177" t="s">
+      <c r="I5" s="185" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="50"/>
+      <c r="K5" s="194" t="s">
         <v>48</v>
-      </c>
-      <c r="I5" s="182" t="s">
-        <v>40</v>
-      </c>
-      <c r="J5" s="50"/>
-      <c r="K5" s="191" t="s">
-        <v>49</v>
       </c>
       <c r="U5" s="6"/>
       <c r="V5" s="6"/>
@@ -7602,32 +7616,32 @@
     <row r="6" spans="1:31" ht="99">
       <c r="A6" s="18"/>
       <c r="B6"/>
-      <c r="C6" s="154" t="s">
-        <v>83</v>
-      </c>
-      <c r="D6" s="159" t="s">
-        <v>116</v>
-      </c>
-      <c r="E6" s="163" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" s="168" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="173" t="s">
+      <c r="C6" s="157" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="162" t="s">
+        <v>111</v>
+      </c>
+      <c r="E6" s="166" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="171" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="176" t="s">
+        <v>93</v>
+      </c>
+      <c r="H6" s="181" t="s">
+        <v>95</v>
+      </c>
+      <c r="I6" s="186" t="s">
         <v>96</v>
       </c>
-      <c r="H6" s="178" t="s">
+      <c r="J6" s="190" t="s">
         <v>98</v>
       </c>
-      <c r="I6" s="183" t="s">
-        <v>99</v>
-      </c>
-      <c r="J6" s="187" t="s">
-        <v>101</v>
-      </c>
-      <c r="K6" s="192" t="s">
-        <v>103</v>
+      <c r="K6" s="195" t="s">
+        <v>100</v>
       </c>
       <c r="U6" s="6"/>
       <c r="V6" s="6"/>
@@ -7640,32 +7654,32 @@
     <row r="7" spans="1:31" ht="99">
       <c r="A7" s="18"/>
       <c r="B7"/>
-      <c r="C7" s="155" t="s">
-        <v>83</v>
-      </c>
-      <c r="D7" s="160" t="s">
-        <v>116</v>
-      </c>
-      <c r="E7" s="164" t="s">
-        <v>41</v>
-      </c>
-      <c r="F7" s="169" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="174" t="s">
+      <c r="C7" s="158" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="163" t="s">
+        <v>111</v>
+      </c>
+      <c r="E7" s="167" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="172" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="177" t="s">
+        <v>88</v>
+      </c>
+      <c r="H7" s="182" t="s">
+        <v>89</v>
+      </c>
+      <c r="I7" s="187" t="s">
+        <v>87</v>
+      </c>
+      <c r="J7" s="191" t="s">
+        <v>90</v>
+      </c>
+      <c r="K7" s="196" t="s">
         <v>91</v>
-      </c>
-      <c r="H7" s="179" t="s">
-        <v>92</v>
-      </c>
-      <c r="I7" s="184" t="s">
-        <v>90</v>
-      </c>
-      <c r="J7" s="188" t="s">
-        <v>93</v>
-      </c>
-      <c r="K7" s="193" t="s">
-        <v>94</v>
       </c>
       <c r="U7" s="6"/>
       <c r="V7" s="6"/>
@@ -9680,55 +9694,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="21.75" customHeight="1">
-      <c r="A1" s="122" t="s">
-        <v>50</v>
-      </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
-      <c r="E1" s="118"/>
-      <c r="F1" s="118"/>
-      <c r="G1" s="118"/>
-      <c r="H1" s="118"/>
-      <c r="I1" s="118"/>
-      <c r="J1" s="118"/>
-      <c r="K1" s="119"/>
+      <c r="A1" s="126" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="122"/>
+      <c r="G1" s="122"/>
+      <c r="H1" s="122"/>
+      <c r="I1" s="122"/>
+      <c r="J1" s="122"/>
+      <c r="K1" s="123"/>
       <c r="L1" s="22"/>
       <c r="M1" s="22"/>
     </row>
     <row r="2" spans="1:31" ht="15.75" customHeight="1">
       <c r="A2" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="C2" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="14" t="s">
+      <c r="F2" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>32</v>
-      </c>
       <c r="I2" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="J2" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="J2" s="24" t="s">
-        <v>52</v>
-      </c>
       <c r="K2" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L2" s="16"/>
       <c r="M2" s="17"/>
@@ -11314,53 +11328,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="18.75" customHeight="1">
-      <c r="A1" s="122" t="s">
-        <v>53</v>
-      </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
-      <c r="E1" s="118"/>
-      <c r="F1" s="118"/>
-      <c r="G1" s="118"/>
-      <c r="H1" s="118"/>
-      <c r="I1" s="118"/>
-      <c r="J1" s="118"/>
-      <c r="K1" s="119"/>
+      <c r="A1" s="126" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="122"/>
+      <c r="G1" s="122"/>
+      <c r="H1" s="122"/>
+      <c r="I1" s="122"/>
+      <c r="J1" s="122"/>
+      <c r="K1" s="123"/>
     </row>
     <row r="2" spans="1:31" ht="18.75" customHeight="1">
       <c r="A2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="C2" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="9" t="s">
+      <c r="H2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>32</v>
-      </c>
       <c r="K2" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L2" s="8"/>
       <c r="M2" s="8"/>
@@ -13631,7 +13645,7 @@
   <dimension ref="A1:AI1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -13650,69 +13664,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="18" customHeight="1">
-      <c r="A1" s="123" t="s">
-        <v>55</v>
-      </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
-      <c r="E1" s="118"/>
-      <c r="F1" s="118"/>
-      <c r="G1" s="118"/>
-      <c r="H1" s="118"/>
-      <c r="I1" s="118"/>
-      <c r="J1" s="118"/>
-      <c r="K1" s="118"/>
-      <c r="L1" s="118"/>
-      <c r="M1" s="118"/>
-      <c r="N1" s="118"/>
-      <c r="O1" s="119"/>
+      <c r="A1" s="127" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="122"/>
+      <c r="G1" s="122"/>
+      <c r="H1" s="122"/>
+      <c r="I1" s="122"/>
+      <c r="J1" s="122"/>
+      <c r="K1" s="122"/>
+      <c r="L1" s="122"/>
+      <c r="M1" s="122"/>
+      <c r="N1" s="122"/>
+      <c r="O1" s="123"/>
     </row>
     <row r="2" spans="1:35" ht="15" customHeight="1">
       <c r="A2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="G2" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="H2" s="27" t="s">
+      <c r="J2" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="I2" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="J2" s="8" t="s">
+      <c r="K2" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="K2" s="27" t="s">
+      <c r="L2" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="L2" s="27" t="s">
+      <c r="M2" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="M2" s="27" t="s">
+      <c r="N2" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="N2" s="27" t="s">
+      <c r="O2" s="27" t="s">
         <v>65</v>
-      </c>
-      <c r="O2" s="27" t="s">
-        <v>66</v>
       </c>
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
@@ -13737,7 +13751,7 @@
     </row>
     <row r="3" spans="1:35" ht="84">
       <c r="A3" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="29"/>
       <c r="C3" s="28">
@@ -13747,22 +13761,22 @@
         <v>1</v>
       </c>
       <c r="E3" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" s="31" t="s">
         <v>68</v>
-      </c>
-      <c r="G3" s="31" t="s">
-        <v>69</v>
       </c>
       <c r="H3" s="31"/>
       <c r="I3" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J3" s="32"/>
       <c r="K3" s="33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L3" s="32"/>
       <c r="M3" s="32" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N3" s="29"/>
       <c r="O3" s="34"/>
@@ -13770,30 +13784,30 @@
     </row>
     <row r="4" spans="1:35" ht="98">
       <c r="A4" s="28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B4" s="29"/>
       <c r="C4" s="28">
         <v>2</v>
       </c>
       <c r="D4" s="30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E4" s="30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F4" s="31" t="s">
-        <v>74</v>
+        <v>124</v>
       </c>
       <c r="G4" s="31" t="s">
-        <v>75</v>
+        <v>127</v>
       </c>
       <c r="H4" s="31"/>
       <c r="J4" s="32"/>
       <c r="K4" s="32"/>
       <c r="L4" s="32"/>
       <c r="M4" s="32" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="N4" s="32"/>
       <c r="O4" s="34"/>
@@ -13801,34 +13815,34 @@
     </row>
     <row r="5" spans="1:35" ht="203" customHeight="1">
       <c r="A5" s="28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B5" s="29"/>
       <c r="C5" s="28">
         <v>3</v>
       </c>
       <c r="D5" s="30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="F5" s="31" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G5" s="31" t="s">
-        <v>106</v>
+        <v>125</v>
       </c>
       <c r="H5" s="31"/>
       <c r="J5" s="32"/>
       <c r="K5" s="51" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="L5" s="32" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="M5" s="32" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="N5" s="29"/>
       <c r="O5" s="34"/>
@@ -13836,34 +13850,34 @@
     </row>
     <row r="6" spans="1:35" ht="84">
       <c r="A6" s="28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B6" s="29"/>
       <c r="C6" s="28">
         <v>4</v>
       </c>
       <c r="D6" s="30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E6" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="F6" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="F6" s="31" t="s">
-        <v>115</v>
-      </c>
       <c r="G6" s="31" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
       <c r="H6" s="31"/>
       <c r="J6" s="32"/>
       <c r="K6" s="51" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="L6" s="32" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="M6" s="32" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="N6" s="29"/>
       <c r="O6" s="34"/>
@@ -18530,27 +18544,27 @@
   <sheetData>
     <row r="1" spans="1:1" ht="26.25" customHeight="1">
       <c r="A1" s="41" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="40.5" customHeight="1">
       <c r="A2" s="42" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="40.5" customHeight="1">
       <c r="A3" s="42" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="40.5" customHeight="1">
       <c r="A4" s="42" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="40.5" customHeight="1">
       <c r="A5" s="42" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="22.5" customHeight="1">
@@ -18558,7 +18572,7 @@
     </row>
     <row r="7" spans="1:1" ht="22.5" customHeight="1">
       <c r="A7" s="42" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="22.5" customHeight="1">

</xml_diff>

<commit_message>
galacticPubs::publish() [2022-04-22 09:55:25]  acknowledgments
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -358,7 +358,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="129">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -1080,7 +1080,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="197">
+  <cellXfs count="473">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1400,6 +1400,834 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="1"/>
@@ -4712,42 +5540,42 @@
       <c r="Z2" s="4"/>
     </row>
     <row r="3" spans="1:26" ht="56">
-      <c r="A3" s="128" t="s">
+      <c r="A3" s="404" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="130" t="s">
+      <c r="B3" s="406" t="s">
         <v>80</v>
       </c>
-      <c r="C3" s="132" t="s">
+      <c r="C3" s="408" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="134" t="s">
+      <c r="D3" s="410" t="s">
         <v>82</v>
       </c>
-      <c r="E3" s="136" t="s">
+      <c r="E3" s="412" t="s">
         <v>84</v>
       </c>
-      <c r="F3" s="138" t="s">
+      <c r="F3" s="414" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="56">
-      <c r="A4" s="129" t="s">
+      <c r="A4" s="405" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="131" t="s">
+      <c r="B4" s="407" t="s">
         <v>81</v>
       </c>
-      <c r="C4" s="133" t="s">
+      <c r="C4" s="409" t="s">
         <v>81</v>
       </c>
-      <c r="D4" s="135" t="s">
+      <c r="D4" s="411" t="s">
         <v>83</v>
       </c>
-      <c r="E4" s="137" t="s">
+      <c r="E4" s="413" t="s">
         <v>85</v>
       </c>
-      <c r="F4" s="139" t="s">
+      <c r="F4" s="415" t="s">
         <v>86</v>
       </c>
     </row>
@@ -5898,25 +6726,25 @@
     <row r="3" spans="1:30" ht="140">
       <c r="A3" s="18"/>
       <c r="B3"/>
-      <c r="C3" s="140" t="s">
+      <c r="C3" s="416" t="s">
         <v>80</v>
       </c>
-      <c r="D3" s="142" t="s">
+      <c r="D3" s="418" t="s">
         <v>128</v>
       </c>
-      <c r="E3" s="144" t="s">
+      <c r="E3" s="420" t="s">
         <v>112</v>
       </c>
-      <c r="F3" s="146" t="s">
+      <c r="F3" s="422" t="s">
         <v>114</v>
       </c>
-      <c r="G3" s="148" t="s">
+      <c r="G3" s="424" t="s">
         <v>116</v>
       </c>
-      <c r="H3" s="150" t="s">
+      <c r="H3" s="426" t="s">
         <v>117</v>
       </c>
-      <c r="I3" s="152" t="s">
+      <c r="I3" s="428" t="s">
         <v>119</v>
       </c>
       <c r="J3"/>
@@ -5924,25 +6752,25 @@
     <row r="4" spans="1:30" ht="126">
       <c r="A4" s="18"/>
       <c r="B4"/>
-      <c r="C4" s="141" t="s">
+      <c r="C4" s="417" t="s">
         <v>80</v>
       </c>
-      <c r="D4" s="143" t="s">
+      <c r="D4" s="419" t="s">
         <v>111</v>
       </c>
-      <c r="E4" s="145" t="s">
+      <c r="E4" s="421" t="s">
         <v>113</v>
       </c>
-      <c r="F4" s="147" t="s">
+      <c r="F4" s="423" t="s">
         <v>115</v>
       </c>
-      <c r="G4" s="149" t="s">
+      <c r="G4" s="425" t="s">
         <v>116</v>
       </c>
-      <c r="H4" s="151" t="s">
+      <c r="H4" s="427" t="s">
         <v>118</v>
       </c>
-      <c r="I4" s="153" t="s">
+      <c r="I4" s="429" t="s">
         <v>120</v>
       </c>
       <c r="J4"/>
@@ -7503,31 +8331,31 @@
     <row r="3" spans="1:31" ht="113">
       <c r="A3" s="18"/>
       <c r="B3"/>
-      <c r="C3" s="154" t="s">
+      <c r="C3" s="430" t="s">
         <v>80</v>
       </c>
-      <c r="D3" s="159" t="s">
+      <c r="D3" s="435" t="s">
         <v>128</v>
       </c>
-      <c r="E3" s="164" t="s">
+      <c r="E3" s="440" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="168" t="s">
+      <c r="F3" s="444" t="s">
         <v>121</v>
       </c>
-      <c r="G3" s="173" t="s">
+      <c r="G3" s="449" t="s">
         <v>92</v>
       </c>
-      <c r="H3" s="178" t="s">
+      <c r="H3" s="454" t="s">
         <v>94</v>
       </c>
-      <c r="I3" s="183" t="s">
+      <c r="I3" s="459" t="s">
         <v>96</v>
       </c>
-      <c r="J3" s="188" t="s">
+      <c r="J3" s="464" t="s">
         <v>97</v>
       </c>
-      <c r="K3" s="192" t="s">
+      <c r="K3" s="468" t="s">
         <v>99</v>
       </c>
       <c r="U3" s="6"/>
@@ -7541,31 +8369,31 @@
     <row r="4" spans="1:31" ht="113">
       <c r="A4" s="18"/>
       <c r="B4"/>
-      <c r="C4" s="155" t="s">
+      <c r="C4" s="431" t="s">
         <v>80</v>
       </c>
-      <c r="D4" s="160" t="s">
+      <c r="D4" s="436" t="s">
         <v>128</v>
       </c>
-      <c r="E4" s="165" t="s">
+      <c r="E4" s="441" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="169" t="s">
+      <c r="F4" s="445" t="s">
         <v>122</v>
       </c>
-      <c r="G4" s="174" t="s">
+      <c r="G4" s="450" t="s">
         <v>41</v>
       </c>
-      <c r="H4" s="179" t="s">
+      <c r="H4" s="455" t="s">
         <v>42</v>
       </c>
-      <c r="I4" s="184" t="s">
+      <c r="I4" s="460" t="s">
         <v>39</v>
       </c>
-      <c r="J4" s="189" t="s">
+      <c r="J4" s="465" t="s">
         <v>43</v>
       </c>
-      <c r="K4" s="193" t="s">
+      <c r="K4" s="469" t="s">
         <v>44</v>
       </c>
       <c r="U4" s="6"/>
@@ -7579,27 +8407,27 @@
     <row r="5" spans="1:31" ht="85">
       <c r="A5" s="18"/>
       <c r="B5"/>
-      <c r="C5" s="156" t="s">
+      <c r="C5" s="432" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="161" t="s">
+      <c r="D5" s="437" t="s">
         <v>128</v>
       </c>
       <c r="E5" s="49"/>
-      <c r="F5" s="170" t="s">
+      <c r="F5" s="446" t="s">
         <v>45</v>
       </c>
-      <c r="G5" s="175" t="s">
+      <c r="G5" s="451" t="s">
         <v>46</v>
       </c>
-      <c r="H5" s="180" t="s">
+      <c r="H5" s="456" t="s">
         <v>47</v>
       </c>
-      <c r="I5" s="185" t="s">
+      <c r="I5" s="461" t="s">
         <v>39</v>
       </c>
       <c r="J5" s="50"/>
-      <c r="K5" s="194" t="s">
+      <c r="K5" s="470" t="s">
         <v>48</v>
       </c>
       <c r="U5" s="6"/>
@@ -7613,31 +8441,31 @@
     <row r="6" spans="1:31" ht="99">
       <c r="A6" s="18"/>
       <c r="B6"/>
-      <c r="C6" s="157" t="s">
+      <c r="C6" s="433" t="s">
         <v>80</v>
       </c>
-      <c r="D6" s="162" t="s">
+      <c r="D6" s="438" t="s">
         <v>111</v>
       </c>
-      <c r="E6" s="166" t="s">
+      <c r="E6" s="442" t="s">
         <v>38</v>
       </c>
-      <c r="F6" s="171" t="s">
+      <c r="F6" s="447" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="176" t="s">
+      <c r="G6" s="452" t="s">
         <v>93</v>
       </c>
-      <c r="H6" s="181" t="s">
+      <c r="H6" s="457" t="s">
         <v>95</v>
       </c>
-      <c r="I6" s="186" t="s">
+      <c r="I6" s="462" t="s">
         <v>96</v>
       </c>
-      <c r="J6" s="190" t="s">
+      <c r="J6" s="466" t="s">
         <v>98</v>
       </c>
-      <c r="K6" s="195" t="s">
+      <c r="K6" s="471" t="s">
         <v>100</v>
       </c>
       <c r="U6" s="6"/>
@@ -7651,31 +8479,31 @@
     <row r="7" spans="1:31" ht="99">
       <c r="A7" s="18"/>
       <c r="B7"/>
-      <c r="C7" s="158" t="s">
+      <c r="C7" s="434" t="s">
         <v>80</v>
       </c>
-      <c r="D7" s="163" t="s">
+      <c r="D7" s="439" t="s">
         <v>111</v>
       </c>
-      <c r="E7" s="167" t="s">
+      <c r="E7" s="443" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="172" t="s">
+      <c r="F7" s="448" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="177" t="s">
+      <c r="G7" s="453" t="s">
         <v>88</v>
       </c>
-      <c r="H7" s="182" t="s">
+      <c r="H7" s="458" t="s">
         <v>89</v>
       </c>
-      <c r="I7" s="187" t="s">
+      <c r="I7" s="463" t="s">
         <v>87</v>
       </c>
-      <c r="J7" s="191" t="s">
+      <c r="J7" s="467" t="s">
         <v>90</v>
       </c>
-      <c r="K7" s="196" t="s">
+      <c r="K7" s="472" t="s">
         <v>91</v>
       </c>
       <c r="U7" s="6"/>

</xml_diff>

<commit_message>
galacticPubs::publish() [2022-06-15 20:03:36]  add locale
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -356,7 +356,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="129">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -1044,7 +1044,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="259">
+  <cellXfs count="328">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1343,6 +1343,213 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="1"/>
@@ -4862,42 +5069,42 @@
       <c r="Z2" s="4"/>
     </row>
     <row r="3" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A3" s="190" t="s">
+      <c r="A3" s="259" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="192" t="s">
+      <c r="B3" s="261" t="s">
         <v>122</v>
       </c>
-      <c r="C3" s="194" t="s">
+      <c r="C3" s="263" t="s">
         <v>123</v>
       </c>
-      <c r="D3" s="196" t="s">
+      <c r="D3" s="265" t="s">
         <v>124</v>
       </c>
-      <c r="E3" s="198" t="s">
+      <c r="E3" s="267" t="s">
         <v>126</v>
       </c>
-      <c r="F3" s="200" t="s">
+      <c r="F3" s="269" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A4" s="191" t="s">
+      <c r="A4" s="260" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="193" t="s">
+      <c r="B4" s="262" t="s">
         <v>123</v>
       </c>
-      <c r="C4" s="195" t="s">
+      <c r="C4" s="264" t="s">
         <v>123</v>
       </c>
-      <c r="D4" s="197" t="s">
+      <c r="D4" s="266" t="s">
         <v>125</v>
       </c>
-      <c r="E4" s="199" t="s">
+      <c r="E4" s="268" t="s">
         <v>127</v>
       </c>
-      <c r="F4" s="201" t="s">
+      <c r="F4" s="270" t="s">
         <v>128</v>
       </c>
     </row>
@@ -6048,25 +6255,25 @@
     <row r="3" spans="1:30" ht="140" x14ac:dyDescent="0.15">
       <c r="A3" s="19"/>
       <c r="B3"/>
-      <c r="C3" s="202" t="s">
+      <c r="C3" s="271" t="s">
         <v>122</v>
       </c>
-      <c r="D3" s="204" t="s">
+      <c r="D3" s="273" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="206" t="s">
+      <c r="E3" s="275" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="208" t="s">
+      <c r="F3" s="277" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="210" t="s">
+      <c r="G3" s="279" t="s">
         <v>38</v>
       </c>
-      <c r="H3" s="212" t="s">
+      <c r="H3" s="281" t="s">
         <v>39</v>
       </c>
-      <c r="I3" s="214" t="s">
+      <c r="I3" s="283" t="s">
         <v>40</v>
       </c>
       <c r="J3"/>
@@ -6074,25 +6281,25 @@
     <row r="4" spans="1:30" ht="126" x14ac:dyDescent="0.15">
       <c r="A4" s="19"/>
       <c r="B4"/>
-      <c r="C4" s="203" t="s">
+      <c r="C4" s="272" t="s">
         <v>122</v>
       </c>
-      <c r="D4" s="205" t="s">
+      <c r="D4" s="274" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="207" t="s">
+      <c r="E4" s="276" t="s">
         <v>42</v>
       </c>
-      <c r="F4" s="209" t="s">
+      <c r="F4" s="278" t="s">
         <v>43</v>
       </c>
-      <c r="G4" s="211" t="s">
+      <c r="G4" s="280" t="s">
         <v>38</v>
       </c>
-      <c r="H4" s="213" t="s">
+      <c r="H4" s="282" t="s">
         <v>44</v>
       </c>
-      <c r="I4" s="215" t="s">
+      <c r="I4" s="284" t="s">
         <v>45</v>
       </c>
       <c r="J4"/>
@@ -7653,31 +7860,31 @@
     <row r="3" spans="1:31" ht="114" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
       <c r="B3"/>
-      <c r="C3" s="216" t="s">
+      <c r="C3" s="285" t="s">
         <v>122</v>
       </c>
-      <c r="D3" s="221" t="s">
+      <c r="D3" s="290" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="226" t="s">
+      <c r="E3" s="295" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="230" t="s">
+      <c r="F3" s="299" t="s">
         <v>51</v>
       </c>
-      <c r="G3" s="235" t="s">
+      <c r="G3" s="304" t="s">
         <v>52</v>
       </c>
-      <c r="H3" s="240" t="s">
+      <c r="H3" s="309" t="s">
         <v>53</v>
       </c>
-      <c r="I3" s="245" t="s">
+      <c r="I3" s="314" t="s">
         <v>54</v>
       </c>
-      <c r="J3" s="250" t="s">
+      <c r="J3" s="319" t="s">
         <v>55</v>
       </c>
-      <c r="K3" s="254" t="s">
+      <c r="K3" s="323" t="s">
         <v>56</v>
       </c>
       <c r="U3" s="6"/>
@@ -7691,31 +7898,31 @@
     <row r="4" spans="1:31" ht="114" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
       <c r="B4"/>
-      <c r="C4" s="217" t="s">
+      <c r="C4" s="286" t="s">
         <v>122</v>
       </c>
-      <c r="D4" s="222" t="s">
+      <c r="D4" s="291" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="227" t="s">
+      <c r="E4" s="296" t="s">
         <v>57</v>
       </c>
-      <c r="F4" s="231" t="s">
+      <c r="F4" s="300" t="s">
         <v>58</v>
       </c>
-      <c r="G4" s="236" t="s">
+      <c r="G4" s="305" t="s">
         <v>59</v>
       </c>
-      <c r="H4" s="241" t="s">
+      <c r="H4" s="310" t="s">
         <v>60</v>
       </c>
-      <c r="I4" s="246" t="s">
+      <c r="I4" s="315" t="s">
         <v>61</v>
       </c>
-      <c r="J4" s="251" t="s">
+      <c r="J4" s="320" t="s">
         <v>62</v>
       </c>
-      <c r="K4" s="255" t="s">
+      <c r="K4" s="324" t="s">
         <v>63</v>
       </c>
       <c r="U4" s="6"/>
@@ -7729,27 +7936,27 @@
     <row r="5" spans="1:31" ht="86" x14ac:dyDescent="0.25">
       <c r="A5" s="19"/>
       <c r="B5"/>
-      <c r="C5" s="218" t="s">
+      <c r="C5" s="287" t="s">
         <v>122</v>
       </c>
-      <c r="D5" s="223" t="s">
+      <c r="D5" s="292" t="s">
         <v>35</v>
       </c>
       <c r="E5" s="11"/>
-      <c r="F5" s="232" t="s">
+      <c r="F5" s="301" t="s">
         <v>64</v>
       </c>
-      <c r="G5" s="237" t="s">
+      <c r="G5" s="306" t="s">
         <v>65</v>
       </c>
-      <c r="H5" s="242" t="s">
+      <c r="H5" s="311" t="s">
         <v>66</v>
       </c>
-      <c r="I5" s="247" t="s">
+      <c r="I5" s="316" t="s">
         <v>61</v>
       </c>
       <c r="J5" s="11"/>
-      <c r="K5" s="256" t="s">
+      <c r="K5" s="325" t="s">
         <v>67</v>
       </c>
       <c r="U5" s="6"/>
@@ -7763,31 +7970,31 @@
     <row r="6" spans="1:31" ht="100" x14ac:dyDescent="0.25">
       <c r="A6" s="19"/>
       <c r="B6"/>
-      <c r="C6" s="219" t="s">
+      <c r="C6" s="288" t="s">
         <v>122</v>
       </c>
-      <c r="D6" s="224" t="s">
+      <c r="D6" s="293" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="228" t="s">
+      <c r="E6" s="297" t="s">
         <v>50</v>
       </c>
-      <c r="F6" s="233" t="s">
+      <c r="F6" s="302" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="238" t="s">
+      <c r="G6" s="307" t="s">
         <v>68</v>
       </c>
-      <c r="H6" s="243" t="s">
+      <c r="H6" s="312" t="s">
         <v>69</v>
       </c>
-      <c r="I6" s="248" t="s">
+      <c r="I6" s="317" t="s">
         <v>54</v>
       </c>
-      <c r="J6" s="252" t="s">
+      <c r="J6" s="321" t="s">
         <v>70</v>
       </c>
-      <c r="K6" s="257" t="s">
+      <c r="K6" s="326" t="s">
         <v>71</v>
       </c>
       <c r="U6" s="6"/>
@@ -7801,31 +8008,31 @@
     <row r="7" spans="1:31" ht="100" x14ac:dyDescent="0.25">
       <c r="A7" s="19"/>
       <c r="B7"/>
-      <c r="C7" s="220" t="s">
+      <c r="C7" s="289" t="s">
         <v>122</v>
       </c>
-      <c r="D7" s="225" t="s">
+      <c r="D7" s="294" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="229" t="s">
+      <c r="E7" s="298" t="s">
         <v>57</v>
       </c>
-      <c r="F7" s="234" t="s">
+      <c r="F7" s="303" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="239" t="s">
+      <c r="G7" s="308" t="s">
         <v>72</v>
       </c>
-      <c r="H7" s="244" t="s">
+      <c r="H7" s="313" t="s">
         <v>73</v>
       </c>
-      <c r="I7" s="249" t="s">
+      <c r="I7" s="318" t="s">
         <v>74</v>
       </c>
-      <c r="J7" s="253" t="s">
+      <c r="J7" s="322" t="s">
         <v>75</v>
       </c>
-      <c r="K7" s="258" t="s">
+      <c r="K7" s="327" t="s">
         <v>76</v>
       </c>
       <c r="U7" s="6"/>

</xml_diff>

<commit_message>
galacticPubs::publish() [2022-06-29 15:33:05]  fix markdown relative link paths
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -356,7 +356,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="142">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -1083,7 +1083,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="458">
+  <cellXfs count="523">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1382,6 +1382,201 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="1"/>
@@ -5498,44 +5693,44 @@
       <c r="Z2" s="4"/>
     </row>
     <row r="3" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A3" s="393" t="s">
+      <c r="A3" s="458" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="395" t="s">
+      <c r="B3" s="460" t="s">
         <v>122</v>
       </c>
-      <c r="C3" s="397" t="s">
+      <c r="C3" s="462" t="s">
         <v>123</v>
       </c>
-      <c r="D3" s="399" t="s">
+      <c r="D3" s="464" t="s">
         <v>124</v>
       </c>
-      <c r="E3" s="401" t="s">
+      <c r="E3" s="466" t="s">
         <v>126</v>
       </c>
       <c r="F3" s="269"/>
-      <c r="G3" t="s" s="403">
+      <c r="G3" t="s" s="468">
         <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A4" s="394" t="s">
+      <c r="A4" s="459" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="396" t="s">
+      <c r="B4" s="461" t="s">
         <v>123</v>
       </c>
-      <c r="C4" s="398" t="s">
+      <c r="C4" s="463" t="s">
         <v>123</v>
       </c>
-      <c r="D4" s="400" t="s">
+      <c r="D4" s="465" t="s">
         <v>125</v>
       </c>
-      <c r="E4" s="402" t="s">
+      <c r="E4" s="467" t="s">
         <v>127</v>
       </c>
       <c r="F4" s="270"/>
-      <c r="G4" t="s" s="404">
+      <c r="G4" t="s" s="469">
         <v>130</v>
       </c>
     </row>
@@ -6686,54 +6881,54 @@
     <row r="3" spans="1:30" ht="140" x14ac:dyDescent="0.15">
       <c r="A3" s="19"/>
       <c r="B3"/>
-      <c r="C3" s="405" t="s">
+      <c r="C3" s="470" t="s">
         <v>122</v>
       </c>
-      <c r="D3" s="407" t="s">
+      <c r="D3" s="472" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="409" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3" s="411" t="s">
+      <c r="E3" s="474" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="476" t="s">
         <v>37</v>
       </c>
       <c r="G3" s="279"/>
-      <c r="H3" s="413" t="s">
+      <c r="H3" s="478" t="s">
         <v>39</v>
       </c>
-      <c r="I3" s="415" t="s">
+      <c r="I3" s="480" t="s">
         <v>40</v>
       </c>
       <c r="J3"/>
-      <c r="K3" t="s" s="417">
+      <c r="K3" t="s" s="482">
         <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:30" ht="126" x14ac:dyDescent="0.15">
       <c r="A4" s="19"/>
       <c r="B4"/>
-      <c r="C4" s="406" t="s">
+      <c r="C4" s="471" t="s">
         <v>122</v>
       </c>
-      <c r="D4" s="408" t="s">
+      <c r="D4" s="473" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="410" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" s="412" t="s">
+      <c r="E4" s="475" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="477" t="s">
         <v>43</v>
       </c>
       <c r="G4" s="280"/>
-      <c r="H4" s="414" t="s">
+      <c r="H4" s="479" t="s">
         <v>44</v>
       </c>
-      <c r="I4" s="416" t="s">
+      <c r="I4" s="481" t="s">
         <v>45</v>
       </c>
       <c r="J4"/>
-      <c r="K4" t="s" s="418">
+      <c r="K4" t="s" s="483">
         <v>132</v>
       </c>
     </row>
@@ -8293,28 +8488,28 @@
     <row r="3" spans="1:31" ht="114" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
       <c r="B3"/>
-      <c r="C3" s="419" t="s">
+      <c r="C3" s="484" t="s">
         <v>122</v>
       </c>
-      <c r="D3" s="424" t="s">
+      <c r="D3" s="489" t="s">
         <v>35</v>
       </c>
       <c r="E3" s="295"/>
-      <c r="F3" s="433" t="s">
+      <c r="F3" s="498" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="434" t="s">
+      <c r="G3" s="499" t="s">
         <v>65</v>
       </c>
-      <c r="H3" s="439" t="s">
+      <c r="H3" s="504" t="s">
         <v>66</v>
       </c>
       <c r="I3" s="314"/>
       <c r="J3" s="319"/>
-      <c r="K3" s="448" t="s">
+      <c r="K3" s="513" t="s">
         <v>67</v>
       </c>
-      <c r="L3" t="s" s="453">
+      <c r="L3" t="s" s="518">
         <v>137</v>
       </c>
       <c r="U3" s="6"/>
@@ -8328,30 +8523,30 @@
     <row r="4" spans="1:31" ht="114" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
       <c r="B4"/>
-      <c r="C4" s="420" t="s">
+      <c r="C4" s="485" t="s">
         <v>122</v>
       </c>
-      <c r="D4" s="425" t="s">
+      <c r="D4" s="490" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="429" t="s">
+      <c r="E4" s="494" t="s">
         <v>50</v>
       </c>
       <c r="F4" s="300"/>
-      <c r="G4" s="435" t="s">
-        <v>134</v>
-      </c>
-      <c r="H4" s="440" t="s">
+      <c r="G4" s="500" t="s">
+        <v>136</v>
+      </c>
+      <c r="H4" s="505" t="s">
         <v>69</v>
       </c>
       <c r="I4" s="315"/>
-      <c r="J4" s="444" t="s">
+      <c r="J4" s="509" t="s">
         <v>70</v>
       </c>
-      <c r="K4" s="449" t="s">
+      <c r="K4" s="514" t="s">
         <v>71</v>
       </c>
-      <c r="L4" t="s" s="454">
+      <c r="L4" t="s" s="519">
         <v>138</v>
       </c>
       <c r="U4" s="6"/>
@@ -8365,30 +8560,30 @@
     <row r="5" spans="1:31" ht="86" x14ac:dyDescent="0.25">
       <c r="A5" s="19"/>
       <c r="B5"/>
-      <c r="C5" s="421" t="s">
+      <c r="C5" s="486" t="s">
         <v>122</v>
       </c>
-      <c r="D5" s="426" t="s">
+      <c r="D5" s="491" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="430" t="s">
+      <c r="E5" s="495" t="s">
         <v>57</v>
       </c>
       <c r="F5" s="301"/>
-      <c r="G5" s="436" t="s">
-        <v>133</v>
-      </c>
-      <c r="H5" s="441" t="s">
+      <c r="G5" s="501" t="s">
+        <v>135</v>
+      </c>
+      <c r="H5" s="506" t="s">
         <v>73</v>
       </c>
       <c r="I5" s="316"/>
-      <c r="J5" s="445" t="s">
+      <c r="J5" s="510" t="s">
         <v>75</v>
       </c>
-      <c r="K5" s="450" t="s">
+      <c r="K5" s="515" t="s">
         <v>76</v>
       </c>
-      <c r="L5" t="s" s="455">
+      <c r="L5" t="s" s="520">
         <v>139</v>
       </c>
       <c r="U5" s="6"/>
@@ -8402,30 +8597,30 @@
     <row r="6" spans="1:31" ht="100" x14ac:dyDescent="0.25">
       <c r="A6" s="19"/>
       <c r="B6"/>
-      <c r="C6" s="422" t="s">
+      <c r="C6" s="487" t="s">
         <v>122</v>
       </c>
-      <c r="D6" s="427" t="s">
+      <c r="D6" s="492" t="s">
         <v>133</v>
       </c>
-      <c r="E6" s="431" t="s">
+      <c r="E6" s="496" t="s">
         <v>50</v>
       </c>
       <c r="F6" s="302"/>
-      <c r="G6" s="437" t="s">
-        <v>135</v>
-      </c>
-      <c r="H6" s="442" t="s">
+      <c r="G6" s="502" t="s">
+        <v>134</v>
+      </c>
+      <c r="H6" s="507" t="s">
         <v>53</v>
       </c>
       <c r="I6" s="317"/>
-      <c r="J6" s="446" t="s">
+      <c r="J6" s="511" t="s">
         <v>55</v>
       </c>
-      <c r="K6" s="451" t="s">
+      <c r="K6" s="516" t="s">
         <v>56</v>
       </c>
-      <c r="L6" t="s" s="456">
+      <c r="L6" t="s" s="521">
         <v>140</v>
       </c>
       <c r="U6" s="6"/>
@@ -8439,30 +8634,30 @@
     <row r="7" spans="1:31" ht="100" x14ac:dyDescent="0.25">
       <c r="A7" s="19"/>
       <c r="B7"/>
-      <c r="C7" s="423" t="s">
+      <c r="C7" s="488" t="s">
         <v>122</v>
       </c>
-      <c r="D7" s="428" t="s">
+      <c r="D7" s="493" t="s">
         <v>134</v>
       </c>
-      <c r="E7" s="432" t="s">
+      <c r="E7" s="497" t="s">
         <v>57</v>
       </c>
       <c r="F7" s="303"/>
-      <c r="G7" s="438" t="s">
-        <v>136</v>
-      </c>
-      <c r="H7" s="443" t="s">
+      <c r="G7" s="503" t="s">
+        <v>133</v>
+      </c>
+      <c r="H7" s="508" t="s">
         <v>60</v>
       </c>
       <c r="I7" s="318"/>
-      <c r="J7" s="447" t="s">
+      <c r="J7" s="512" t="s">
         <v>62</v>
       </c>
-      <c r="K7" s="452" t="s">
+      <c r="K7" s="517" t="s">
         <v>63</v>
       </c>
-      <c r="L7" t="s" s="457">
+      <c r="L7" t="s" s="522">
         <v>141</v>
       </c>
       <c r="U7" s="6"/>

</xml_diff>

<commit_message>
galacticPubs::publish() [2022-06-30 11:50:14]  update QuickPrep for all lessons
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -356,7 +356,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="142">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -1083,7 +1083,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="523">
+  <cellXfs count="913">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1382,6 +1382,1176 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="1"/>
@@ -5693,44 +6863,44 @@
       <c r="Z2" s="4"/>
     </row>
     <row r="3" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A3" s="458" t="s">
+      <c r="A3" s="848" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="460" t="s">
+      <c r="B3" s="850" t="s">
         <v>122</v>
       </c>
-      <c r="C3" s="462" t="s">
+      <c r="C3" s="852" t="s">
         <v>123</v>
       </c>
-      <c r="D3" s="464" t="s">
+      <c r="D3" s="854" t="s">
         <v>124</v>
       </c>
-      <c r="E3" s="466" t="s">
+      <c r="E3" s="856" t="s">
         <v>126</v>
       </c>
       <c r="F3" s="269"/>
-      <c r="G3" t="s" s="468">
+      <c r="G3" t="s" s="858">
         <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A4" s="459" t="s">
+      <c r="A4" s="849" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="461" t="s">
+      <c r="B4" s="851" t="s">
         <v>123</v>
       </c>
-      <c r="C4" s="463" t="s">
+      <c r="C4" s="853" t="s">
         <v>123</v>
       </c>
-      <c r="D4" s="465" t="s">
+      <c r="D4" s="855" t="s">
         <v>125</v>
       </c>
-      <c r="E4" s="467" t="s">
+      <c r="E4" s="857" t="s">
         <v>127</v>
       </c>
       <c r="F4" s="270"/>
-      <c r="G4" t="s" s="469">
+      <c r="G4" t="s" s="859">
         <v>130</v>
       </c>
     </row>
@@ -6881,54 +8051,54 @@
     <row r="3" spans="1:30" ht="140" x14ac:dyDescent="0.15">
       <c r="A3" s="19"/>
       <c r="B3"/>
-      <c r="C3" s="470" t="s">
+      <c r="C3" s="860" t="s">
         <v>122</v>
       </c>
-      <c r="D3" s="472" t="s">
+      <c r="D3" s="862" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="474" t="s">
+      <c r="E3" s="864" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="476" t="s">
+      <c r="F3" s="866" t="s">
         <v>37</v>
       </c>
       <c r="G3" s="279"/>
-      <c r="H3" s="478" t="s">
+      <c r="H3" s="868" t="s">
         <v>39</v>
       </c>
-      <c r="I3" s="480" t="s">
+      <c r="I3" s="870" t="s">
         <v>40</v>
       </c>
       <c r="J3"/>
-      <c r="K3" t="s" s="482">
+      <c r="K3" t="s" s="872">
         <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:30" ht="126" x14ac:dyDescent="0.15">
       <c r="A4" s="19"/>
       <c r="B4"/>
-      <c r="C4" s="471" t="s">
+      <c r="C4" s="861" t="s">
         <v>122</v>
       </c>
-      <c r="D4" s="473" t="s">
+      <c r="D4" s="863" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="475" t="s">
+      <c r="E4" s="865" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="477" t="s">
+      <c r="F4" s="867" t="s">
         <v>43</v>
       </c>
       <c r="G4" s="280"/>
-      <c r="H4" s="479" t="s">
+      <c r="H4" s="869" t="s">
         <v>44</v>
       </c>
-      <c r="I4" s="481" t="s">
+      <c r="I4" s="871" t="s">
         <v>45</v>
       </c>
       <c r="J4"/>
-      <c r="K4" t="s" s="483">
+      <c r="K4" t="s" s="873">
         <v>132</v>
       </c>
     </row>
@@ -8488,28 +9658,28 @@
     <row r="3" spans="1:31" ht="114" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
       <c r="B3"/>
-      <c r="C3" s="484" t="s">
+      <c r="C3" s="874" t="s">
         <v>122</v>
       </c>
-      <c r="D3" s="489" t="s">
+      <c r="D3" s="879" t="s">
         <v>35</v>
       </c>
       <c r="E3" s="295"/>
-      <c r="F3" s="498" t="s">
+      <c r="F3" s="888" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="499" t="s">
+      <c r="G3" s="889" t="s">
         <v>65</v>
       </c>
-      <c r="H3" s="504" t="s">
+      <c r="H3" s="894" t="s">
         <v>66</v>
       </c>
       <c r="I3" s="314"/>
       <c r="J3" s="319"/>
-      <c r="K3" s="513" t="s">
+      <c r="K3" s="903" t="s">
         <v>67</v>
       </c>
-      <c r="L3" t="s" s="518">
+      <c r="L3" t="s" s="908">
         <v>137</v>
       </c>
       <c r="U3" s="6"/>
@@ -8523,30 +9693,30 @@
     <row r="4" spans="1:31" ht="114" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
       <c r="B4"/>
-      <c r="C4" s="485" t="s">
+      <c r="C4" s="875" t="s">
         <v>122</v>
       </c>
-      <c r="D4" s="490" t="s">
+      <c r="D4" s="880" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="494" t="s">
+      <c r="E4" s="884" t="s">
         <v>50</v>
       </c>
       <c r="F4" s="300"/>
-      <c r="G4" s="500" t="s">
-        <v>136</v>
+      <c r="G4" s="890" t="s">
+        <v>135</v>
       </c>
-      <c r="H4" s="505" t="s">
+      <c r="H4" s="895" t="s">
         <v>69</v>
       </c>
       <c r="I4" s="315"/>
-      <c r="J4" s="509" t="s">
+      <c r="J4" s="899" t="s">
         <v>70</v>
       </c>
-      <c r="K4" s="514" t="s">
+      <c r="K4" s="904" t="s">
         <v>71</v>
       </c>
-      <c r="L4" t="s" s="519">
+      <c r="L4" t="s" s="909">
         <v>138</v>
       </c>
       <c r="U4" s="6"/>
@@ -8560,30 +9730,30 @@
     <row r="5" spans="1:31" ht="86" x14ac:dyDescent="0.25">
       <c r="A5" s="19"/>
       <c r="B5"/>
-      <c r="C5" s="486" t="s">
+      <c r="C5" s="876" t="s">
         <v>122</v>
       </c>
-      <c r="D5" s="491" t="s">
+      <c r="D5" s="881" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="495" t="s">
+      <c r="E5" s="885" t="s">
         <v>57</v>
       </c>
       <c r="F5" s="301"/>
-      <c r="G5" s="501" t="s">
-        <v>135</v>
+      <c r="G5" s="891" t="s">
+        <v>136</v>
       </c>
-      <c r="H5" s="506" t="s">
+      <c r="H5" s="896" t="s">
         <v>73</v>
       </c>
       <c r="I5" s="316"/>
-      <c r="J5" s="510" t="s">
+      <c r="J5" s="900" t="s">
         <v>75</v>
       </c>
-      <c r="K5" s="515" t="s">
+      <c r="K5" s="905" t="s">
         <v>76</v>
       </c>
-      <c r="L5" t="s" s="520">
+      <c r="L5" t="s" s="910">
         <v>139</v>
       </c>
       <c r="U5" s="6"/>
@@ -8597,30 +9767,30 @@
     <row r="6" spans="1:31" ht="100" x14ac:dyDescent="0.25">
       <c r="A6" s="19"/>
       <c r="B6"/>
-      <c r="C6" s="487" t="s">
+      <c r="C6" s="877" t="s">
         <v>122</v>
       </c>
-      <c r="D6" s="492" t="s">
+      <c r="D6" s="882" t="s">
         <v>133</v>
       </c>
-      <c r="E6" s="496" t="s">
+      <c r="E6" s="886" t="s">
         <v>50</v>
       </c>
       <c r="F6" s="302"/>
-      <c r="G6" s="502" t="s">
-        <v>134</v>
+      <c r="G6" s="892" t="s">
+        <v>133</v>
       </c>
-      <c r="H6" s="507" t="s">
+      <c r="H6" s="897" t="s">
         <v>53</v>
       </c>
       <c r="I6" s="317"/>
-      <c r="J6" s="511" t="s">
+      <c r="J6" s="901" t="s">
         <v>55</v>
       </c>
-      <c r="K6" s="516" t="s">
+      <c r="K6" s="906" t="s">
         <v>56</v>
       </c>
-      <c r="L6" t="s" s="521">
+      <c r="L6" t="s" s="911">
         <v>140</v>
       </c>
       <c r="U6" s="6"/>
@@ -8634,30 +9804,30 @@
     <row r="7" spans="1:31" ht="100" x14ac:dyDescent="0.25">
       <c r="A7" s="19"/>
       <c r="B7"/>
-      <c r="C7" s="488" t="s">
+      <c r="C7" s="878" t="s">
         <v>122</v>
       </c>
-      <c r="D7" s="493" t="s">
+      <c r="D7" s="883" t="s">
         <v>134</v>
       </c>
-      <c r="E7" s="497" t="s">
+      <c r="E7" s="887" t="s">
         <v>57</v>
       </c>
       <c r="F7" s="303"/>
-      <c r="G7" s="503" t="s">
-        <v>133</v>
+      <c r="G7" s="893" t="s">
+        <v>134</v>
       </c>
-      <c r="H7" s="508" t="s">
+      <c r="H7" s="898" t="s">
         <v>60</v>
       </c>
       <c r="I7" s="318"/>
-      <c r="J7" s="512" t="s">
+      <c r="J7" s="902" t="s">
         <v>62</v>
       </c>
-      <c r="K7" s="517" t="s">
+      <c r="K7" s="907" t="s">
         <v>63</v>
       </c>
-      <c r="L7" t="s" s="522">
+      <c r="L7" t="s" s="912">
         <v>141</v>
       </c>
       <c r="U7" s="6"/>

</xml_diff>

<commit_message>
galacticPubs::publish() [2022-07-15 23:24:10]  All projects rebuilt with DefaultLocale
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -356,7 +356,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1183" uniqueCount="142">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -1083,7 +1083,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="913">
+  <cellXfs count="1108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1382,6 +1382,591 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="1"/>
@@ -6863,44 +7448,44 @@
       <c r="Z2" s="4"/>
     </row>
     <row r="3" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A3" s="848" t="s">
+      <c r="A3" s="1043" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="850" t="s">
+      <c r="B3" s="1045" t="s">
         <v>122</v>
       </c>
-      <c r="C3" s="852" t="s">
+      <c r="C3" s="1047" t="s">
         <v>123</v>
       </c>
-      <c r="D3" s="854" t="s">
+      <c r="D3" s="1049" t="s">
         <v>124</v>
       </c>
-      <c r="E3" s="856" t="s">
+      <c r="E3" s="1051" t="s">
         <v>126</v>
       </c>
       <c r="F3" s="269"/>
-      <c r="G3" t="s" s="858">
+      <c r="G3" t="s" s="1053">
         <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A4" s="849" t="s">
+      <c r="A4" s="1044" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="851" t="s">
+      <c r="B4" s="1046" t="s">
         <v>123</v>
       </c>
-      <c r="C4" s="853" t="s">
+      <c r="C4" s="1048" t="s">
         <v>123</v>
       </c>
-      <c r="D4" s="855" t="s">
+      <c r="D4" s="1050" t="s">
         <v>125</v>
       </c>
-      <c r="E4" s="857" t="s">
+      <c r="E4" s="1052" t="s">
         <v>127</v>
       </c>
       <c r="F4" s="270"/>
-      <c r="G4" t="s" s="859">
+      <c r="G4" t="s" s="1054">
         <v>130</v>
       </c>
     </row>
@@ -8051,54 +8636,54 @@
     <row r="3" spans="1:30" ht="140" x14ac:dyDescent="0.15">
       <c r="A3" s="19"/>
       <c r="B3"/>
-      <c r="C3" s="860" t="s">
+      <c r="C3" s="1055" t="s">
         <v>122</v>
       </c>
-      <c r="D3" s="862" t="s">
+      <c r="D3" s="1057" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="864" t="s">
-        <v>42</v>
+      <c r="E3" s="1059" t="s">
+        <v>36</v>
       </c>
-      <c r="F3" s="866" t="s">
+      <c r="F3" s="1061" t="s">
         <v>37</v>
       </c>
       <c r="G3" s="279"/>
-      <c r="H3" s="868" t="s">
+      <c r="H3" s="1063" t="s">
         <v>39</v>
       </c>
-      <c r="I3" s="870" t="s">
+      <c r="I3" s="1065" t="s">
         <v>40</v>
       </c>
       <c r="J3"/>
-      <c r="K3" t="s" s="872">
+      <c r="K3" t="s" s="1067">
         <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:30" ht="126" x14ac:dyDescent="0.15">
       <c r="A4" s="19"/>
       <c r="B4"/>
-      <c r="C4" s="861" t="s">
+      <c r="C4" s="1056" t="s">
         <v>122</v>
       </c>
-      <c r="D4" s="863" t="s">
+      <c r="D4" s="1058" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="865" t="s">
-        <v>36</v>
+      <c r="E4" s="1060" t="s">
+        <v>42</v>
       </c>
-      <c r="F4" s="867" t="s">
+      <c r="F4" s="1062" t="s">
         <v>43</v>
       </c>
       <c r="G4" s="280"/>
-      <c r="H4" s="869" t="s">
+      <c r="H4" s="1064" t="s">
         <v>44</v>
       </c>
-      <c r="I4" s="871" t="s">
+      <c r="I4" s="1066" t="s">
         <v>45</v>
       </c>
       <c r="J4"/>
-      <c r="K4" t="s" s="873">
+      <c r="K4" t="s" s="1068">
         <v>132</v>
       </c>
     </row>
@@ -9658,28 +10243,28 @@
     <row r="3" spans="1:31" ht="114" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
       <c r="B3"/>
-      <c r="C3" s="874" t="s">
+      <c r="C3" s="1069" t="s">
         <v>122</v>
       </c>
-      <c r="D3" s="879" t="s">
+      <c r="D3" s="1074" t="s">
         <v>35</v>
       </c>
       <c r="E3" s="295"/>
-      <c r="F3" s="888" t="s">
+      <c r="F3" s="1083" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="889" t="s">
+      <c r="G3" s="1084" t="s">
         <v>65</v>
       </c>
-      <c r="H3" s="894" t="s">
+      <c r="H3" s="1089" t="s">
         <v>66</v>
       </c>
       <c r="I3" s="314"/>
       <c r="J3" s="319"/>
-      <c r="K3" s="903" t="s">
+      <c r="K3" s="1098" t="s">
         <v>67</v>
       </c>
-      <c r="L3" t="s" s="908">
+      <c r="L3" t="s" s="1103">
         <v>137</v>
       </c>
       <c r="U3" s="6"/>
@@ -9693,30 +10278,30 @@
     <row r="4" spans="1:31" ht="114" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
       <c r="B4"/>
-      <c r="C4" s="875" t="s">
+      <c r="C4" s="1070" t="s">
         <v>122</v>
       </c>
-      <c r="D4" s="880" t="s">
+      <c r="D4" s="1075" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="884" t="s">
+      <c r="E4" s="1079" t="s">
         <v>50</v>
       </c>
       <c r="F4" s="300"/>
-      <c r="G4" s="890" t="s">
-        <v>135</v>
+      <c r="G4" s="1085" t="s">
+        <v>133</v>
       </c>
-      <c r="H4" s="895" t="s">
+      <c r="H4" s="1090" t="s">
         <v>69</v>
       </c>
       <c r="I4" s="315"/>
-      <c r="J4" s="899" t="s">
+      <c r="J4" s="1094" t="s">
         <v>70</v>
       </c>
-      <c r="K4" s="904" t="s">
+      <c r="K4" s="1099" t="s">
         <v>71</v>
       </c>
-      <c r="L4" t="s" s="909">
+      <c r="L4" t="s" s="1104">
         <v>138</v>
       </c>
       <c r="U4" s="6"/>
@@ -9730,30 +10315,30 @@
     <row r="5" spans="1:31" ht="86" x14ac:dyDescent="0.25">
       <c r="A5" s="19"/>
       <c r="B5"/>
-      <c r="C5" s="876" t="s">
+      <c r="C5" s="1071" t="s">
         <v>122</v>
       </c>
-      <c r="D5" s="881" t="s">
+      <c r="D5" s="1076" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="885" t="s">
+      <c r="E5" s="1080" t="s">
         <v>57</v>
       </c>
       <c r="F5" s="301"/>
-      <c r="G5" s="891" t="s">
-        <v>136</v>
+      <c r="G5" s="1086" t="s">
+        <v>134</v>
       </c>
-      <c r="H5" s="896" t="s">
+      <c r="H5" s="1091" t="s">
         <v>73</v>
       </c>
       <c r="I5" s="316"/>
-      <c r="J5" s="900" t="s">
+      <c r="J5" s="1095" t="s">
         <v>75</v>
       </c>
-      <c r="K5" s="905" t="s">
+      <c r="K5" s="1100" t="s">
         <v>76</v>
       </c>
-      <c r="L5" t="s" s="910">
+      <c r="L5" t="s" s="1105">
         <v>139</v>
       </c>
       <c r="U5" s="6"/>
@@ -9767,30 +10352,30 @@
     <row r="6" spans="1:31" ht="100" x14ac:dyDescent="0.25">
       <c r="A6" s="19"/>
       <c r="B6"/>
-      <c r="C6" s="877" t="s">
+      <c r="C6" s="1072" t="s">
         <v>122</v>
       </c>
-      <c r="D6" s="882" t="s">
+      <c r="D6" s="1077" t="s">
         <v>133</v>
       </c>
-      <c r="E6" s="886" t="s">
+      <c r="E6" s="1081" t="s">
         <v>50</v>
       </c>
       <c r="F6" s="302"/>
-      <c r="G6" s="892" t="s">
-        <v>133</v>
+      <c r="G6" s="1087" t="s">
+        <v>136</v>
       </c>
-      <c r="H6" s="897" t="s">
+      <c r="H6" s="1092" t="s">
         <v>53</v>
       </c>
       <c r="I6" s="317"/>
-      <c r="J6" s="901" t="s">
+      <c r="J6" s="1096" t="s">
         <v>55</v>
       </c>
-      <c r="K6" s="906" t="s">
+      <c r="K6" s="1101" t="s">
         <v>56</v>
       </c>
-      <c r="L6" t="s" s="911">
+      <c r="L6" t="s" s="1106">
         <v>140</v>
       </c>
       <c r="U6" s="6"/>
@@ -9804,30 +10389,30 @@
     <row r="7" spans="1:31" ht="100" x14ac:dyDescent="0.25">
       <c r="A7" s="19"/>
       <c r="B7"/>
-      <c r="C7" s="878" t="s">
+      <c r="C7" s="1073" t="s">
         <v>122</v>
       </c>
-      <c r="D7" s="883" t="s">
+      <c r="D7" s="1078" t="s">
         <v>134</v>
       </c>
-      <c r="E7" s="887" t="s">
+      <c r="E7" s="1082" t="s">
         <v>57</v>
       </c>
       <c r="F7" s="303"/>
-      <c r="G7" s="893" t="s">
-        <v>134</v>
+      <c r="G7" s="1088" t="s">
+        <v>135</v>
       </c>
-      <c r="H7" s="898" t="s">
+      <c r="H7" s="1093" t="s">
         <v>60</v>
       </c>
       <c r="I7" s="318"/>
-      <c r="J7" s="902" t="s">
+      <c r="J7" s="1097" t="s">
         <v>62</v>
       </c>
-      <c r="K7" s="907" t="s">
+      <c r="K7" s="1102" t="s">
         <v>63</v>
       </c>
-      <c r="L7" t="s" s="912">
+      <c r="L7" t="s" s="1107">
         <v>141</v>
       </c>
       <c r="U7" s="6"/>

</xml_diff>

<commit_message>
galacticPubs::publish() [2022-07-19 15:21:26]  fix epaulette
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -356,7 +356,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="140">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -1077,7 +1077,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="402">
+  <cellXfs count="471">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1409,6 +1409,213 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="1"/>
@@ -5324,44 +5531,44 @@
       <c r="Z2" s="4"/>
     </row>
     <row r="3" spans="1:26" ht="56" x14ac:dyDescent="0.15">
-      <c r="A3" s="332" t="s">
+      <c r="A3" s="402" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="334" t="s">
+      <c r="B3" s="404" t="s">
         <v>98</v>
       </c>
-      <c r="C3" s="336" t="s">
+      <c r="C3" s="406" t="s">
         <v>99</v>
       </c>
-      <c r="D3" s="338" t="s">
+      <c r="D3" s="408" t="s">
         <v>100</v>
       </c>
-      <c r="E3" s="340" t="s">
+      <c r="E3" s="410" t="s">
         <v>102</v>
       </c>
       <c r="F3" s="46"/>
-      <c r="G3" s="342" t="s">
+      <c r="G3" s="412" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="56" x14ac:dyDescent="0.15">
-      <c r="A4" s="333" t="s">
+      <c r="A4" s="403" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="335" t="s">
+      <c r="B4" s="405" t="s">
         <v>99</v>
       </c>
-      <c r="C4" s="337" t="s">
+      <c r="C4" s="407" t="s">
         <v>99</v>
       </c>
-      <c r="D4" s="339" t="s">
+      <c r="D4" s="409" t="s">
         <v>101</v>
       </c>
-      <c r="E4" s="341" t="s">
+      <c r="E4" s="411" t="s">
         <v>103</v>
       </c>
       <c r="F4" s="47"/>
-      <c r="G4" s="343" t="s">
+      <c r="G4" s="413" t="s">
         <v>105</v>
       </c>
     </row>
@@ -6512,54 +6719,54 @@
     <row r="3" spans="1:30" ht="140" x14ac:dyDescent="0.15">
       <c r="A3" s="19"/>
       <c r="B3"/>
-      <c r="C3" s="344" t="s">
+      <c r="C3" s="414" t="s">
         <v>98</v>
       </c>
-      <c r="D3" s="346" t="s">
+      <c r="D3" s="416" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="348" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3" s="350" t="s">
+      <c r="E3" s="418" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="420" t="s">
         <v>37</v>
       </c>
       <c r="G3" s="48"/>
-      <c r="H3" s="352" t="s">
+      <c r="H3" s="422" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="354" t="s">
+      <c r="I3" s="424" t="s">
         <v>39</v>
       </c>
       <c r="J3"/>
-      <c r="K3" s="356" t="s">
+      <c r="K3" s="426" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:30" ht="126" x14ac:dyDescent="0.15">
       <c r="A4" s="19"/>
       <c r="B4"/>
-      <c r="C4" s="345" t="s">
+      <c r="C4" s="415" t="s">
         <v>98</v>
       </c>
-      <c r="D4" s="347" t="s">
+      <c r="D4" s="417" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="349" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" s="351" t="s">
+      <c r="E4" s="419" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="421" t="s">
         <v>42</v>
       </c>
       <c r="G4" s="49"/>
-      <c r="H4" s="353" t="s">
+      <c r="H4" s="423" t="s">
         <v>43</v>
       </c>
-      <c r="I4" s="355" t="s">
+      <c r="I4" s="425" t="s">
         <v>44</v>
       </c>
       <c r="J4"/>
-      <c r="K4" s="357" t="s">
+      <c r="K4" s="427" t="s">
         <v>107</v>
       </c>
     </row>
@@ -8119,33 +8326,29 @@
     <row r="3" spans="1:31" ht="86" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
       <c r="B3"/>
-      <c r="C3" s="358" t="s">
+      <c r="C3" s="428" t="s">
         <v>98</v>
       </c>
-      <c r="D3" s="363" t="s">
+      <c r="D3" s="433" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="368" t="s">
-        <v>111</v>
-      </c>
-      <c r="F3" s="372" t="s">
-        <v>131</v>
-      </c>
-      <c r="G3" s="377" t="s">
-        <v>109</v>
-      </c>
-      <c r="H3" s="382" t="s">
-        <v>117</v>
+      <c r="E3" s="368"/>
+      <c r="F3" s="442" t="s">
+        <v>133</v>
+      </c>
+      <c r="G3" s="447" t="s">
+        <v>113</v>
+      </c>
+      <c r="H3" s="452" t="s">
+        <v>51</v>
       </c>
       <c r="I3" s="55"/>
-      <c r="J3" s="387" t="s">
-        <v>136</v>
-      </c>
-      <c r="K3" s="392" t="s">
-        <v>125</v>
-      </c>
-      <c r="L3" s="397" t="s">
-        <v>129</v>
+      <c r="J3" s="387"/>
+      <c r="K3" s="461" t="s">
+        <v>52</v>
+      </c>
+      <c r="L3" s="466" t="s">
+        <v>108</v>
       </c>
       <c r="U3" s="6"/>
       <c r="V3" s="6"/>
@@ -8158,33 +8361,33 @@
     <row r="4" spans="1:31" ht="100" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
       <c r="B4"/>
-      <c r="C4" s="359" t="s">
+      <c r="C4" s="429" t="s">
         <v>98</v>
       </c>
-      <c r="D4" s="364" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="369" t="s">
-        <v>112</v>
-      </c>
-      <c r="F4" s="373" t="s">
-        <v>132</v>
-      </c>
-      <c r="G4" s="378" t="s">
-        <v>110</v>
-      </c>
-      <c r="H4" s="383" t="s">
-        <v>118</v>
+      <c r="D4" s="434" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="438" t="s">
+        <v>111</v>
+      </c>
+      <c r="F4" s="443" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" s="448" t="s">
+        <v>50</v>
+      </c>
+      <c r="H4" s="453" t="s">
+        <v>115</v>
       </c>
       <c r="I4" s="56"/>
-      <c r="J4" s="388" t="s">
-        <v>137</v>
-      </c>
-      <c r="K4" s="393" t="s">
-        <v>126</v>
-      </c>
-      <c r="L4" s="398" t="s">
-        <v>130</v>
+      <c r="J4" s="457" t="s">
+        <v>119</v>
+      </c>
+      <c r="K4" s="462" t="s">
+        <v>123</v>
+      </c>
+      <c r="L4" s="467" t="s">
+        <v>127</v>
       </c>
       <c r="U4" s="6"/>
       <c r="V4" s="6"/>
@@ -8197,31 +8400,33 @@
     <row r="5" spans="1:31" ht="100" x14ac:dyDescent="0.25">
       <c r="A5" s="19"/>
       <c r="B5"/>
-      <c r="C5" s="360" t="s">
+      <c r="C5" s="430" t="s">
         <v>98</v>
       </c>
-      <c r="D5" s="365" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="169"/>
-      <c r="F5" s="374" t="s">
-        <v>49</v>
-      </c>
-      <c r="G5" s="379" t="s">
-        <v>50</v>
-      </c>
-      <c r="H5" s="384" t="s">
-        <v>51</v>
+      <c r="D5" s="435" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="439" t="s">
+        <v>112</v>
+      </c>
+      <c r="F5" s="444" t="s">
+        <v>132</v>
+      </c>
+      <c r="G5" s="449" t="s">
+        <v>110</v>
+      </c>
+      <c r="H5" s="454" t="s">
+        <v>116</v>
       </c>
       <c r="I5" s="57"/>
-      <c r="J5" s="389" t="s">
-        <v>52</v>
-      </c>
-      <c r="K5" s="394" t="s">
-        <v>52</v>
-      </c>
-      <c r="L5" s="399" t="s">
-        <v>108</v>
+      <c r="J5" s="458" t="s">
+        <v>120</v>
+      </c>
+      <c r="K5" s="463" t="s">
+        <v>124</v>
+      </c>
+      <c r="L5" s="468" t="s">
+        <v>128</v>
       </c>
       <c r="U5" s="6"/>
       <c r="V5" s="6"/>
@@ -8234,33 +8439,33 @@
     <row r="6" spans="1:31" ht="114" x14ac:dyDescent="0.25">
       <c r="A6" s="19"/>
       <c r="B6"/>
-      <c r="C6" s="361" t="s">
+      <c r="C6" s="431" t="s">
         <v>98</v>
       </c>
-      <c r="D6" s="366" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" s="370" t="s">
+      <c r="D6" s="436" t="s">
+        <v>109</v>
+      </c>
+      <c r="E6" s="440" t="s">
         <v>111</v>
       </c>
-      <c r="F6" s="375" t="s">
-        <v>133</v>
-      </c>
-      <c r="G6" s="380" t="s">
-        <v>113</v>
-      </c>
-      <c r="H6" s="385" t="s">
-        <v>115</v>
+      <c r="F6" s="445" t="s">
+        <v>134</v>
+      </c>
+      <c r="G6" s="450" t="s">
+        <v>114</v>
+      </c>
+      <c r="H6" s="455" t="s">
+        <v>117</v>
       </c>
       <c r="I6" s="58"/>
-      <c r="J6" s="390" t="s">
-        <v>138</v>
-      </c>
-      <c r="K6" s="395" t="s">
-        <v>123</v>
-      </c>
-      <c r="L6" s="400" t="s">
-        <v>127</v>
+      <c r="J6" s="459" t="s">
+        <v>121</v>
+      </c>
+      <c r="K6" s="464" t="s">
+        <v>125</v>
+      </c>
+      <c r="L6" s="469" t="s">
+        <v>129</v>
       </c>
       <c r="U6" s="6"/>
       <c r="V6" s="6"/>
@@ -8273,33 +8478,33 @@
     <row r="7" spans="1:31" ht="114" x14ac:dyDescent="0.25">
       <c r="A7" s="19"/>
       <c r="B7"/>
-      <c r="C7" s="362" t="s">
+      <c r="C7" s="432" t="s">
         <v>98</v>
       </c>
-      <c r="D7" s="367" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="371" t="s">
+      <c r="D7" s="437" t="s">
+        <v>110</v>
+      </c>
+      <c r="E7" s="441" t="s">
         <v>112</v>
       </c>
-      <c r="F7" s="376" t="s">
-        <v>134</v>
-      </c>
-      <c r="G7" s="381" t="s">
-        <v>114</v>
-      </c>
-      <c r="H7" s="386" t="s">
-        <v>116</v>
+      <c r="F7" s="446" t="s">
+        <v>131</v>
+      </c>
+      <c r="G7" s="451" t="s">
+        <v>109</v>
+      </c>
+      <c r="H7" s="456" t="s">
+        <v>118</v>
       </c>
       <c r="I7" s="59"/>
-      <c r="J7" s="391" t="s">
-        <v>139</v>
-      </c>
-      <c r="K7" s="396" t="s">
-        <v>124</v>
-      </c>
-      <c r="L7" s="401" t="s">
-        <v>128</v>
+      <c r="J7" s="460" t="s">
+        <v>122</v>
+      </c>
+      <c r="K7" s="465" t="s">
+        <v>126</v>
+      </c>
+      <c r="L7" s="470" t="s">
+        <v>130</v>
       </c>
       <c r="U7" s="6"/>
       <c r="V7" s="6"/>

</xml_diff>

<commit_message>
"galacticPubs::publish() [2022-07-26 17:59:09] "
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -356,7 +356,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="140">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -1077,7 +1077,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="471">
+  <cellXfs count="681">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1409,6 +1409,636 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="1"/>
@@ -5531,44 +6161,44 @@
       <c r="Z2" s="4"/>
     </row>
     <row r="3" spans="1:26" ht="56" x14ac:dyDescent="0.15">
-      <c r="A3" s="402" t="s">
+      <c r="A3" s="611" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="404" t="s">
+      <c r="B3" s="613" t="s">
         <v>98</v>
       </c>
-      <c r="C3" s="406" t="s">
+      <c r="C3" s="615" t="s">
         <v>99</v>
       </c>
-      <c r="D3" s="408" t="s">
+      <c r="D3" s="617" t="s">
         <v>100</v>
       </c>
-      <c r="E3" s="410" t="s">
+      <c r="E3" s="619" t="s">
         <v>102</v>
       </c>
       <c r="F3" s="46"/>
-      <c r="G3" s="412" t="s">
+      <c r="G3" s="621" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="56" x14ac:dyDescent="0.15">
-      <c r="A4" s="403" t="s">
+      <c r="A4" s="612" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="405" t="s">
+      <c r="B4" s="614" t="s">
         <v>99</v>
       </c>
-      <c r="C4" s="407" t="s">
+      <c r="C4" s="616" t="s">
         <v>99</v>
       </c>
-      <c r="D4" s="409" t="s">
+      <c r="D4" s="618" t="s">
         <v>101</v>
       </c>
-      <c r="E4" s="411" t="s">
+      <c r="E4" s="620" t="s">
         <v>103</v>
       </c>
       <c r="F4" s="47"/>
-      <c r="G4" s="413" t="s">
+      <c r="G4" s="622" t="s">
         <v>105</v>
       </c>
     </row>
@@ -6719,54 +7349,54 @@
     <row r="3" spans="1:30" ht="140" x14ac:dyDescent="0.15">
       <c r="A3" s="19"/>
       <c r="B3"/>
-      <c r="C3" s="414" t="s">
+      <c r="C3" s="623" t="s">
         <v>98</v>
       </c>
-      <c r="D3" s="416" t="s">
+      <c r="D3" s="625" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="418" t="s">
-        <v>41</v>
-      </c>
-      <c r="F3" s="420" t="s">
+      <c r="E3" s="627" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="629" t="s">
         <v>37</v>
       </c>
       <c r="G3" s="48"/>
-      <c r="H3" s="422" t="s">
+      <c r="H3" s="631" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="424" t="s">
+      <c r="I3" s="633" t="s">
         <v>39</v>
       </c>
       <c r="J3"/>
-      <c r="K3" s="426" t="s">
+      <c r="K3" s="635" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:30" ht="126" x14ac:dyDescent="0.15">
       <c r="A4" s="19"/>
       <c r="B4"/>
-      <c r="C4" s="415" t="s">
+      <c r="C4" s="624" t="s">
         <v>98</v>
       </c>
-      <c r="D4" s="417" t="s">
+      <c r="D4" s="626" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="419" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4" s="421" t="s">
+      <c r="E4" s="628" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="630" t="s">
         <v>42</v>
       </c>
       <c r="G4" s="49"/>
-      <c r="H4" s="423" t="s">
+      <c r="H4" s="632" t="s">
         <v>43</v>
       </c>
-      <c r="I4" s="425" t="s">
+      <c r="I4" s="634" t="s">
         <v>44</v>
       </c>
       <c r="J4"/>
-      <c r="K4" s="427" t="s">
+      <c r="K4" s="636" t="s">
         <v>107</v>
       </c>
     </row>
@@ -8326,29 +8956,33 @@
     <row r="3" spans="1:31" ht="86" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
       <c r="B3"/>
-      <c r="C3" s="428" t="s">
+      <c r="C3" s="637" t="s">
         <v>98</v>
       </c>
-      <c r="D3" s="433" t="s">
+      <c r="D3" s="642" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="368"/>
-      <c r="F3" s="442" t="s">
-        <v>133</v>
-      </c>
-      <c r="G3" s="447" t="s">
-        <v>113</v>
-      </c>
-      <c r="H3" s="452" t="s">
-        <v>51</v>
+      <c r="E3" s="647" t="s">
+        <v>111</v>
+      </c>
+      <c r="F3" s="651" t="s">
+        <v>131</v>
+      </c>
+      <c r="G3" s="656" t="s">
+        <v>109</v>
+      </c>
+      <c r="H3" s="661" t="s">
+        <v>117</v>
       </c>
       <c r="I3" s="55"/>
-      <c r="J3" s="387"/>
-      <c r="K3" s="461" t="s">
-        <v>52</v>
-      </c>
-      <c r="L3" s="466" t="s">
-        <v>108</v>
+      <c r="J3" s="666" t="s">
+        <v>136</v>
+      </c>
+      <c r="K3" s="671" t="s">
+        <v>125</v>
+      </c>
+      <c r="L3" s="676" t="s">
+        <v>129</v>
       </c>
       <c r="U3" s="6"/>
       <c r="V3" s="6"/>
@@ -8361,33 +8995,33 @@
     <row r="4" spans="1:31" ht="100" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
       <c r="B4"/>
-      <c r="C4" s="429" t="s">
+      <c r="C4" s="638" t="s">
         <v>98</v>
       </c>
-      <c r="D4" s="434" t="s">
-        <v>40</v>
-      </c>
-      <c r="E4" s="438" t="s">
-        <v>111</v>
-      </c>
-      <c r="F4" s="443" t="s">
-        <v>49</v>
-      </c>
-      <c r="G4" s="448" t="s">
-        <v>50</v>
-      </c>
-      <c r="H4" s="453" t="s">
-        <v>115</v>
+      <c r="D4" s="643" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="648" t="s">
+        <v>112</v>
+      </c>
+      <c r="F4" s="652" t="s">
+        <v>132</v>
+      </c>
+      <c r="G4" s="657" t="s">
+        <v>110</v>
+      </c>
+      <c r="H4" s="662" t="s">
+        <v>118</v>
       </c>
       <c r="I4" s="56"/>
-      <c r="J4" s="457" t="s">
-        <v>119</v>
-      </c>
-      <c r="K4" s="462" t="s">
-        <v>123</v>
-      </c>
-      <c r="L4" s="467" t="s">
-        <v>127</v>
+      <c r="J4" s="667" t="s">
+        <v>137</v>
+      </c>
+      <c r="K4" s="672" t="s">
+        <v>126</v>
+      </c>
+      <c r="L4" s="677" t="s">
+        <v>130</v>
       </c>
       <c r="U4" s="6"/>
       <c r="V4" s="6"/>
@@ -8400,33 +9034,31 @@
     <row r="5" spans="1:31" ht="100" x14ac:dyDescent="0.25">
       <c r="A5" s="19"/>
       <c r="B5"/>
-      <c r="C5" s="430" t="s">
+      <c r="C5" s="639" t="s">
         <v>98</v>
       </c>
-      <c r="D5" s="435" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" s="439" t="s">
-        <v>112</v>
-      </c>
-      <c r="F5" s="444" t="s">
-        <v>132</v>
-      </c>
-      <c r="G5" s="449" t="s">
-        <v>110</v>
-      </c>
-      <c r="H5" s="454" t="s">
-        <v>116</v>
+      <c r="D5" s="644" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="439"/>
+      <c r="F5" s="653" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="658" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" s="663" t="s">
+        <v>51</v>
       </c>
       <c r="I5" s="57"/>
-      <c r="J5" s="458" t="s">
-        <v>120</v>
-      </c>
-      <c r="K5" s="463" t="s">
-        <v>124</v>
-      </c>
-      <c r="L5" s="468" t="s">
-        <v>128</v>
+      <c r="J5" s="668" t="s">
+        <v>52</v>
+      </c>
+      <c r="K5" s="673" t="s">
+        <v>52</v>
+      </c>
+      <c r="L5" s="678" t="s">
+        <v>108</v>
       </c>
       <c r="U5" s="6"/>
       <c r="V5" s="6"/>
@@ -8439,33 +9071,33 @@
     <row r="6" spans="1:31" ht="114" x14ac:dyDescent="0.25">
       <c r="A6" s="19"/>
       <c r="B6"/>
-      <c r="C6" s="431" t="s">
+      <c r="C6" s="640" t="s">
         <v>98</v>
       </c>
-      <c r="D6" s="436" t="s">
-        <v>109</v>
-      </c>
-      <c r="E6" s="440" t="s">
+      <c r="D6" s="645" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="649" t="s">
         <v>111</v>
       </c>
-      <c r="F6" s="445" t="s">
-        <v>134</v>
-      </c>
-      <c r="G6" s="450" t="s">
-        <v>114</v>
-      </c>
-      <c r="H6" s="455" t="s">
-        <v>117</v>
+      <c r="F6" s="654" t="s">
+        <v>133</v>
+      </c>
+      <c r="G6" s="659" t="s">
+        <v>113</v>
+      </c>
+      <c r="H6" s="664" t="s">
+        <v>115</v>
       </c>
       <c r="I6" s="58"/>
-      <c r="J6" s="459" t="s">
-        <v>121</v>
-      </c>
-      <c r="K6" s="464" t="s">
-        <v>125</v>
-      </c>
-      <c r="L6" s="469" t="s">
-        <v>129</v>
+      <c r="J6" s="669" t="s">
+        <v>138</v>
+      </c>
+      <c r="K6" s="674" t="s">
+        <v>123</v>
+      </c>
+      <c r="L6" s="679" t="s">
+        <v>127</v>
       </c>
       <c r="U6" s="6"/>
       <c r="V6" s="6"/>
@@ -8478,33 +9110,33 @@
     <row r="7" spans="1:31" ht="114" x14ac:dyDescent="0.25">
       <c r="A7" s="19"/>
       <c r="B7"/>
-      <c r="C7" s="432" t="s">
+      <c r="C7" s="641" t="s">
         <v>98</v>
       </c>
-      <c r="D7" s="437" t="s">
-        <v>110</v>
-      </c>
-      <c r="E7" s="441" t="s">
+      <c r="D7" s="646" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="650" t="s">
         <v>112</v>
       </c>
-      <c r="F7" s="446" t="s">
-        <v>131</v>
-      </c>
-      <c r="G7" s="451" t="s">
-        <v>109</v>
-      </c>
-      <c r="H7" s="456" t="s">
-        <v>118</v>
+      <c r="F7" s="655" t="s">
+        <v>134</v>
+      </c>
+      <c r="G7" s="660" t="s">
+        <v>114</v>
+      </c>
+      <c r="H7" s="665" t="s">
+        <v>116</v>
       </c>
       <c r="I7" s="59"/>
-      <c r="J7" s="460" t="s">
-        <v>122</v>
-      </c>
-      <c r="K7" s="465" t="s">
-        <v>126</v>
-      </c>
-      <c r="L7" s="470" t="s">
-        <v>130</v>
+      <c r="J7" s="670" t="s">
+        <v>139</v>
+      </c>
+      <c r="K7" s="675" t="s">
+        <v>124</v>
+      </c>
+      <c r="L7" s="680" t="s">
+        <v>128</v>
       </c>
       <c r="U7" s="6"/>
       <c r="V7" s="6"/>

</xml_diff>

<commit_message>
"galacticPubs::publish() [2022-08-03 19:16:30]  fixed missing standards"
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -356,7 +356,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="140">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -1077,7 +1077,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="681">
+  <cellXfs count="751">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1409,6 +1409,216 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="1"/>
@@ -6161,44 +6371,44 @@
       <c r="Z2" s="4"/>
     </row>
     <row r="3" spans="1:26" ht="56" x14ac:dyDescent="0.15">
-      <c r="A3" s="611" t="s">
+      <c r="A3" s="681" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="613" t="s">
+      <c r="B3" s="683" t="s">
         <v>98</v>
       </c>
-      <c r="C3" s="615" t="s">
+      <c r="C3" s="685" t="s">
         <v>99</v>
       </c>
-      <c r="D3" s="617" t="s">
+      <c r="D3" s="687" t="s">
         <v>100</v>
       </c>
-      <c r="E3" s="619" t="s">
+      <c r="E3" s="689" t="s">
         <v>102</v>
       </c>
       <c r="F3" s="46"/>
-      <c r="G3" s="621" t="s">
+      <c r="G3" s="691" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="56" x14ac:dyDescent="0.15">
-      <c r="A4" s="612" t="s">
+      <c r="A4" s="682" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="614" t="s">
+      <c r="B4" s="684" t="s">
         <v>99</v>
       </c>
-      <c r="C4" s="616" t="s">
+      <c r="C4" s="686" t="s">
         <v>99</v>
       </c>
-      <c r="D4" s="618" t="s">
+      <c r="D4" s="688" t="s">
         <v>101</v>
       </c>
-      <c r="E4" s="620" t="s">
+      <c r="E4" s="690" t="s">
         <v>103</v>
       </c>
       <c r="F4" s="47"/>
-      <c r="G4" s="622" t="s">
+      <c r="G4" s="692" t="s">
         <v>105</v>
       </c>
     </row>
@@ -7349,54 +7559,54 @@
     <row r="3" spans="1:30" ht="140" x14ac:dyDescent="0.15">
       <c r="A3" s="19"/>
       <c r="B3"/>
-      <c r="C3" s="623" t="s">
+      <c r="C3" s="693" t="s">
         <v>98</v>
       </c>
-      <c r="D3" s="625" t="s">
+      <c r="D3" s="695" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="627" t="s">
+      <c r="E3" s="697" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="629" t="s">
+      <c r="F3" s="699" t="s">
         <v>37</v>
       </c>
       <c r="G3" s="48"/>
-      <c r="H3" s="631" t="s">
+      <c r="H3" s="701" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="633" t="s">
+      <c r="I3" s="703" t="s">
         <v>39</v>
       </c>
       <c r="J3"/>
-      <c r="K3" s="635" t="s">
+      <c r="K3" s="705" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:30" ht="126" x14ac:dyDescent="0.15">
       <c r="A4" s="19"/>
       <c r="B4"/>
-      <c r="C4" s="624" t="s">
+      <c r="C4" s="694" t="s">
         <v>98</v>
       </c>
-      <c r="D4" s="626" t="s">
+      <c r="D4" s="696" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="628" t="s">
+      <c r="E4" s="698" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="630" t="s">
+      <c r="F4" s="700" t="s">
         <v>42</v>
       </c>
       <c r="G4" s="49"/>
-      <c r="H4" s="632" t="s">
+      <c r="H4" s="702" t="s">
         <v>43</v>
       </c>
-      <c r="I4" s="634" t="s">
+      <c r="I4" s="704" t="s">
         <v>44</v>
       </c>
       <c r="J4"/>
-      <c r="K4" s="636" t="s">
+      <c r="K4" s="706" t="s">
         <v>107</v>
       </c>
     </row>
@@ -8956,32 +9166,32 @@
     <row r="3" spans="1:31" ht="86" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
       <c r="B3"/>
-      <c r="C3" s="637" t="s">
+      <c r="C3" s="707" t="s">
         <v>98</v>
       </c>
-      <c r="D3" s="642" t="s">
+      <c r="D3" s="712" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="647" t="s">
+      <c r="E3" s="717" t="s">
         <v>111</v>
       </c>
-      <c r="F3" s="651" t="s">
+      <c r="F3" s="721" t="s">
         <v>131</v>
       </c>
-      <c r="G3" s="656" t="s">
+      <c r="G3" s="726" t="s">
         <v>109</v>
       </c>
-      <c r="H3" s="661" t="s">
+      <c r="H3" s="731" t="s">
         <v>117</v>
       </c>
       <c r="I3" s="55"/>
-      <c r="J3" s="666" t="s">
+      <c r="J3" s="736" t="s">
         <v>136</v>
       </c>
-      <c r="K3" s="671" t="s">
+      <c r="K3" s="741" t="s">
         <v>125</v>
       </c>
-      <c r="L3" s="676" t="s">
+      <c r="L3" s="746" t="s">
         <v>129</v>
       </c>
       <c r="U3" s="6"/>
@@ -8995,32 +9205,32 @@
     <row r="4" spans="1:31" ht="100" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
       <c r="B4"/>
-      <c r="C4" s="638" t="s">
+      <c r="C4" s="708" t="s">
         <v>98</v>
       </c>
-      <c r="D4" s="643" t="s">
+      <c r="D4" s="713" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="648" t="s">
+      <c r="E4" s="718" t="s">
         <v>112</v>
       </c>
-      <c r="F4" s="652" t="s">
+      <c r="F4" s="722" t="s">
         <v>132</v>
       </c>
-      <c r="G4" s="657" t="s">
+      <c r="G4" s="727" t="s">
         <v>110</v>
       </c>
-      <c r="H4" s="662" t="s">
+      <c r="H4" s="732" t="s">
         <v>118</v>
       </c>
       <c r="I4" s="56"/>
-      <c r="J4" s="667" t="s">
+      <c r="J4" s="737" t="s">
         <v>137</v>
       </c>
-      <c r="K4" s="672" t="s">
+      <c r="K4" s="742" t="s">
         <v>126</v>
       </c>
-      <c r="L4" s="677" t="s">
+      <c r="L4" s="747" t="s">
         <v>130</v>
       </c>
       <c r="U4" s="6"/>
@@ -9034,30 +9244,30 @@
     <row r="5" spans="1:31" ht="100" x14ac:dyDescent="0.25">
       <c r="A5" s="19"/>
       <c r="B5"/>
-      <c r="C5" s="639" t="s">
+      <c r="C5" s="709" t="s">
         <v>98</v>
       </c>
-      <c r="D5" s="644" t="s">
+      <c r="D5" s="714" t="s">
         <v>35</v>
       </c>
       <c r="E5" s="439"/>
-      <c r="F5" s="653" t="s">
+      <c r="F5" s="723" t="s">
         <v>49</v>
       </c>
-      <c r="G5" s="658" t="s">
+      <c r="G5" s="728" t="s">
         <v>50</v>
       </c>
-      <c r="H5" s="663" t="s">
+      <c r="H5" s="733" t="s">
         <v>51</v>
       </c>
       <c r="I5" s="57"/>
-      <c r="J5" s="668" t="s">
+      <c r="J5" s="738" t="s">
         <v>52</v>
       </c>
-      <c r="K5" s="673" t="s">
+      <c r="K5" s="743" t="s">
         <v>52</v>
       </c>
-      <c r="L5" s="678" t="s">
+      <c r="L5" s="748" t="s">
         <v>108</v>
       </c>
       <c r="U5" s="6"/>
@@ -9071,32 +9281,32 @@
     <row r="6" spans="1:31" ht="114" x14ac:dyDescent="0.25">
       <c r="A6" s="19"/>
       <c r="B6"/>
-      <c r="C6" s="640" t="s">
+      <c r="C6" s="710" t="s">
         <v>98</v>
       </c>
-      <c r="D6" s="645" t="s">
+      <c r="D6" s="715" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="649" t="s">
+      <c r="E6" s="719" t="s">
         <v>111</v>
       </c>
-      <c r="F6" s="654" t="s">
+      <c r="F6" s="724" t="s">
         <v>133</v>
       </c>
-      <c r="G6" s="659" t="s">
+      <c r="G6" s="729" t="s">
         <v>113</v>
       </c>
-      <c r="H6" s="664" t="s">
+      <c r="H6" s="734" t="s">
         <v>115</v>
       </c>
       <c r="I6" s="58"/>
-      <c r="J6" s="669" t="s">
+      <c r="J6" s="739" t="s">
         <v>138</v>
       </c>
-      <c r="K6" s="674" t="s">
+      <c r="K6" s="744" t="s">
         <v>123</v>
       </c>
-      <c r="L6" s="679" t="s">
+      <c r="L6" s="749" t="s">
         <v>127</v>
       </c>
       <c r="U6" s="6"/>
@@ -9110,32 +9320,32 @@
     <row r="7" spans="1:31" ht="114" x14ac:dyDescent="0.25">
       <c r="A7" s="19"/>
       <c r="B7"/>
-      <c r="C7" s="641" t="s">
+      <c r="C7" s="711" t="s">
         <v>98</v>
       </c>
-      <c r="D7" s="646" t="s">
+      <c r="D7" s="716" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="650" t="s">
+      <c r="E7" s="720" t="s">
         <v>112</v>
       </c>
-      <c r="F7" s="655" t="s">
+      <c r="F7" s="725" t="s">
         <v>134</v>
       </c>
-      <c r="G7" s="660" t="s">
+      <c r="G7" s="730" t="s">
         <v>114</v>
       </c>
-      <c r="H7" s="665" t="s">
+      <c r="H7" s="735" t="s">
         <v>116</v>
       </c>
       <c r="I7" s="59"/>
-      <c r="J7" s="670" t="s">
+      <c r="J7" s="740" t="s">
         <v>139</v>
       </c>
-      <c r="K7" s="675" t="s">
+      <c r="K7" s="745" t="s">
         <v>124</v>
       </c>
-      <c r="L7" s="680" t="s">
+      <c r="L7" s="750" t="s">
         <v>128</v>
       </c>
       <c r="U7" s="6"/>

</xml_diff>

<commit_message>
"galacticPubs::publish() [2022-09-01 08:58:37] "
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -207,7 +207,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="136">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -910,7 +910,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="550">
+  <cellXfs count="620">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1017,6 +1017,216 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
@@ -5599,44 +5809,44 @@
       <c r="Z2" s="7"/>
     </row>
     <row r="3">
-      <c r="A3" s="480" t="s">
+      <c r="A3" s="550" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="482" t="s">
+      <c r="B3" s="552" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="484" t="s">
+      <c r="C3" s="554" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="486" t="s">
+      <c r="D3" s="556" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="488" t="s">
+      <c r="E3" s="558" t="s">
         <v>31</v>
       </c>
       <c r="F3" s="14"/>
-      <c r="G3" s="490" t="s">
+      <c r="G3" s="560" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="481" t="s">
+      <c r="A4" s="551" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="483" t="s">
+      <c r="B4" s="553" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="485" t="s">
+      <c r="C4" s="555" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="487" t="s">
+      <c r="D4" s="557" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="489" t="s">
+      <c r="E4" s="559" t="s">
         <v>34</v>
       </c>
       <c r="F4" s="14"/>
-      <c r="G4" s="491" t="s">
+      <c r="G4" s="561" t="s">
         <v>35</v>
       </c>
     </row>
@@ -6790,54 +7000,54 @@
     <row r="3">
       <c r="A3" s="23"/>
       <c r="B3"/>
-      <c r="C3" s="492" t="s">
+      <c r="C3" s="562" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="494" t="s">
+      <c r="D3" s="564" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="496" t="s">
+      <c r="E3" s="566" t="s">
         <v>44</v>
       </c>
-      <c r="F3" s="498" t="s">
+      <c r="F3" s="568" t="s">
         <v>45</v>
       </c>
       <c r="G3" s="14"/>
-      <c r="H3" s="500" t="s">
+      <c r="H3" s="570" t="s">
         <v>46</v>
       </c>
-      <c r="I3" s="502" t="s">
+      <c r="I3" s="572" t="s">
         <v>47</v>
       </c>
       <c r="J3"/>
-      <c r="K3" s="504" t="s">
+      <c r="K3" s="574" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="23"/>
       <c r="B4"/>
-      <c r="C4" s="493" t="s">
+      <c r="C4" s="563" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="495" t="s">
+      <c r="D4" s="565" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="497" t="s">
+      <c r="E4" s="567" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="499" t="s">
+      <c r="F4" s="569" t="s">
         <v>51</v>
       </c>
       <c r="G4" s="14"/>
-      <c r="H4" s="501" t="s">
+      <c r="H4" s="571" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="503" t="s">
+      <c r="I4" s="573" t="s">
         <v>53</v>
       </c>
       <c r="J4"/>
-      <c r="K4" s="505" t="s">
+      <c r="K4" s="575" t="s">
         <v>54</v>
       </c>
     </row>
@@ -10202,32 +10412,32 @@
     <row r="3">
       <c r="A3" s="23"/>
       <c r="B3"/>
-      <c r="C3" s="506" t="s">
+      <c r="C3" s="576" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="511" t="s">
+      <c r="D3" s="581" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="516" t="s">
+      <c r="E3" s="586" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="520" t="s">
+      <c r="F3" s="590" t="s">
         <v>60</v>
       </c>
-      <c r="G3" s="525" t="s">
+      <c r="G3" s="595" t="s">
         <v>61</v>
       </c>
-      <c r="H3" s="530" t="s">
+      <c r="H3" s="600" t="s">
         <v>62</v>
       </c>
       <c r="I3" s="14"/>
-      <c r="J3" s="535" t="s">
+      <c r="J3" s="605" t="s">
         <v>63</v>
       </c>
-      <c r="K3" s="540" t="s">
+      <c r="K3" s="610" t="s">
         <v>64</v>
       </c>
-      <c r="L3" s="545" t="s">
+      <c r="L3" s="615" t="s">
         <v>65</v>
       </c>
       <c r="U3" s="9"/>
@@ -10241,32 +10451,32 @@
     <row r="4">
       <c r="A4" s="23"/>
       <c r="B4"/>
-      <c r="C4" s="507" t="s">
+      <c r="C4" s="577" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="512" t="s">
+      <c r="D4" s="582" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="517" t="s">
+      <c r="E4" s="587" t="s">
         <v>66</v>
       </c>
-      <c r="F4" s="521" t="s">
+      <c r="F4" s="591" t="s">
         <v>67</v>
       </c>
-      <c r="G4" s="526" t="s">
+      <c r="G4" s="596" t="s">
         <v>68</v>
       </c>
-      <c r="H4" s="531" t="s">
+      <c r="H4" s="601" t="s">
         <v>69</v>
       </c>
       <c r="I4" s="14"/>
-      <c r="J4" s="536" t="s">
+      <c r="J4" s="606" t="s">
         <v>70</v>
       </c>
-      <c r="K4" s="541" t="s">
+      <c r="K4" s="611" t="s">
         <v>71</v>
       </c>
-      <c r="L4" s="546" t="s">
+      <c r="L4" s="616" t="s">
         <v>72</v>
       </c>
       <c r="U4" s="9"/>
@@ -10280,30 +10490,30 @@
     <row r="5">
       <c r="A5" s="23"/>
       <c r="B5"/>
-      <c r="C5" s="508" t="s">
+      <c r="C5" s="578" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="513" t="s">
+      <c r="D5" s="583" t="s">
         <v>43</v>
       </c>
       <c r="E5" s="14"/>
-      <c r="F5" s="522" t="s">
+      <c r="F5" s="592" t="s">
         <v>73</v>
       </c>
-      <c r="G5" s="527" t="s">
+      <c r="G5" s="597" t="s">
         <v>74</v>
       </c>
-      <c r="H5" s="532" t="s">
+      <c r="H5" s="602" t="s">
         <v>75</v>
       </c>
       <c r="I5" s="14"/>
-      <c r="J5" s="537" t="s">
+      <c r="J5" s="607" t="s">
         <v>76</v>
       </c>
-      <c r="K5" s="542" t="s">
+      <c r="K5" s="612" t="s">
         <v>76</v>
       </c>
-      <c r="L5" s="547" t="s">
+      <c r="L5" s="617" t="s">
         <v>77</v>
       </c>
       <c r="U5" s="9"/>
@@ -10317,32 +10527,32 @@
     <row r="6">
       <c r="A6" s="23"/>
       <c r="B6"/>
-      <c r="C6" s="509" t="s">
+      <c r="C6" s="579" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="514" t="s">
+      <c r="D6" s="584" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="518" t="s">
+      <c r="E6" s="588" t="s">
         <v>59</v>
       </c>
-      <c r="F6" s="523" t="s">
+      <c r="F6" s="593" t="s">
         <v>78</v>
       </c>
-      <c r="G6" s="528" t="s">
+      <c r="G6" s="598" t="s">
         <v>79</v>
       </c>
-      <c r="H6" s="533" t="s">
+      <c r="H6" s="603" t="s">
         <v>80</v>
       </c>
       <c r="I6" s="14"/>
-      <c r="J6" s="538" t="s">
+      <c r="J6" s="608" t="s">
         <v>81</v>
       </c>
-      <c r="K6" s="543" t="s">
+      <c r="K6" s="613" t="s">
         <v>82</v>
       </c>
-      <c r="L6" s="548" t="s">
+      <c r="L6" s="618" t="s">
         <v>83</v>
       </c>
       <c r="U6" s="9"/>
@@ -10356,32 +10566,32 @@
     <row r="7">
       <c r="A7" s="23"/>
       <c r="B7"/>
-      <c r="C7" s="510" t="s">
+      <c r="C7" s="580" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="515" t="s">
+      <c r="D7" s="585" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="519" t="s">
+      <c r="E7" s="589" t="s">
         <v>66</v>
       </c>
-      <c r="F7" s="524" t="s">
+      <c r="F7" s="594" t="s">
         <v>84</v>
       </c>
-      <c r="G7" s="529" t="s">
+      <c r="G7" s="599" t="s">
         <v>85</v>
       </c>
-      <c r="H7" s="534" t="s">
+      <c r="H7" s="604" t="s">
         <v>86</v>
       </c>
       <c r="I7" s="14"/>
-      <c r="J7" s="539" t="s">
+      <c r="J7" s="609" t="s">
         <v>87</v>
       </c>
-      <c r="K7" s="544" t="s">
+      <c r="K7" s="614" t="s">
         <v>88</v>
       </c>
-      <c r="L7" s="549" t="s">
+      <c r="L7" s="619" t="s">
         <v>89</v>
       </c>
       <c r="U7" s="9"/>

</xml_diff>

<commit_message>
"galacticPubs::publish() [2022-09-08 23:20:20] "
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -207,7 +207,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="923" uniqueCount="142">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -616,6 +616,24 @@
   <si>
     <t>*asset-links is for worksheets and other resources that you may want to link to in presentations</t>
   </si>
+  <si>
+    <t>(P1)</t>
+  </si>
+  <si>
+    <t>GuardianFrogs_P1_Role With It_Cards</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/1Q37IPnIAQPkdTgCT-icgFsLeu9-JXB_OJKVx7yYLIP0/edit?usp=drivesdk</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/1Q37IPnIAQPkdTgCT-icgFsLeu9-JXB_OJKVx7yYLIP0/template/preview</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/1Q37IPnIAQPkdTgCT-icgFsLeu9-JXB_OJKVx7yYLIP0/export?format=pdf</t>
+  </si>
+  <si>
+    <t>1Q37IPnIAQPkdTgCT-icgFsLeu9-JXB_OJKVx7yYLIP0</t>
+  </si>
 </sst>
 </file>
 
@@ -910,7 +928,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="620">
+  <cellXfs count="698">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1017,6 +1035,240 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
@@ -5809,44 +6061,44 @@
       <c r="Z2" s="7"/>
     </row>
     <row r="3">
-      <c r="A3" s="550" t="s">
+      <c r="A3" s="620" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="552" t="s">
+      <c r="B3" s="622" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="554" t="s">
+      <c r="C3" s="624" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="556" t="s">
+      <c r="D3" s="626" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="558" t="s">
+      <c r="E3" s="628" t="s">
         <v>31</v>
       </c>
       <c r="F3" s="14"/>
-      <c r="G3" s="560" t="s">
+      <c r="G3" s="630" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="551" t="s">
+      <c r="A4" s="621" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="553" t="s">
+      <c r="B4" s="623" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="555" t="s">
+      <c r="C4" s="625" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="557" t="s">
+      <c r="D4" s="627" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="559" t="s">
+      <c r="E4" s="629" t="s">
         <v>34</v>
       </c>
       <c r="F4" s="14"/>
-      <c r="G4" s="561" t="s">
+      <c r="G4" s="631" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7000,54 +7252,54 @@
     <row r="3">
       <c r="A3" s="23"/>
       <c r="B3"/>
-      <c r="C3" s="562" t="s">
+      <c r="C3" s="632" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="564" t="s">
+      <c r="D3" s="634" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="566" t="s">
+      <c r="E3" s="636" t="s">
         <v>44</v>
       </c>
-      <c r="F3" s="568" t="s">
+      <c r="F3" s="638" t="s">
         <v>45</v>
       </c>
       <c r="G3" s="14"/>
-      <c r="H3" s="570" t="s">
+      <c r="H3" s="640" t="s">
         <v>46</v>
       </c>
-      <c r="I3" s="572" t="s">
+      <c r="I3" s="642" t="s">
         <v>47</v>
       </c>
       <c r="J3"/>
-      <c r="K3" s="574" t="s">
+      <c r="K3" s="644" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="23"/>
       <c r="B4"/>
-      <c r="C4" s="563" t="s">
+      <c r="C4" s="633" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="565" t="s">
+      <c r="D4" s="635" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="567" t="s">
+      <c r="E4" s="637" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="569" t="s">
+      <c r="F4" s="639" t="s">
         <v>51</v>
       </c>
       <c r="G4" s="14"/>
-      <c r="H4" s="571" t="s">
+      <c r="H4" s="641" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="573" t="s">
+      <c r="I4" s="643" t="s">
         <v>53</v>
       </c>
       <c r="J4"/>
-      <c r="K4" s="575" t="s">
+      <c r="K4" s="645" t="s">
         <v>54</v>
       </c>
     </row>
@@ -10412,32 +10664,32 @@
     <row r="3">
       <c r="A3" s="23"/>
       <c r="B3"/>
-      <c r="C3" s="576" t="s">
+      <c r="C3" s="646" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="581" t="s">
+      <c r="D3" s="652" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="586" t="s">
+      <c r="E3" s="658" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="590" t="s">
+      <c r="F3" s="662" t="s">
         <v>60</v>
       </c>
-      <c r="G3" s="595" t="s">
+      <c r="G3" s="668" t="s">
         <v>61</v>
       </c>
-      <c r="H3" s="600" t="s">
+      <c r="H3" s="674" t="s">
         <v>62</v>
       </c>
       <c r="I3" s="14"/>
-      <c r="J3" s="605" t="s">
+      <c r="J3" s="680" t="s">
         <v>63</v>
       </c>
-      <c r="K3" s="610" t="s">
+      <c r="K3" s="686" t="s">
         <v>64</v>
       </c>
-      <c r="L3" s="615" t="s">
+      <c r="L3" s="692" t="s">
         <v>65</v>
       </c>
       <c r="U3" s="9"/>
@@ -10451,32 +10703,32 @@
     <row r="4">
       <c r="A4" s="23"/>
       <c r="B4"/>
-      <c r="C4" s="577" t="s">
+      <c r="C4" s="647" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="582" t="s">
+      <c r="D4" s="653" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="587" t="s">
+      <c r="E4" s="659" t="s">
         <v>66</v>
       </c>
-      <c r="F4" s="591" t="s">
+      <c r="F4" s="663" t="s">
         <v>67</v>
       </c>
-      <c r="G4" s="596" t="s">
+      <c r="G4" s="669" t="s">
         <v>68</v>
       </c>
-      <c r="H4" s="601" t="s">
+      <c r="H4" s="675" t="s">
         <v>69</v>
       </c>
       <c r="I4" s="14"/>
-      <c r="J4" s="606" t="s">
+      <c r="J4" s="681" t="s">
         <v>70</v>
       </c>
-      <c r="K4" s="611" t="s">
+      <c r="K4" s="687" t="s">
         <v>71</v>
       </c>
-      <c r="L4" s="616" t="s">
+      <c r="L4" s="693" t="s">
         <v>72</v>
       </c>
       <c r="U4" s="9"/>
@@ -10490,30 +10742,30 @@
     <row r="5">
       <c r="A5" s="23"/>
       <c r="B5"/>
-      <c r="C5" s="578" t="s">
+      <c r="C5" s="648" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="583" t="s">
+      <c r="D5" s="654" t="s">
         <v>43</v>
       </c>
       <c r="E5" s="14"/>
-      <c r="F5" s="592" t="s">
+      <c r="F5" s="664" t="s">
         <v>73</v>
       </c>
-      <c r="G5" s="597" t="s">
+      <c r="G5" s="670" t="s">
         <v>74</v>
       </c>
-      <c r="H5" s="602" t="s">
+      <c r="H5" s="676" t="s">
         <v>75</v>
       </c>
       <c r="I5" s="14"/>
-      <c r="J5" s="607" t="s">
+      <c r="J5" s="682" t="s">
         <v>76</v>
       </c>
-      <c r="K5" s="612" t="s">
+      <c r="K5" s="688" t="s">
         <v>76</v>
       </c>
-      <c r="L5" s="617" t="s">
+      <c r="L5" s="694" t="s">
         <v>77</v>
       </c>
       <c r="U5" s="9"/>
@@ -10527,33 +10779,31 @@
     <row r="6">
       <c r="A6" s="23"/>
       <c r="B6"/>
-      <c r="C6" s="579" t="s">
+      <c r="C6" s="649" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="584" t="s">
-        <v>49</v>
+      <c r="D6" s="655" t="s">
+        <v>43</v>
       </c>
-      <c r="E6" s="588" t="s">
-        <v>59</v>
+      <c r="E6" s="588"/>
+      <c r="F6" s="665" t="s">
+        <v>136</v>
       </c>
-      <c r="F6" s="593" t="s">
-        <v>78</v>
+      <c r="G6" s="671" t="s">
+        <v>137</v>
       </c>
-      <c r="G6" s="598" t="s">
-        <v>79</v>
-      </c>
-      <c r="H6" s="603" t="s">
-        <v>80</v>
+      <c r="H6" s="677" t="s">
+        <v>138</v>
       </c>
       <c r="I6" s="14"/>
-      <c r="J6" s="608" t="s">
-        <v>81</v>
+      <c r="J6" s="683" t="s">
+        <v>139</v>
       </c>
-      <c r="K6" s="613" t="s">
-        <v>82</v>
+      <c r="K6" s="689" t="s">
+        <v>140</v>
       </c>
-      <c r="L6" s="618" t="s">
-        <v>83</v>
+      <c r="L6" s="695" t="s">
+        <v>141</v>
       </c>
       <c r="U6" s="9"/>
       <c r="V6" s="9"/>
@@ -10566,33 +10816,33 @@
     <row r="7">
       <c r="A7" s="23"/>
       <c r="B7"/>
-      <c r="C7" s="580" t="s">
+      <c r="C7" s="650" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="585" t="s">
+      <c r="D7" s="656" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="589" t="s">
-        <v>66</v>
+      <c r="E7" s="660" t="s">
+        <v>59</v>
       </c>
-      <c r="F7" s="594" t="s">
-        <v>84</v>
+      <c r="F7" s="666" t="s">
+        <v>78</v>
       </c>
-      <c r="G7" s="599" t="s">
-        <v>85</v>
+      <c r="G7" s="672" t="s">
+        <v>79</v>
       </c>
-      <c r="H7" s="604" t="s">
-        <v>86</v>
+      <c r="H7" s="678" t="s">
+        <v>80</v>
       </c>
       <c r="I7" s="14"/>
-      <c r="J7" s="609" t="s">
-        <v>87</v>
+      <c r="J7" s="684" t="s">
+        <v>81</v>
       </c>
-      <c r="K7" s="614" t="s">
-        <v>88</v>
+      <c r="K7" s="690" t="s">
+        <v>82</v>
       </c>
-      <c r="L7" s="619" t="s">
-        <v>89</v>
+      <c r="L7" s="696" t="s">
+        <v>83</v>
       </c>
       <c r="U7" s="9"/>
       <c r="V7" s="9"/>
@@ -10604,15 +10854,35 @@
     </row>
     <row r="8">
       <c r="A8" s="23"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
+      <c r="B8"/>
+      <c r="C8" s="651" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="657" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="661" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" s="667" t="s">
+        <v>84</v>
+      </c>
+      <c r="G8" s="673" t="s">
+        <v>85</v>
+      </c>
+      <c r="H8" s="679" t="s">
+        <v>86</v>
+      </c>
       <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
+      <c r="J8" s="685" t="s">
+        <v>87</v>
+      </c>
+      <c r="K8" s="691" t="s">
+        <v>88</v>
+      </c>
+      <c r="L8" t="s" s="697">
+        <v>89</v>
+      </c>
       <c r="U8" s="9"/>
       <c r="V8" s="9"/>
       <c r="W8" s="9"/>

</xml_diff>

<commit_message>
"galacticPubs::publish() [2022-09-09 00:22:11] "
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -207,7 +207,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="923" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="142">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -928,7 +928,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="698">
+  <cellXfs count="776">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1035,6 +1035,240 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
@@ -6061,44 +6295,44 @@
       <c r="Z2" s="7"/>
     </row>
     <row r="3">
-      <c r="A3" s="620" t="s">
+      <c r="A3" s="698" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="622" t="s">
+      <c r="B3" s="700" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="624" t="s">
+      <c r="C3" s="702" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="626" t="s">
+      <c r="D3" s="704" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="628" t="s">
+      <c r="E3" s="706" t="s">
         <v>31</v>
       </c>
       <c r="F3" s="14"/>
-      <c r="G3" s="630" t="s">
+      <c r="G3" s="708" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="621" t="s">
+      <c r="A4" s="699" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="623" t="s">
+      <c r="B4" s="701" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="625" t="s">
+      <c r="C4" s="703" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="627" t="s">
+      <c r="D4" s="705" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="629" t="s">
+      <c r="E4" s="707" t="s">
         <v>34</v>
       </c>
       <c r="F4" s="14"/>
-      <c r="G4" s="631" t="s">
+      <c r="G4" s="709" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7252,54 +7486,54 @@
     <row r="3">
       <c r="A3" s="23"/>
       <c r="B3"/>
-      <c r="C3" s="632" t="s">
+      <c r="C3" s="710" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="634" t="s">
+      <c r="D3" s="712" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="636" t="s">
+      <c r="E3" s="714" t="s">
         <v>44</v>
       </c>
-      <c r="F3" s="638" t="s">
+      <c r="F3" s="716" t="s">
         <v>45</v>
       </c>
       <c r="G3" s="14"/>
-      <c r="H3" s="640" t="s">
+      <c r="H3" s="718" t="s">
         <v>46</v>
       </c>
-      <c r="I3" s="642" t="s">
+      <c r="I3" s="720" t="s">
         <v>47</v>
       </c>
       <c r="J3"/>
-      <c r="K3" s="644" t="s">
+      <c r="K3" s="722" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="23"/>
       <c r="B4"/>
-      <c r="C4" s="633" t="s">
+      <c r="C4" s="711" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="635" t="s">
+      <c r="D4" s="713" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="637" t="s">
+      <c r="E4" s="715" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="639" t="s">
+      <c r="F4" s="717" t="s">
         <v>51</v>
       </c>
       <c r="G4" s="14"/>
-      <c r="H4" s="641" t="s">
+      <c r="H4" s="719" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="643" t="s">
+      <c r="I4" s="721" t="s">
         <v>53</v>
       </c>
       <c r="J4"/>
-      <c r="K4" s="645" t="s">
+      <c r="K4" s="723" t="s">
         <v>54</v>
       </c>
     </row>
@@ -10664,32 +10898,32 @@
     <row r="3">
       <c r="A3" s="23"/>
       <c r="B3"/>
-      <c r="C3" s="646" t="s">
+      <c r="C3" s="724" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="652" t="s">
+      <c r="D3" s="730" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="658" t="s">
+      <c r="E3" s="736" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="662" t="s">
+      <c r="F3" s="740" t="s">
         <v>60</v>
       </c>
-      <c r="G3" s="668" t="s">
+      <c r="G3" s="746" t="s">
         <v>61</v>
       </c>
-      <c r="H3" s="674" t="s">
+      <c r="H3" s="752" t="s">
         <v>62</v>
       </c>
       <c r="I3" s="14"/>
-      <c r="J3" s="680" t="s">
+      <c r="J3" s="758" t="s">
         <v>63</v>
       </c>
-      <c r="K3" s="686" t="s">
+      <c r="K3" s="764" t="s">
         <v>64</v>
       </c>
-      <c r="L3" s="692" t="s">
+      <c r="L3" s="770" t="s">
         <v>65</v>
       </c>
       <c r="U3" s="9"/>
@@ -10703,32 +10937,32 @@
     <row r="4">
       <c r="A4" s="23"/>
       <c r="B4"/>
-      <c r="C4" s="647" t="s">
+      <c r="C4" s="725" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="653" t="s">
+      <c r="D4" s="731" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="659" t="s">
+      <c r="E4" s="737" t="s">
         <v>66</v>
       </c>
-      <c r="F4" s="663" t="s">
+      <c r="F4" s="741" t="s">
         <v>67</v>
       </c>
-      <c r="G4" s="669" t="s">
+      <c r="G4" s="747" t="s">
         <v>68</v>
       </c>
-      <c r="H4" s="675" t="s">
+      <c r="H4" s="753" t="s">
         <v>69</v>
       </c>
       <c r="I4" s="14"/>
-      <c r="J4" s="681" t="s">
+      <c r="J4" s="759" t="s">
         <v>70</v>
       </c>
-      <c r="K4" s="687" t="s">
+      <c r="K4" s="765" t="s">
         <v>71</v>
       </c>
-      <c r="L4" s="693" t="s">
+      <c r="L4" s="771" t="s">
         <v>72</v>
       </c>
       <c r="U4" s="9"/>
@@ -10742,30 +10976,30 @@
     <row r="5">
       <c r="A5" s="23"/>
       <c r="B5"/>
-      <c r="C5" s="648" t="s">
+      <c r="C5" s="726" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="654" t="s">
+      <c r="D5" s="732" t="s">
         <v>43</v>
       </c>
       <c r="E5" s="14"/>
-      <c r="F5" s="664" t="s">
+      <c r="F5" s="742" t="s">
         <v>73</v>
       </c>
-      <c r="G5" s="670" t="s">
+      <c r="G5" s="748" t="s">
         <v>74</v>
       </c>
-      <c r="H5" s="676" t="s">
+      <c r="H5" s="754" t="s">
         <v>75</v>
       </c>
       <c r="I5" s="14"/>
-      <c r="J5" s="682" t="s">
+      <c r="J5" s="760" t="s">
         <v>76</v>
       </c>
-      <c r="K5" s="688" t="s">
+      <c r="K5" s="766" t="s">
         <v>76</v>
       </c>
-      <c r="L5" s="694" t="s">
+      <c r="L5" s="772" t="s">
         <v>77</v>
       </c>
       <c r="U5" s="9"/>
@@ -10779,30 +11013,30 @@
     <row r="6">
       <c r="A6" s="23"/>
       <c r="B6"/>
-      <c r="C6" s="649" t="s">
+      <c r="C6" s="727" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="655" t="s">
+      <c r="D6" s="733" t="s">
         <v>43</v>
       </c>
       <c r="E6" s="588"/>
-      <c r="F6" s="665" t="s">
+      <c r="F6" s="743" t="s">
         <v>136</v>
       </c>
-      <c r="G6" s="671" t="s">
+      <c r="G6" s="749" t="s">
         <v>137</v>
       </c>
-      <c r="H6" s="677" t="s">
+      <c r="H6" s="755" t="s">
         <v>138</v>
       </c>
       <c r="I6" s="14"/>
-      <c r="J6" s="683" t="s">
+      <c r="J6" s="761" t="s">
         <v>139</v>
       </c>
-      <c r="K6" s="689" t="s">
+      <c r="K6" s="767" t="s">
         <v>140</v>
       </c>
-      <c r="L6" s="695" t="s">
+      <c r="L6" s="773" t="s">
         <v>141</v>
       </c>
       <c r="U6" s="9"/>
@@ -10816,32 +11050,32 @@
     <row r="7">
       <c r="A7" s="23"/>
       <c r="B7"/>
-      <c r="C7" s="650" t="s">
+      <c r="C7" s="728" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="656" t="s">
+      <c r="D7" s="734" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="660" t="s">
+      <c r="E7" s="738" t="s">
         <v>59</v>
       </c>
-      <c r="F7" s="666" t="s">
+      <c r="F7" s="744" t="s">
         <v>78</v>
       </c>
-      <c r="G7" s="672" t="s">
+      <c r="G7" s="750" t="s">
         <v>79</v>
       </c>
-      <c r="H7" s="678" t="s">
+      <c r="H7" s="756" t="s">
         <v>80</v>
       </c>
       <c r="I7" s="14"/>
-      <c r="J7" s="684" t="s">
+      <c r="J7" s="762" t="s">
         <v>81</v>
       </c>
-      <c r="K7" s="690" t="s">
+      <c r="K7" s="768" t="s">
         <v>82</v>
       </c>
-      <c r="L7" s="696" t="s">
+      <c r="L7" s="774" t="s">
         <v>83</v>
       </c>
       <c r="U7" s="9"/>
@@ -10855,32 +11089,32 @@
     <row r="8">
       <c r="A8" s="23"/>
       <c r="B8"/>
-      <c r="C8" s="651" t="s">
+      <c r="C8" s="729" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="657" t="s">
+      <c r="D8" s="735" t="s">
         <v>49</v>
       </c>
-      <c r="E8" s="661" t="s">
+      <c r="E8" s="739" t="s">
         <v>66</v>
       </c>
-      <c r="F8" s="667" t="s">
+      <c r="F8" s="745" t="s">
         <v>84</v>
       </c>
-      <c r="G8" s="673" t="s">
+      <c r="G8" s="751" t="s">
         <v>85</v>
       </c>
-      <c r="H8" s="679" t="s">
+      <c r="H8" s="757" t="s">
         <v>86</v>
       </c>
       <c r="I8" s="14"/>
-      <c r="J8" s="685" t="s">
+      <c r="J8" s="763" t="s">
         <v>87</v>
       </c>
-      <c r="K8" s="691" t="s">
+      <c r="K8" s="769" t="s">
         <v>88</v>
       </c>
-      <c r="L8" t="s" s="697">
+      <c r="L8" t="s" s="775">
         <v>89</v>
       </c>
       <c r="U8" s="9"/>

</xml_diff>

<commit_message>
"galacticPubs::publish() [2022-09-16 18:17:22] "
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -207,7 +207,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1079" uniqueCount="142">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -928,7 +928,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="776">
+  <cellXfs count="854">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1035,6 +1035,240 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
@@ -6295,44 +6529,44 @@
       <c r="Z2" s="7"/>
     </row>
     <row r="3">
-      <c r="A3" s="698" t="s">
+      <c r="A3" s="776" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="700" t="s">
+      <c r="B3" s="778" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="702" t="s">
+      <c r="C3" s="780" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="704" t="s">
+      <c r="D3" s="782" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="706" t="s">
+      <c r="E3" s="784" t="s">
         <v>31</v>
       </c>
       <c r="F3" s="14"/>
-      <c r="G3" s="708" t="s">
+      <c r="G3" s="786" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="699" t="s">
+      <c r="A4" s="777" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="701" t="s">
+      <c r="B4" s="779" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="703" t="s">
+      <c r="C4" s="781" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="705" t="s">
+      <c r="D4" s="783" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="707" t="s">
+      <c r="E4" s="785" t="s">
         <v>34</v>
       </c>
       <c r="F4" s="14"/>
-      <c r="G4" s="709" t="s">
+      <c r="G4" s="787" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7486,54 +7720,54 @@
     <row r="3">
       <c r="A3" s="23"/>
       <c r="B3"/>
-      <c r="C3" s="710" t="s">
+      <c r="C3" s="788" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="712" t="s">
+      <c r="D3" s="790" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="714" t="s">
+      <c r="E3" s="792" t="s">
         <v>44</v>
       </c>
-      <c r="F3" s="716" t="s">
+      <c r="F3" s="794" t="s">
         <v>45</v>
       </c>
       <c r="G3" s="14"/>
-      <c r="H3" s="718" t="s">
+      <c r="H3" s="796" t="s">
         <v>46</v>
       </c>
-      <c r="I3" s="720" t="s">
+      <c r="I3" s="798" t="s">
         <v>47</v>
       </c>
       <c r="J3"/>
-      <c r="K3" s="722" t="s">
+      <c r="K3" s="800" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="23"/>
       <c r="B4"/>
-      <c r="C4" s="711" t="s">
+      <c r="C4" s="789" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="713" t="s">
+      <c r="D4" s="791" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="715" t="s">
+      <c r="E4" s="793" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="717" t="s">
+      <c r="F4" s="795" t="s">
         <v>51</v>
       </c>
       <c r="G4" s="14"/>
-      <c r="H4" s="719" t="s">
+      <c r="H4" s="797" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="721" t="s">
+      <c r="I4" s="799" t="s">
         <v>53</v>
       </c>
       <c r="J4"/>
-      <c r="K4" s="723" t="s">
+      <c r="K4" s="801" t="s">
         <v>54</v>
       </c>
     </row>
@@ -10898,32 +11132,32 @@
     <row r="3">
       <c r="A3" s="23"/>
       <c r="B3"/>
-      <c r="C3" s="724" t="s">
+      <c r="C3" s="802" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="730" t="s">
+      <c r="D3" s="808" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="736" t="s">
+      <c r="E3" s="814" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="740" t="s">
+      <c r="F3" s="818" t="s">
         <v>60</v>
       </c>
-      <c r="G3" s="746" t="s">
+      <c r="G3" s="824" t="s">
         <v>61</v>
       </c>
-      <c r="H3" s="752" t="s">
+      <c r="H3" s="830" t="s">
         <v>62</v>
       </c>
       <c r="I3" s="14"/>
-      <c r="J3" s="758" t="s">
+      <c r="J3" s="836" t="s">
         <v>63</v>
       </c>
-      <c r="K3" s="764" t="s">
+      <c r="K3" s="842" t="s">
         <v>64</v>
       </c>
-      <c r="L3" s="770" t="s">
+      <c r="L3" s="848" t="s">
         <v>65</v>
       </c>
       <c r="U3" s="9"/>
@@ -10937,32 +11171,32 @@
     <row r="4">
       <c r="A4" s="23"/>
       <c r="B4"/>
-      <c r="C4" s="725" t="s">
+      <c r="C4" s="803" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="731" t="s">
+      <c r="D4" s="809" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="737" t="s">
+      <c r="E4" s="815" t="s">
         <v>66</v>
       </c>
-      <c r="F4" s="741" t="s">
+      <c r="F4" s="819" t="s">
         <v>67</v>
       </c>
-      <c r="G4" s="747" t="s">
+      <c r="G4" s="825" t="s">
         <v>68</v>
       </c>
-      <c r="H4" s="753" t="s">
+      <c r="H4" s="831" t="s">
         <v>69</v>
       </c>
       <c r="I4" s="14"/>
-      <c r="J4" s="759" t="s">
+      <c r="J4" s="837" t="s">
         <v>70</v>
       </c>
-      <c r="K4" s="765" t="s">
+      <c r="K4" s="843" t="s">
         <v>71</v>
       </c>
-      <c r="L4" s="771" t="s">
+      <c r="L4" s="849" t="s">
         <v>72</v>
       </c>
       <c r="U4" s="9"/>
@@ -10976,30 +11210,30 @@
     <row r="5">
       <c r="A5" s="23"/>
       <c r="B5"/>
-      <c r="C5" s="726" t="s">
+      <c r="C5" s="804" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="732" t="s">
+      <c r="D5" s="810" t="s">
         <v>43</v>
       </c>
       <c r="E5" s="14"/>
-      <c r="F5" s="742" t="s">
+      <c r="F5" s="820" t="s">
         <v>73</v>
       </c>
-      <c r="G5" s="748" t="s">
+      <c r="G5" s="826" t="s">
         <v>74</v>
       </c>
-      <c r="H5" s="754" t="s">
+      <c r="H5" s="832" t="s">
         <v>75</v>
       </c>
       <c r="I5" s="14"/>
-      <c r="J5" s="760" t="s">
+      <c r="J5" s="838" t="s">
         <v>76</v>
       </c>
-      <c r="K5" s="766" t="s">
+      <c r="K5" s="844" t="s">
         <v>76</v>
       </c>
-      <c r="L5" s="772" t="s">
+      <c r="L5" s="850" t="s">
         <v>77</v>
       </c>
       <c r="U5" s="9"/>
@@ -11013,30 +11247,30 @@
     <row r="6">
       <c r="A6" s="23"/>
       <c r="B6"/>
-      <c r="C6" s="727" t="s">
+      <c r="C6" s="805" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="733" t="s">
+      <c r="D6" s="811" t="s">
         <v>43</v>
       </c>
       <c r="E6" s="588"/>
-      <c r="F6" s="743" t="s">
+      <c r="F6" s="821" t="s">
         <v>136</v>
       </c>
-      <c r="G6" s="749" t="s">
+      <c r="G6" s="827" t="s">
         <v>137</v>
       </c>
-      <c r="H6" s="755" t="s">
+      <c r="H6" s="833" t="s">
         <v>138</v>
       </c>
       <c r="I6" s="14"/>
-      <c r="J6" s="761" t="s">
+      <c r="J6" s="839" t="s">
         <v>139</v>
       </c>
-      <c r="K6" s="767" t="s">
+      <c r="K6" s="845" t="s">
         <v>140</v>
       </c>
-      <c r="L6" s="773" t="s">
+      <c r="L6" s="851" t="s">
         <v>141</v>
       </c>
       <c r="U6" s="9"/>
@@ -11050,32 +11284,32 @@
     <row r="7">
       <c r="A7" s="23"/>
       <c r="B7"/>
-      <c r="C7" s="728" t="s">
+      <c r="C7" s="806" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="734" t="s">
+      <c r="D7" s="812" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="738" t="s">
+      <c r="E7" s="816" t="s">
         <v>59</v>
       </c>
-      <c r="F7" s="744" t="s">
+      <c r="F7" s="822" t="s">
         <v>78</v>
       </c>
-      <c r="G7" s="750" t="s">
+      <c r="G7" s="828" t="s">
         <v>79</v>
       </c>
-      <c r="H7" s="756" t="s">
+      <c r="H7" s="834" t="s">
         <v>80</v>
       </c>
       <c r="I7" s="14"/>
-      <c r="J7" s="762" t="s">
+      <c r="J7" s="840" t="s">
         <v>81</v>
       </c>
-      <c r="K7" s="768" t="s">
+      <c r="K7" s="846" t="s">
         <v>82</v>
       </c>
-      <c r="L7" s="774" t="s">
+      <c r="L7" s="852" t="s">
         <v>83</v>
       </c>
       <c r="U7" s="9"/>
@@ -11089,32 +11323,32 @@
     <row r="8">
       <c r="A8" s="23"/>
       <c r="B8"/>
-      <c r="C8" s="729" t="s">
+      <c r="C8" s="807" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="735" t="s">
+      <c r="D8" s="813" t="s">
         <v>49</v>
       </c>
-      <c r="E8" s="739" t="s">
+      <c r="E8" s="817" t="s">
         <v>66</v>
       </c>
-      <c r="F8" s="745" t="s">
+      <c r="F8" s="823" t="s">
         <v>84</v>
       </c>
-      <c r="G8" s="751" t="s">
+      <c r="G8" s="829" t="s">
         <v>85</v>
       </c>
-      <c r="H8" s="757" t="s">
+      <c r="H8" s="835" t="s">
         <v>86</v>
       </c>
       <c r="I8" s="14"/>
-      <c r="J8" s="763" t="s">
+      <c r="J8" s="841" t="s">
         <v>87</v>
       </c>
-      <c r="K8" s="769" t="s">
+      <c r="K8" s="847" t="s">
         <v>88</v>
       </c>
-      <c r="L8" t="s" s="775">
+      <c r="L8" t="s" s="853">
         <v>89</v>
       </c>
       <c r="U8" s="9"/>

</xml_diff>

<commit_message>
"galacticPubs::publish() [2022-09-19 11:26:56] "
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -207,7 +207,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1079" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1149" uniqueCount="142">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -928,7 +928,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="854">
+  <cellXfs count="924">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1035,6 +1035,216 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
@@ -6529,44 +6739,44 @@
       <c r="Z2" s="7"/>
     </row>
     <row r="3">
-      <c r="A3" s="776" t="s">
+      <c r="A3" s="854" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="778" t="s">
+      <c r="B3" s="856" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="780" t="s">
+      <c r="C3" s="858" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="782" t="s">
+      <c r="D3" s="860" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="784" t="s">
+      <c r="E3" s="862" t="s">
         <v>31</v>
       </c>
       <c r="F3" s="14"/>
-      <c r="G3" s="786" t="s">
+      <c r="G3" s="864" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="777" t="s">
+      <c r="A4" s="855" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="779" t="s">
+      <c r="B4" s="857" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="781" t="s">
+      <c r="C4" s="859" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="783" t="s">
+      <c r="D4" s="861" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="785" t="s">
+      <c r="E4" s="863" t="s">
         <v>34</v>
       </c>
       <c r="F4" s="14"/>
-      <c r="G4" s="787" t="s">
+      <c r="G4" s="865" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7720,54 +7930,54 @@
     <row r="3">
       <c r="A3" s="23"/>
       <c r="B3"/>
-      <c r="C3" s="788" t="s">
+      <c r="C3" s="866" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="790" t="s">
+      <c r="D3" s="868" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="792" t="s">
+      <c r="E3" s="870" t="s">
         <v>44</v>
       </c>
-      <c r="F3" s="794" t="s">
+      <c r="F3" s="872" t="s">
         <v>45</v>
       </c>
       <c r="G3" s="14"/>
-      <c r="H3" s="796" t="s">
+      <c r="H3" s="874" t="s">
         <v>46</v>
       </c>
-      <c r="I3" s="798" t="s">
+      <c r="I3" s="876" t="s">
         <v>47</v>
       </c>
       <c r="J3"/>
-      <c r="K3" s="800" t="s">
+      <c r="K3" s="878" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="23"/>
       <c r="B4"/>
-      <c r="C4" s="789" t="s">
+      <c r="C4" s="867" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="791" t="s">
+      <c r="D4" s="869" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="793" t="s">
+      <c r="E4" s="871" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="795" t="s">
+      <c r="F4" s="873" t="s">
         <v>51</v>
       </c>
       <c r="G4" s="14"/>
-      <c r="H4" s="797" t="s">
+      <c r="H4" s="875" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="799" t="s">
+      <c r="I4" s="877" t="s">
         <v>53</v>
       </c>
       <c r="J4"/>
-      <c r="K4" s="801" t="s">
+      <c r="K4" s="879" t="s">
         <v>54</v>
       </c>
     </row>
@@ -11132,32 +11342,32 @@
     <row r="3">
       <c r="A3" s="23"/>
       <c r="B3"/>
-      <c r="C3" s="802" t="s">
+      <c r="C3" s="880" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="808" t="s">
+      <c r="D3" s="885" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="814" t="s">
+      <c r="E3" s="890" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="818" t="s">
+      <c r="F3" s="894" t="s">
         <v>60</v>
       </c>
-      <c r="G3" s="824" t="s">
+      <c r="G3" s="899" t="s">
         <v>61</v>
       </c>
-      <c r="H3" s="830" t="s">
+      <c r="H3" s="904" t="s">
         <v>62</v>
       </c>
       <c r="I3" s="14"/>
-      <c r="J3" s="836" t="s">
+      <c r="J3" s="909" t="s">
         <v>63</v>
       </c>
-      <c r="K3" s="842" t="s">
+      <c r="K3" s="914" t="s">
         <v>64</v>
       </c>
-      <c r="L3" s="848" t="s">
+      <c r="L3" s="919" t="s">
         <v>65</v>
       </c>
       <c r="U3" s="9"/>
@@ -11171,32 +11381,32 @@
     <row r="4">
       <c r="A4" s="23"/>
       <c r="B4"/>
-      <c r="C4" s="803" t="s">
+      <c r="C4" s="881" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="809" t="s">
+      <c r="D4" s="886" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="815" t="s">
+      <c r="E4" s="891" t="s">
         <v>66</v>
       </c>
-      <c r="F4" s="819" t="s">
+      <c r="F4" s="895" t="s">
         <v>67</v>
       </c>
-      <c r="G4" s="825" t="s">
+      <c r="G4" s="900" t="s">
         <v>68</v>
       </c>
-      <c r="H4" s="831" t="s">
+      <c r="H4" s="905" t="s">
         <v>69</v>
       </c>
       <c r="I4" s="14"/>
-      <c r="J4" s="837" t="s">
+      <c r="J4" s="910" t="s">
         <v>70</v>
       </c>
-      <c r="K4" s="843" t="s">
+      <c r="K4" s="915" t="s">
         <v>71</v>
       </c>
-      <c r="L4" s="849" t="s">
+      <c r="L4" s="920" t="s">
         <v>72</v>
       </c>
       <c r="U4" s="9"/>
@@ -11210,30 +11420,30 @@
     <row r="5">
       <c r="A5" s="23"/>
       <c r="B5"/>
-      <c r="C5" s="804" t="s">
+      <c r="C5" s="882" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="810" t="s">
+      <c r="D5" s="887" t="s">
         <v>43</v>
       </c>
       <c r="E5" s="14"/>
-      <c r="F5" s="820" t="s">
+      <c r="F5" s="896" t="s">
         <v>73</v>
       </c>
-      <c r="G5" s="826" t="s">
+      <c r="G5" s="901" t="s">
         <v>74</v>
       </c>
-      <c r="H5" s="832" t="s">
+      <c r="H5" s="906" t="s">
         <v>75</v>
       </c>
       <c r="I5" s="14"/>
-      <c r="J5" s="838" t="s">
+      <c r="J5" s="911" t="s">
         <v>76</v>
       </c>
-      <c r="K5" s="844" t="s">
+      <c r="K5" s="916" t="s">
         <v>76</v>
       </c>
-      <c r="L5" s="850" t="s">
+      <c r="L5" s="921" t="s">
         <v>77</v>
       </c>
       <c r="U5" s="9"/>
@@ -11247,31 +11457,33 @@
     <row r="6">
       <c r="A6" s="23"/>
       <c r="B6"/>
-      <c r="C6" s="805" t="s">
+      <c r="C6" s="883" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="811" t="s">
-        <v>43</v>
+      <c r="D6" s="888" t="s">
+        <v>49</v>
       </c>
-      <c r="E6" s="588"/>
-      <c r="F6" s="821" t="s">
-        <v>136</v>
+      <c r="E6" s="892" t="s">
+        <v>59</v>
       </c>
-      <c r="G6" s="827" t="s">
-        <v>137</v>
+      <c r="F6" s="897" t="s">
+        <v>78</v>
       </c>
-      <c r="H6" s="833" t="s">
-        <v>138</v>
+      <c r="G6" s="902" t="s">
+        <v>79</v>
+      </c>
+      <c r="H6" s="907" t="s">
+        <v>80</v>
       </c>
       <c r="I6" s="14"/>
-      <c r="J6" s="839" t="s">
-        <v>139</v>
+      <c r="J6" s="912" t="s">
+        <v>81</v>
       </c>
-      <c r="K6" s="845" t="s">
-        <v>140</v>
+      <c r="K6" s="917" t="s">
+        <v>82</v>
       </c>
-      <c r="L6" s="851" t="s">
-        <v>141</v>
+      <c r="L6" s="922" t="s">
+        <v>83</v>
       </c>
       <c r="U6" s="9"/>
       <c r="V6" s="9"/>
@@ -11284,33 +11496,33 @@
     <row r="7">
       <c r="A7" s="23"/>
       <c r="B7"/>
-      <c r="C7" s="806" t="s">
+      <c r="C7" s="884" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="812" t="s">
+      <c r="D7" s="889" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="816" t="s">
-        <v>59</v>
+      <c r="E7" s="893" t="s">
+        <v>66</v>
       </c>
-      <c r="F7" s="822" t="s">
-        <v>78</v>
+      <c r="F7" s="898" t="s">
+        <v>84</v>
       </c>
-      <c r="G7" s="828" t="s">
-        <v>79</v>
+      <c r="G7" s="903" t="s">
+        <v>85</v>
       </c>
-      <c r="H7" s="834" t="s">
-        <v>80</v>
+      <c r="H7" s="908" t="s">
+        <v>86</v>
       </c>
       <c r="I7" s="14"/>
-      <c r="J7" s="840" t="s">
-        <v>81</v>
+      <c r="J7" s="913" t="s">
+        <v>87</v>
       </c>
-      <c r="K7" s="846" t="s">
-        <v>82</v>
+      <c r="K7" s="918" t="s">
+        <v>88</v>
       </c>
-      <c r="L7" s="852" t="s">
-        <v>83</v>
+      <c r="L7" s="923" t="s">
+        <v>89</v>
       </c>
       <c r="U7" s="9"/>
       <c r="V7" s="9"/>

</xml_diff>